<commit_message>
fix small issues in DB sim
</commit_message>
<xml_diff>
--- a/RunControl.xlsx
+++ b/RunControl.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C556A100-FCB7-4622-BF06-66FA87532A77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F45A375-C4DF-4B0A-AB6D-A6134485FDDE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -844,21 +844,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BO36"/>
+  <dimension ref="A1:BO43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="6" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="M18" sqref="M18"/>
+      <selection pane="bottomRight" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.140625" customWidth="1"/>
     <col min="2" max="2" width="10.140625" customWidth="1"/>
-    <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" customWidth="1"/>
+    <col min="3" max="4" width="11.7109375" customWidth="1"/>
     <col min="5" max="5" width="11.140625" customWidth="1"/>
     <col min="6" max="6" width="14.28515625" customWidth="1"/>
     <col min="7" max="7" width="12.28515625" customWidth="1"/>
@@ -1251,7 +1250,7 @@
         <v>1</v>
       </c>
       <c r="AE3" s="12">
-        <f t="shared" ref="AE3:AE28" si="0">0.15/20</f>
+        <f t="shared" ref="AE3:AE35" si="0">0.15/20</f>
         <v>7.4999999999999997E-3</v>
       </c>
       <c r="AF3" s="12">
@@ -2619,984 +2618,28 @@
     <row r="13" spans="1:67" s="12" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="1:67" s="12" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="1:67" s="12" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:67" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="B16" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="D16" s="12">
-        <v>1</v>
-      </c>
-      <c r="E16" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="F16" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="G16" s="12">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="R16" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="S16" s="12">
-        <v>0</v>
-      </c>
-      <c r="T16" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="U16" s="12">
-        <v>0</v>
-      </c>
-      <c r="V16" s="12">
-        <v>0.9</v>
-      </c>
-      <c r="W16" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="X16" s="12">
-        <v>0</v>
-      </c>
-      <c r="Y16" s="12">
-        <v>0.9</v>
-      </c>
-      <c r="Z16" s="12">
-        <v>0.01</v>
-      </c>
-      <c r="AA16" s="12">
-        <v>1E-3</v>
-      </c>
-      <c r="AB16" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="AC16" s="12">
-        <v>0</v>
-      </c>
-      <c r="AD16" s="12">
-        <v>1</v>
-      </c>
-      <c r="AE16" s="12">
-        <f t="shared" si="0"/>
-        <v>7.4999999999999997E-3</v>
-      </c>
-      <c r="AF16" s="12">
-        <v>1E-3</v>
-      </c>
-      <c r="AG16" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="AH16" s="12">
-        <v>0</v>
-      </c>
-      <c r="AI16" s="12">
-        <v>1</v>
-      </c>
-      <c r="AJ16" s="12">
-        <v>1</v>
-      </c>
-      <c r="AN16" s="12">
-        <v>0.06</v>
-      </c>
-      <c r="AY16" s="12">
-        <v>15</v>
-      </c>
-      <c r="AZ16" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="BA16" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="BB16" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="BC16" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="BD16" s="12">
-        <v>5</v>
-      </c>
-      <c r="BE16" s="12">
-        <v>8.2199999999999995E-2</v>
-      </c>
-      <c r="BF16" s="12">
-        <v>0.12</v>
-      </c>
-      <c r="BG16" s="12">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="BH16" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="BI16" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="BJ16" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="BK16" s="12">
-        <v>0.01</v>
-      </c>
-      <c r="BL16" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="BM16" s="12">
-        <v>1</v>
-      </c>
-      <c r="BN16" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="BO16" s="12" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:67" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="B17" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="D17" s="12">
-        <v>1</v>
-      </c>
-      <c r="E17" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="F17" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="G17" s="12">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="R17" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="S17" s="12">
-        <v>0</v>
-      </c>
-      <c r="T17" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="U17" s="12">
-        <v>0</v>
-      </c>
-      <c r="V17" s="12">
-        <v>0.9</v>
-      </c>
-      <c r="W17" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="X17" s="12">
-        <v>0</v>
-      </c>
-      <c r="Y17" s="12">
-        <v>0.9</v>
-      </c>
-      <c r="Z17" s="12">
-        <v>0.01</v>
-      </c>
-      <c r="AA17" s="12">
-        <v>1E-3</v>
-      </c>
-      <c r="AB17" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="AC17" s="12">
-        <v>0</v>
-      </c>
-      <c r="AD17" s="12">
-        <v>1</v>
-      </c>
-      <c r="AE17" s="12">
-        <f t="shared" si="0"/>
-        <v>7.4999999999999997E-3</v>
-      </c>
-      <c r="AF17" s="12">
-        <v>1E-3</v>
-      </c>
-      <c r="AG17" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="AH17" s="12">
-        <v>0</v>
-      </c>
-      <c r="AI17" s="12">
-        <v>1</v>
-      </c>
-      <c r="AJ17" s="12">
-        <v>1</v>
-      </c>
-      <c r="AN17" s="12">
-        <v>0.06</v>
-      </c>
-      <c r="AY17" s="12">
-        <v>15</v>
-      </c>
-      <c r="AZ17" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="BA17" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="BB17" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="BC17" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="BD17" s="12">
-        <v>5</v>
-      </c>
-      <c r="BE17" s="12">
-        <v>8.2199999999999995E-2</v>
-      </c>
-      <c r="BF17" s="12">
-        <v>0.12</v>
-      </c>
-      <c r="BG17" s="12">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="BH17" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="BI17" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="BJ17" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="BK17" s="12">
-        <v>0.01</v>
-      </c>
-      <c r="BL17" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="BM17" s="12">
-        <v>1</v>
-      </c>
-      <c r="BN17" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="BO17" s="12" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:67" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="B18" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="D18" s="12">
-        <v>1</v>
-      </c>
-      <c r="E18" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="F18" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="G18" s="12">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="R18" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="S18" s="12">
-        <v>0</v>
-      </c>
-      <c r="T18" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="U18" s="12">
-        <v>0</v>
-      </c>
-      <c r="V18" s="12">
-        <v>0.9</v>
-      </c>
-      <c r="W18" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="X18" s="12">
-        <v>0</v>
-      </c>
-      <c r="Y18" s="12">
-        <v>0.9</v>
-      </c>
-      <c r="Z18" s="12">
-        <v>0.01</v>
-      </c>
-      <c r="AA18" s="12">
-        <v>1E-3</v>
-      </c>
-      <c r="AB18" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="AC18" s="12">
-        <v>0</v>
-      </c>
-      <c r="AD18" s="12">
-        <v>1</v>
-      </c>
-      <c r="AE18" s="12">
-        <f t="shared" si="0"/>
-        <v>7.4999999999999997E-3</v>
-      </c>
-      <c r="AF18" s="12">
-        <v>1E-3</v>
-      </c>
-      <c r="AG18" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="AH18" s="12">
-        <v>0</v>
-      </c>
-      <c r="AI18" s="12">
-        <v>1</v>
-      </c>
-      <c r="AJ18" s="12">
-        <v>1</v>
-      </c>
-      <c r="AN18" s="12">
-        <v>0.06</v>
-      </c>
-      <c r="AY18" s="12">
-        <v>15</v>
-      </c>
-      <c r="AZ18" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="BA18" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="BB18" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="BC18" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="BD18" s="12">
-        <v>5</v>
-      </c>
-      <c r="BE18" s="12">
-        <v>8.2199999999999995E-2</v>
-      </c>
-      <c r="BF18" s="12">
-        <v>0.12</v>
-      </c>
-      <c r="BG18" s="12">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="BH18" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="BI18" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="BJ18" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="BK18" s="12">
-        <v>0.01</v>
-      </c>
-      <c r="BL18" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="BM18" s="12">
-        <v>1</v>
-      </c>
-      <c r="BN18" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="BO18" s="12" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:67" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="B19" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="C19" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="D19" s="12">
-        <v>1</v>
-      </c>
-      <c r="E19" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="F19" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="G19" s="12">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="R19" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="S19" s="12">
-        <v>0</v>
-      </c>
-      <c r="T19" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="U19" s="12">
-        <v>0</v>
-      </c>
-      <c r="V19" s="12">
-        <v>0.9</v>
-      </c>
-      <c r="W19" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="X19" s="12">
-        <v>0</v>
-      </c>
-      <c r="Y19" s="12">
-        <v>0.9</v>
-      </c>
-      <c r="Z19" s="12">
-        <v>0.01</v>
-      </c>
-      <c r="AA19" s="12">
-        <v>1E-3</v>
-      </c>
-      <c r="AB19" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="AC19" s="12">
-        <v>0</v>
-      </c>
-      <c r="AD19" s="12">
-        <v>1</v>
-      </c>
-      <c r="AE19" s="12">
-        <f t="shared" si="0"/>
-        <v>7.4999999999999997E-3</v>
-      </c>
-      <c r="AF19" s="12">
-        <v>1E-3</v>
-      </c>
-      <c r="AG19" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="AH19" s="12">
-        <v>0</v>
-      </c>
-      <c r="AI19" s="12">
-        <v>1</v>
-      </c>
-      <c r="AJ19" s="12">
-        <v>1</v>
-      </c>
-      <c r="AN19" s="12">
-        <v>0.06</v>
-      </c>
-      <c r="AY19" s="12">
-        <v>15</v>
-      </c>
-      <c r="AZ19" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="BA19" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="BB19" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="BC19" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="BD19" s="12">
-        <v>5</v>
-      </c>
-      <c r="BE19" s="12">
-        <v>8.2199999999999995E-2</v>
-      </c>
-      <c r="BF19" s="12">
-        <v>0.12</v>
-      </c>
-      <c r="BG19" s="12">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="BH19" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="BI19" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="BJ19" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="BK19" s="12">
-        <v>0.01</v>
-      </c>
-      <c r="BL19" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="BM19" s="12">
-        <v>1</v>
-      </c>
-      <c r="BN19" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="BO19" s="12" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:67" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="B20" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="C20" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="D20" s="12">
-        <v>1</v>
-      </c>
-      <c r="E20" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="F20" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="G20" s="12">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="R20" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="S20" s="12">
-        <v>0</v>
-      </c>
-      <c r="T20" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="U20" s="12">
-        <v>0</v>
-      </c>
-      <c r="V20" s="12">
-        <v>0.9</v>
-      </c>
-      <c r="W20" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="X20" s="12">
-        <v>0</v>
-      </c>
-      <c r="Y20" s="12">
-        <v>0.9</v>
-      </c>
-      <c r="Z20" s="12">
-        <v>0.01</v>
-      </c>
-      <c r="AA20" s="12">
-        <v>1E-3</v>
-      </c>
-      <c r="AB20" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="AC20" s="12">
-        <v>0</v>
-      </c>
-      <c r="AD20" s="12">
-        <v>1</v>
-      </c>
-      <c r="AE20" s="12">
-        <f t="shared" si="0"/>
-        <v>7.4999999999999997E-3</v>
-      </c>
-      <c r="AF20" s="12">
-        <v>1E-3</v>
-      </c>
-      <c r="AG20" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="AH20" s="12">
-        <v>0</v>
-      </c>
-      <c r="AI20" s="12">
-        <v>1</v>
-      </c>
-      <c r="AJ20" s="12">
-        <v>1</v>
-      </c>
-      <c r="AK20" s="12">
-        <v>0.5</v>
-      </c>
-      <c r="AL20" s="12">
-        <v>0.5</v>
-      </c>
-      <c r="AN20" s="12">
-        <v>0.06</v>
-      </c>
-      <c r="AY20" s="12">
-        <v>15</v>
-      </c>
-      <c r="AZ20" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="BA20" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="BB20" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="BC20" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="BD20" s="12">
-        <v>5</v>
-      </c>
-      <c r="BE20" s="12">
-        <v>8.2199999999999995E-2</v>
-      </c>
-      <c r="BF20" s="12">
-        <v>0.12</v>
-      </c>
-      <c r="BG20" s="12">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="BH20" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="BI20" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="BJ20" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="BK20" s="12">
-        <v>0.01</v>
-      </c>
-      <c r="BL20" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="BM20" s="12">
-        <v>1</v>
-      </c>
-      <c r="BN20" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="BO20" s="12" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:67" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="B21" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="D21" s="12">
-        <v>1</v>
-      </c>
-      <c r="E21" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="F21" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="G21" s="12">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="R21" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="S21" s="12">
-        <v>0</v>
-      </c>
-      <c r="T21" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="U21" s="12">
-        <v>0</v>
-      </c>
-      <c r="V21" s="12">
-        <v>0.9</v>
-      </c>
-      <c r="W21" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="X21" s="12">
-        <v>0</v>
-      </c>
-      <c r="Y21" s="12">
-        <v>0.9</v>
-      </c>
-      <c r="Z21" s="12">
-        <v>0.01</v>
-      </c>
-      <c r="AA21" s="12">
-        <v>1E-3</v>
-      </c>
-      <c r="AB21" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="AC21" s="12">
-        <v>0</v>
-      </c>
-      <c r="AD21" s="12">
-        <v>1</v>
-      </c>
-      <c r="AE21" s="12">
-        <f t="shared" si="0"/>
-        <v>7.4999999999999997E-3</v>
-      </c>
-      <c r="AF21" s="12">
-        <v>1E-3</v>
-      </c>
-      <c r="AG21" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="AH21" s="12">
-        <v>0</v>
-      </c>
-      <c r="AI21" s="12">
-        <v>1</v>
-      </c>
-      <c r="AJ21" s="12">
-        <v>2</v>
-      </c>
-      <c r="AK21" s="12">
-        <v>0.5</v>
-      </c>
-      <c r="AL21" s="12">
-        <v>0.5</v>
-      </c>
-      <c r="AN21" s="12">
-        <v>0.06</v>
-      </c>
-      <c r="AY21" s="12">
-        <v>15</v>
-      </c>
-      <c r="AZ21" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="BA21" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="BB21" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="BC21" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="BD21" s="12">
-        <v>5</v>
-      </c>
-      <c r="BE21" s="12">
-        <v>8.2199999999999995E-2</v>
-      </c>
-      <c r="BF21" s="12">
-        <v>0.12</v>
-      </c>
-      <c r="BG21" s="12">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="BH21" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="BI21" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="BJ21" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="BK21" s="12">
-        <v>0.01</v>
-      </c>
-      <c r="BL21" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="BM21" s="12">
-        <v>1</v>
-      </c>
-      <c r="BN21" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="BO21" s="12" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:67" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="B22" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="C22" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="D22" s="12">
-        <v>1</v>
-      </c>
-      <c r="E22" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="F22" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="G22" s="12">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="R22" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="S22" s="12">
-        <v>0</v>
-      </c>
-      <c r="T22" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="U22" s="12">
-        <v>0</v>
-      </c>
-      <c r="V22" s="12">
-        <v>0.9</v>
-      </c>
-      <c r="W22" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="X22" s="12">
-        <v>0</v>
-      </c>
-      <c r="Y22" s="12">
-        <v>0.9</v>
-      </c>
-      <c r="Z22" s="12">
-        <v>0.01</v>
-      </c>
-      <c r="AA22" s="12">
-        <v>1E-3</v>
-      </c>
-      <c r="AB22" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="AC22" s="12">
-        <v>0</v>
-      </c>
-      <c r="AD22" s="12">
-        <v>1</v>
-      </c>
-      <c r="AE22" s="12">
-        <f t="shared" si="0"/>
-        <v>7.4999999999999997E-3</v>
-      </c>
-      <c r="AF22" s="12">
-        <v>1E-3</v>
-      </c>
-      <c r="AG22" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="AH22" s="12">
-        <v>0</v>
-      </c>
-      <c r="AI22" s="12">
-        <v>1</v>
-      </c>
-      <c r="AJ22" s="12">
-        <v>1</v>
-      </c>
-      <c r="AK22" s="12">
-        <v>0.5</v>
-      </c>
-      <c r="AL22" s="12">
-        <v>0.5</v>
-      </c>
-      <c r="AN22" s="12">
-        <v>0.06</v>
-      </c>
-      <c r="AY22" s="12">
-        <v>15</v>
-      </c>
-      <c r="AZ22" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="BA22" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="BB22" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="BC22" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="BD22" s="12">
-        <v>5</v>
-      </c>
-      <c r="BE22" s="12">
-        <v>8.2199999999999995E-2</v>
-      </c>
-      <c r="BF22" s="12">
-        <v>0.12</v>
-      </c>
-      <c r="BG22" s="12">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="BH22" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="BI22" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="BJ22" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="BK22" s="12">
-        <v>0.01</v>
-      </c>
-      <c r="BL22" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="BM22" s="12">
-        <v>1</v>
-      </c>
-      <c r="BN22" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="BO22" s="12" t="b">
-        <v>1</v>
-      </c>
-    </row>
+    <row r="16" spans="1:67" s="12" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="1:67" s="12" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="1:67" s="12" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="1:67" s="12" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:67" s="12" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="1:67" s="12" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:67" s="12" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="23" spans="1:67" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
-        <v>90</v>
+        <v>61</v>
       </c>
       <c r="B23" s="12" t="b">
         <v>0</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D23" s="12">
         <v>1</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="F23" s="12" t="s">
         <v>83</v>
@@ -3660,13 +2703,7 @@
         <v>1</v>
       </c>
       <c r="AJ23" s="12">
-        <v>2</v>
-      </c>
-      <c r="AK23" s="12">
-        <v>0.5</v>
-      </c>
-      <c r="AL23" s="12">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="AN23" s="12">
         <v>0.06</v>
@@ -3723,28 +2760,159 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:67" x14ac:dyDescent="0.25">
-      <c r="BJ24" s="12"/>
-      <c r="BK24" s="12"/>
+    <row r="24" spans="1:67" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="B24" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="D24" s="12">
+        <v>1</v>
+      </c>
+      <c r="E24" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="F24" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="G24" s="12">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="R24" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="S24" s="12">
+        <v>0</v>
+      </c>
+      <c r="T24" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="U24" s="12">
+        <v>0</v>
+      </c>
+      <c r="V24" s="12">
+        <v>0.9</v>
+      </c>
+      <c r="W24" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="X24" s="12">
+        <v>0</v>
+      </c>
+      <c r="Y24" s="12">
+        <v>0.9</v>
+      </c>
+      <c r="Z24" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="AA24" s="12">
+        <v>1E-3</v>
+      </c>
+      <c r="AB24" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="AC24" s="12">
+        <v>0</v>
+      </c>
+      <c r="AD24" s="12">
+        <v>1</v>
+      </c>
+      <c r="AE24" s="12">
+        <f t="shared" si="0"/>
+        <v>7.4999999999999997E-3</v>
+      </c>
+      <c r="AF24" s="12">
+        <v>1E-3</v>
+      </c>
+      <c r="AG24" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="AH24" s="12">
+        <v>0</v>
+      </c>
+      <c r="AI24" s="12">
+        <v>1</v>
+      </c>
+      <c r="AJ24" s="12">
+        <v>1</v>
+      </c>
+      <c r="AN24" s="12">
+        <v>0.06</v>
+      </c>
+      <c r="AY24" s="12">
+        <v>15</v>
+      </c>
+      <c r="AZ24" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="BA24" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="BB24" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="BC24" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="BD24" s="12">
+        <v>5</v>
+      </c>
+      <c r="BE24" s="12">
+        <v>8.2199999999999995E-2</v>
+      </c>
+      <c r="BF24" s="12">
+        <v>0.12</v>
+      </c>
+      <c r="BG24" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="BH24" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="BI24" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="BJ24" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="BK24" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="BL24" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="BM24" s="12">
+        <v>1</v>
+      </c>
+      <c r="BN24" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="BO24" s="12" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="25" spans="1:67" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="B25" s="12" t="b">
         <v>0</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="D25" s="12">
         <v>1</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="F25" s="12" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="G25" s="12">
         <v>1.4999999999999999E-2</v>
@@ -3807,9 +2975,6 @@
       <c r="AJ25" s="12">
         <v>1</v>
       </c>
-      <c r="AM25" s="12">
-        <v>0.02</v>
-      </c>
       <c r="AN25" s="12">
         <v>0.06</v>
       </c>
@@ -3865,22 +3030,156 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:67" s="12" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:67" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B26" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="D26" s="12">
+        <v>1</v>
+      </c>
+      <c r="E26" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="F26" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="G26" s="12">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="R26" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="S26" s="12">
+        <v>0</v>
+      </c>
+      <c r="T26" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="U26" s="12">
+        <v>0</v>
+      </c>
+      <c r="V26" s="12">
+        <v>0.9</v>
+      </c>
+      <c r="W26" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="X26" s="12">
+        <v>0</v>
+      </c>
+      <c r="Y26" s="12">
+        <v>0.9</v>
+      </c>
+      <c r="Z26" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="AA26" s="12">
+        <v>1E-3</v>
+      </c>
+      <c r="AB26" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="AC26" s="12">
+        <v>0</v>
+      </c>
+      <c r="AD26" s="12">
+        <v>1</v>
+      </c>
+      <c r="AE26" s="12">
+        <f t="shared" si="0"/>
+        <v>7.4999999999999997E-3</v>
+      </c>
+      <c r="AF26" s="12">
+        <v>1E-3</v>
+      </c>
+      <c r="AG26" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="AH26" s="12">
+        <v>0</v>
+      </c>
+      <c r="AI26" s="12">
+        <v>1</v>
+      </c>
+      <c r="AJ26" s="12">
+        <v>1</v>
+      </c>
+      <c r="AN26" s="12">
+        <v>0.06</v>
+      </c>
+      <c r="AY26" s="12">
+        <v>15</v>
+      </c>
+      <c r="AZ26" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="BA26" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="BB26" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="BC26" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="BD26" s="12">
+        <v>5</v>
+      </c>
+      <c r="BE26" s="12">
+        <v>8.2199999999999995E-2</v>
+      </c>
+      <c r="BF26" s="12">
+        <v>0.12</v>
+      </c>
+      <c r="BG26" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="BH26" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="BI26" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="BJ26" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="BK26" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="BL26" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="BM26" s="12">
+        <v>1</v>
+      </c>
+      <c r="BN26" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="BO26" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
     <row r="27" spans="1:67" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
-        <v>96</v>
+        <v>67</v>
       </c>
       <c r="B27" s="12" t="b">
         <v>0</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="D27" s="12">
         <v>1</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>97</v>
+        <v>63</v>
       </c>
       <c r="F27" s="12" t="s">
         <v>83</v>
@@ -3895,7 +3194,7 @@
         <v>0</v>
       </c>
       <c r="T27" s="12">
-        <v>0.04</v>
+        <v>0.02</v>
       </c>
       <c r="U27" s="12">
         <v>0</v>
@@ -3946,6 +3245,12 @@
       <c r="AJ27" s="12">
         <v>1</v>
       </c>
+      <c r="AK27" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="AL27" s="12">
+        <v>0.5</v>
+      </c>
       <c r="AN27" s="12">
         <v>0.06</v>
       </c>
@@ -3980,7 +3285,7 @@
         <v>0.02</v>
       </c>
       <c r="BI27" s="12" t="s">
-        <v>95</v>
+        <v>55</v>
       </c>
       <c r="BJ27" s="12">
         <v>0.02</v>
@@ -4003,19 +3308,19 @@
     </row>
     <row r="28" spans="1:67" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
-        <v>93</v>
+        <v>66</v>
       </c>
       <c r="B28" s="12" t="b">
         <v>0</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="D28" s="12">
         <v>1</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="F28" s="12" t="s">
         <v>83</v>
@@ -4030,7 +3335,7 @@
         <v>0</v>
       </c>
       <c r="T28" s="12">
-        <v>0.04</v>
+        <v>0.02</v>
       </c>
       <c r="U28" s="12">
         <v>0</v>
@@ -4079,7 +3384,13 @@
         <v>1</v>
       </c>
       <c r="AJ28" s="12">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="AK28" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="AL28" s="12">
+        <v>0.5</v>
       </c>
       <c r="AN28" s="12">
         <v>0.06</v>
@@ -4115,7 +3426,7 @@
         <v>0.02</v>
       </c>
       <c r="BI28" s="12" t="s">
-        <v>95</v>
+        <v>55</v>
       </c>
       <c r="BJ28" s="12">
         <v>0.02</v>
@@ -4133,27 +3444,171 @@
         <v>1</v>
       </c>
       <c r="BO28" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:67" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="B29" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="D29" s="12">
+        <v>1</v>
+      </c>
+      <c r="E29" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="F29" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="G29" s="12">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="R29" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="S29" s="12">
+        <v>0</v>
+      </c>
+      <c r="T29" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="U29" s="12">
+        <v>0</v>
+      </c>
+      <c r="V29" s="12">
+        <v>0.9</v>
+      </c>
+      <c r="W29" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="X29" s="12">
+        <v>0</v>
+      </c>
+      <c r="Y29" s="12">
+        <v>0.9</v>
+      </c>
+      <c r="Z29" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="AA29" s="12">
+        <v>1E-3</v>
+      </c>
+      <c r="AB29" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="AC29" s="12">
+        <v>0</v>
+      </c>
+      <c r="AD29" s="12">
+        <v>1</v>
+      </c>
+      <c r="AE29" s="12">
+        <f t="shared" si="0"/>
+        <v>7.4999999999999997E-3</v>
+      </c>
+      <c r="AF29" s="12">
+        <v>1E-3</v>
+      </c>
+      <c r="AG29" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="AH29" s="12">
+        <v>0</v>
+      </c>
+      <c r="AI29" s="12">
+        <v>1</v>
+      </c>
+      <c r="AJ29" s="12">
+        <v>1</v>
+      </c>
+      <c r="AK29" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="AL29" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="AN29" s="12">
+        <v>0.06</v>
+      </c>
+      <c r="AY29" s="12">
+        <v>15</v>
+      </c>
+      <c r="AZ29" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="BA29" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="BB29" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="BC29" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="BD29" s="12">
+        <v>5</v>
+      </c>
+      <c r="BE29" s="12">
+        <v>8.2199999999999995E-2</v>
+      </c>
+      <c r="BF29" s="12">
+        <v>0.12</v>
+      </c>
+      <c r="BG29" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="BH29" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="BI29" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="BJ29" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="BK29" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="BL29" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="BM29" s="12">
+        <v>1</v>
+      </c>
+      <c r="BN29" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="BO29" s="12" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:67" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
-        <v>74</v>
+        <v>90</v>
       </c>
       <c r="B30" s="12" t="b">
         <v>0</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="D30" s="12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>55</v>
+        <v>63</v>
+      </c>
+      <c r="F30" s="12" t="s">
+        <v>83</v>
       </c>
       <c r="G30" s="12">
-        <v>0.02</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="R30" s="12">
         <v>0.02</v>
@@ -4195,7 +3650,7 @@
         <v>1</v>
       </c>
       <c r="AE30" s="12">
-        <f t="shared" ref="AE30:AE36" si="1">0.15/20</f>
+        <f t="shared" si="0"/>
         <v>7.4999999999999997E-3</v>
       </c>
       <c r="AF30" s="12">
@@ -4211,7 +3666,13 @@
         <v>1</v>
       </c>
       <c r="AJ30" s="12">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="AK30" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="AL30" s="12">
+        <v>0.5</v>
       </c>
       <c r="AN30" s="12">
         <v>0.06</v>
@@ -4234,8 +3695,8 @@
       <c r="BD30" s="12">
         <v>5</v>
       </c>
-      <c r="BE30" s="13">
-        <v>6.7199999999999996E-2</v>
+      <c r="BE30" s="12">
+        <v>8.2199999999999995E-2</v>
       </c>
       <c r="BF30" s="12">
         <v>0.12</v>
@@ -4268,156 +3729,31 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:67" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="B31" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="C31" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="D31" s="12">
-        <v>2</v>
-      </c>
-      <c r="E31" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="G31" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="R31" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="S31" s="12">
-        <v>0</v>
-      </c>
-      <c r="T31" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="U31" s="12">
-        <v>0</v>
-      </c>
-      <c r="V31" s="12">
-        <v>0.9</v>
-      </c>
-      <c r="W31" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="X31" s="12">
-        <v>0</v>
-      </c>
-      <c r="Y31" s="12">
-        <v>0.9</v>
-      </c>
-      <c r="Z31" s="12">
-        <v>0.01</v>
-      </c>
-      <c r="AA31" s="12">
-        <v>1E-3</v>
-      </c>
-      <c r="AB31" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="AC31" s="12">
-        <v>0</v>
-      </c>
-      <c r="AD31" s="12">
-        <v>1</v>
-      </c>
-      <c r="AE31" s="12">
-        <f t="shared" si="1"/>
-        <v>7.4999999999999997E-3</v>
-      </c>
-      <c r="AF31" s="12">
-        <v>1E-3</v>
-      </c>
-      <c r="AG31" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="AH31" s="12">
-        <v>0</v>
-      </c>
-      <c r="AI31" s="12">
-        <v>1</v>
-      </c>
-      <c r="AJ31" s="12">
-        <v>1</v>
-      </c>
-      <c r="AN31" s="12">
-        <v>0.06</v>
-      </c>
-      <c r="AY31" s="12">
-        <v>15</v>
-      </c>
-      <c r="AZ31" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="BA31" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="BB31" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="BC31" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="BD31" s="12">
-        <v>5</v>
-      </c>
-      <c r="BE31" s="13">
-        <v>6.7199999999999996E-2</v>
-      </c>
-      <c r="BF31" s="12">
-        <v>0.12</v>
-      </c>
-      <c r="BG31" s="12">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="BH31" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="BI31" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="BJ31" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="BK31" s="12">
-        <v>0.01</v>
-      </c>
-      <c r="BL31" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="BM31" s="12">
-        <v>1</v>
-      </c>
-      <c r="BN31" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="BO31" s="12" t="b">
-        <v>1</v>
-      </c>
+    <row r="31" spans="1:67" x14ac:dyDescent="0.25">
+      <c r="BJ31" s="12"/>
+      <c r="BK31" s="12"/>
     </row>
     <row r="32" spans="1:67" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="B32" s="12" t="b">
         <v>0</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D32" s="12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E32" s="12" t="s">
-        <v>58</v>
+        <v>55</v>
+      </c>
+      <c r="F32" s="12" t="s">
+        <v>86</v>
       </c>
       <c r="G32" s="12">
-        <v>0.02</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="R32" s="12">
         <v>0.02</v>
@@ -4459,7 +3795,7 @@
         <v>1</v>
       </c>
       <c r="AE32" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>7.4999999999999997E-3</v>
       </c>
       <c r="AF32" s="12">
@@ -4477,6 +3813,9 @@
       <c r="AJ32" s="12">
         <v>1</v>
       </c>
+      <c r="AM32" s="12">
+        <v>0.02</v>
+      </c>
       <c r="AN32" s="12">
         <v>0.06</v>
       </c>
@@ -4498,8 +3837,8 @@
       <c r="BD32" s="12">
         <v>5</v>
       </c>
-      <c r="BE32" s="13">
-        <v>6.7199999999999996E-2</v>
+      <c r="BE32" s="12">
+        <v>8.2199999999999995E-2</v>
       </c>
       <c r="BF32" s="12">
         <v>0.12</v>
@@ -4532,156 +3871,28 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:67" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="B33" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="C33" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="D33" s="12">
-        <v>2</v>
-      </c>
-      <c r="E33" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="G33" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="R33" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="S33" s="12">
-        <v>0</v>
-      </c>
-      <c r="T33" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="U33" s="12">
-        <v>0</v>
-      </c>
-      <c r="V33" s="12">
-        <v>0.9</v>
-      </c>
-      <c r="W33" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="X33" s="12">
-        <v>0</v>
-      </c>
-      <c r="Y33" s="12">
-        <v>0.9</v>
-      </c>
-      <c r="Z33" s="12">
-        <v>0.01</v>
-      </c>
-      <c r="AA33" s="12">
-        <v>1E-3</v>
-      </c>
-      <c r="AB33" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="AC33" s="12">
-        <v>0</v>
-      </c>
-      <c r="AD33" s="12">
-        <v>1</v>
-      </c>
-      <c r="AE33" s="12">
-        <f t="shared" si="1"/>
-        <v>7.4999999999999997E-3</v>
-      </c>
-      <c r="AF33" s="12">
-        <v>1E-3</v>
-      </c>
-      <c r="AG33" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="AH33" s="12">
-        <v>0</v>
-      </c>
-      <c r="AI33" s="12">
-        <v>1</v>
-      </c>
-      <c r="AJ33" s="12">
-        <v>1</v>
-      </c>
-      <c r="AN33" s="12">
-        <v>0.06</v>
-      </c>
-      <c r="AY33" s="12">
-        <v>15</v>
-      </c>
-      <c r="AZ33" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="BA33" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="BB33" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="BC33" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="BD33" s="12">
-        <v>5</v>
-      </c>
-      <c r="BE33" s="13">
-        <v>6.7199999999999996E-2</v>
-      </c>
-      <c r="BF33" s="12">
-        <v>0.12</v>
-      </c>
-      <c r="BG33" s="12">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="BH33" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="BI33" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="BJ33" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="BK33" s="12">
-        <v>0.01</v>
-      </c>
-      <c r="BL33" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="BM33" s="12">
-        <v>1</v>
-      </c>
-      <c r="BN33" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="BO33" s="12" t="b">
-        <v>1</v>
-      </c>
-    </row>
+    <row r="33" spans="1:67" s="12" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="34" spans="1:67" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
-        <v>78</v>
+        <v>96</v>
       </c>
       <c r="B34" s="12" t="b">
         <v>0</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>65</v>
+        <v>81</v>
       </c>
       <c r="D34" s="12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E34" s="12" t="s">
-        <v>60</v>
+        <v>97</v>
+      </c>
+      <c r="F34" s="12" t="s">
+        <v>83</v>
       </c>
       <c r="G34" s="12">
-        <v>0.02</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="R34" s="12">
         <v>0.02</v>
@@ -4690,7 +3901,7 @@
         <v>0</v>
       </c>
       <c r="T34" s="12">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
       <c r="U34" s="12">
         <v>0</v>
@@ -4723,7 +3934,7 @@
         <v>1</v>
       </c>
       <c r="AE34" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>7.4999999999999997E-3</v>
       </c>
       <c r="AF34" s="12">
@@ -4762,8 +3973,8 @@
       <c r="BD34" s="12">
         <v>5</v>
       </c>
-      <c r="BE34" s="13">
-        <v>6.7199999999999996E-2</v>
+      <c r="BE34" s="12">
+        <v>8.2199999999999995E-2</v>
       </c>
       <c r="BF34" s="12">
         <v>0.12</v>
@@ -4775,7 +3986,7 @@
         <v>0.02</v>
       </c>
       <c r="BI34" s="12" t="s">
-        <v>55</v>
+        <v>95</v>
       </c>
       <c r="BJ34" s="12">
         <v>0.02</v>
@@ -4798,22 +4009,25 @@
     </row>
     <row r="35" spans="1:67" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
-        <v>79</v>
+        <v>93</v>
       </c>
       <c r="B35" s="12" t="b">
         <v>0</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D35" s="12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E35" s="12" t="s">
-        <v>63</v>
+        <v>58</v>
+      </c>
+      <c r="F35" s="12" t="s">
+        <v>83</v>
       </c>
       <c r="G35" s="12">
-        <v>0.02</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="R35" s="12">
         <v>0.02</v>
@@ -4822,7 +4036,7 @@
         <v>0</v>
       </c>
       <c r="T35" s="12">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
       <c r="U35" s="12">
         <v>0</v>
@@ -4855,214 +4069,1006 @@
         <v>1</v>
       </c>
       <c r="AE35" s="12">
+        <f t="shared" si="0"/>
+        <v>7.4999999999999997E-3</v>
+      </c>
+      <c r="AF35" s="12">
+        <v>1E-3</v>
+      </c>
+      <c r="AG35" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="AH35" s="12">
+        <v>0</v>
+      </c>
+      <c r="AI35" s="12">
+        <v>1</v>
+      </c>
+      <c r="AJ35" s="12">
+        <v>1</v>
+      </c>
+      <c r="AN35" s="12">
+        <v>0.06</v>
+      </c>
+      <c r="AY35" s="12">
+        <v>15</v>
+      </c>
+      <c r="AZ35" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="BA35" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="BB35" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="BC35" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="BD35" s="12">
+        <v>5</v>
+      </c>
+      <c r="BE35" s="12">
+        <v>8.2199999999999995E-2</v>
+      </c>
+      <c r="BF35" s="12">
+        <v>0.12</v>
+      </c>
+      <c r="BG35" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="BH35" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="BI35" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="BJ35" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="BK35" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="BL35" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="BM35" s="12">
+        <v>1</v>
+      </c>
+      <c r="BN35" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="BO35" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:67" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="B37" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="C37" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="D37" s="12">
+        <v>2</v>
+      </c>
+      <c r="E37" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="G37" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="R37" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="S37" s="12">
+        <v>0</v>
+      </c>
+      <c r="T37" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="U37" s="12">
+        <v>0</v>
+      </c>
+      <c r="V37" s="12">
+        <v>0.9</v>
+      </c>
+      <c r="W37" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="X37" s="12">
+        <v>0</v>
+      </c>
+      <c r="Y37" s="12">
+        <v>0.9</v>
+      </c>
+      <c r="Z37" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="AA37" s="12">
+        <v>1E-3</v>
+      </c>
+      <c r="AB37" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="AC37" s="12">
+        <v>0</v>
+      </c>
+      <c r="AD37" s="12">
+        <v>1</v>
+      </c>
+      <c r="AE37" s="12">
+        <f t="shared" ref="AE37:AE43" si="1">0.15/20</f>
+        <v>7.4999999999999997E-3</v>
+      </c>
+      <c r="AF37" s="12">
+        <v>1E-3</v>
+      </c>
+      <c r="AG37" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="AH37" s="12">
+        <v>0</v>
+      </c>
+      <c r="AI37" s="12">
+        <v>1</v>
+      </c>
+      <c r="AJ37" s="12">
+        <v>1</v>
+      </c>
+      <c r="AN37" s="12">
+        <v>0.06</v>
+      </c>
+      <c r="AY37" s="12">
+        <v>15</v>
+      </c>
+      <c r="AZ37" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="BA37" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="BB37" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="BC37" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="BD37" s="12">
+        <v>5</v>
+      </c>
+      <c r="BE37" s="13">
+        <v>6.7199999999999996E-2</v>
+      </c>
+      <c r="BF37" s="12">
+        <v>0.12</v>
+      </c>
+      <c r="BG37" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="BH37" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="BI37" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="BJ37" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="BK37" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="BL37" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="BM37" s="12">
+        <v>1</v>
+      </c>
+      <c r="BN37" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="BO37" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:67" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="B38" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="C38" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="D38" s="12">
+        <v>2</v>
+      </c>
+      <c r="E38" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="G38" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="R38" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="S38" s="12">
+        <v>0</v>
+      </c>
+      <c r="T38" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="U38" s="12">
+        <v>0</v>
+      </c>
+      <c r="V38" s="12">
+        <v>0.9</v>
+      </c>
+      <c r="W38" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="X38" s="12">
+        <v>0</v>
+      </c>
+      <c r="Y38" s="12">
+        <v>0.9</v>
+      </c>
+      <c r="Z38" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="AA38" s="12">
+        <v>1E-3</v>
+      </c>
+      <c r="AB38" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="AC38" s="12">
+        <v>0</v>
+      </c>
+      <c r="AD38" s="12">
+        <v>1</v>
+      </c>
+      <c r="AE38" s="12">
         <f t="shared" si="1"/>
         <v>7.4999999999999997E-3</v>
       </c>
-      <c r="AF35" s="12">
+      <c r="AF38" s="12">
         <v>1E-3</v>
       </c>
-      <c r="AG35" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="AH35" s="12">
-        <v>0</v>
-      </c>
-      <c r="AI35" s="12">
-        <v>1</v>
-      </c>
-      <c r="AJ35" s="12">
-        <v>1</v>
-      </c>
-      <c r="AN35" s="12">
+      <c r="AG38" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="AH38" s="12">
+        <v>0</v>
+      </c>
+      <c r="AI38" s="12">
+        <v>1</v>
+      </c>
+      <c r="AJ38" s="12">
+        <v>1</v>
+      </c>
+      <c r="AN38" s="12">
         <v>0.06</v>
       </c>
-      <c r="AY35" s="12">
+      <c r="AY38" s="12">
         <v>15</v>
       </c>
-      <c r="AZ35" s="12" t="s">
+      <c r="AZ38" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="BA35" s="12" t="s">
+      <c r="BA38" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="BB35" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="BC35" s="12" t="s">
+      <c r="BB38" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="BC38" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="BD35" s="12">
+      <c r="BD38" s="12">
         <v>5</v>
       </c>
-      <c r="BE35" s="13">
+      <c r="BE38" s="13">
         <v>6.7199999999999996E-2</v>
       </c>
-      <c r="BF35" s="12">
+      <c r="BF38" s="12">
         <v>0.12</v>
       </c>
-      <c r="BG35" s="12">
+      <c r="BG38" s="12">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="BH35" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="BI35" s="12" t="s">
+      <c r="BH38" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="BI38" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="BJ35" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="BK35" s="12">
+      <c r="BJ38" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="BK38" s="12">
         <v>0.01</v>
       </c>
-      <c r="BL35" s="12" t="s">
+      <c r="BL38" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="BM35" s="12">
-        <v>1</v>
-      </c>
-      <c r="BN35" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="BO35" s="12" t="b">
+      <c r="BM38" s="12">
+        <v>1</v>
+      </c>
+      <c r="BN38" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="BO38" s="12" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:67" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="B36" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="C36" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="D36" s="12">
+    <row r="39" spans="1:67" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="B39" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="C39" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="D39" s="12">
         <v>2</v>
       </c>
-      <c r="E36" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="G36" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="R36" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="S36" s="12">
-        <v>0</v>
-      </c>
-      <c r="T36" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="U36" s="12">
-        <v>0</v>
-      </c>
-      <c r="V36" s="12">
+      <c r="E39" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="G39" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="R39" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="S39" s="12">
+        <v>0</v>
+      </c>
+      <c r="T39" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="U39" s="12">
+        <v>0</v>
+      </c>
+      <c r="V39" s="12">
         <v>0.9</v>
       </c>
-      <c r="W36" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="X36" s="12">
-        <v>0</v>
-      </c>
-      <c r="Y36" s="12">
+      <c r="W39" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="X39" s="12">
+        <v>0</v>
+      </c>
+      <c r="Y39" s="12">
         <v>0.9</v>
       </c>
-      <c r="Z36" s="12">
+      <c r="Z39" s="12">
         <v>0.01</v>
       </c>
-      <c r="AA36" s="12">
+      <c r="AA39" s="12">
         <v>1E-3</v>
       </c>
-      <c r="AB36" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="AC36" s="12">
-        <v>0</v>
-      </c>
-      <c r="AD36" s="12">
-        <v>1</v>
-      </c>
-      <c r="AE36" s="12">
+      <c r="AB39" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="AC39" s="12">
+        <v>0</v>
+      </c>
+      <c r="AD39" s="12">
+        <v>1</v>
+      </c>
+      <c r="AE39" s="12">
         <f t="shared" si="1"/>
         <v>7.4999999999999997E-3</v>
       </c>
-      <c r="AF36" s="12">
+      <c r="AF39" s="12">
         <v>1E-3</v>
       </c>
-      <c r="AG36" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="AH36" s="12">
-        <v>0</v>
-      </c>
-      <c r="AI36" s="12">
-        <v>1</v>
-      </c>
-      <c r="AJ36" s="12">
+      <c r="AG39" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="AH39" s="12">
+        <v>0</v>
+      </c>
+      <c r="AI39" s="12">
+        <v>1</v>
+      </c>
+      <c r="AJ39" s="12">
+        <v>1</v>
+      </c>
+      <c r="AN39" s="12">
+        <v>0.06</v>
+      </c>
+      <c r="AY39" s="12">
+        <v>15</v>
+      </c>
+      <c r="AZ39" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="BA39" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="BB39" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="BC39" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="BD39" s="12">
+        <v>5</v>
+      </c>
+      <c r="BE39" s="13">
+        <v>6.7199999999999996E-2</v>
+      </c>
+      <c r="BF39" s="12">
+        <v>0.12</v>
+      </c>
+      <c r="BG39" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="BH39" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="BI39" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="BJ39" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="BK39" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="BL39" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="BM39" s="12">
+        <v>1</v>
+      </c>
+      <c r="BN39" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="BO39" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:67" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="B40" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="C40" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="D40" s="12">
         <v>2</v>
       </c>
-      <c r="AN36" s="12">
+      <c r="E40" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="G40" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="R40" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="S40" s="12">
+        <v>0</v>
+      </c>
+      <c r="T40" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="U40" s="12">
+        <v>0</v>
+      </c>
+      <c r="V40" s="12">
+        <v>0.9</v>
+      </c>
+      <c r="W40" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="X40" s="12">
+        <v>0</v>
+      </c>
+      <c r="Y40" s="12">
+        <v>0.9</v>
+      </c>
+      <c r="Z40" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="AA40" s="12">
+        <v>1E-3</v>
+      </c>
+      <c r="AB40" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="AC40" s="12">
+        <v>0</v>
+      </c>
+      <c r="AD40" s="12">
+        <v>1</v>
+      </c>
+      <c r="AE40" s="12">
+        <f t="shared" si="1"/>
+        <v>7.4999999999999997E-3</v>
+      </c>
+      <c r="AF40" s="12">
+        <v>1E-3</v>
+      </c>
+      <c r="AG40" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="AH40" s="12">
+        <v>0</v>
+      </c>
+      <c r="AI40" s="12">
+        <v>1</v>
+      </c>
+      <c r="AJ40" s="12">
+        <v>1</v>
+      </c>
+      <c r="AN40" s="12">
         <v>0.06</v>
       </c>
-      <c r="AY36" s="12">
+      <c r="AY40" s="12">
         <v>15</v>
       </c>
-      <c r="AZ36" s="12" t="s">
+      <c r="AZ40" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="BA36" s="12" t="s">
+      <c r="BA40" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="BB36" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="BC36" s="12" t="s">
+      <c r="BB40" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="BC40" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="BD36" s="12">
+      <c r="BD40" s="12">
         <v>5</v>
       </c>
-      <c r="BE36" s="13">
+      <c r="BE40" s="13">
         <v>6.7199999999999996E-2</v>
       </c>
-      <c r="BF36" s="12">
+      <c r="BF40" s="12">
         <v>0.12</v>
       </c>
-      <c r="BG36" s="12">
+      <c r="BG40" s="12">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="BH36" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="BI36" s="12" t="s">
+      <c r="BH40" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="BI40" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="BJ36" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="BK36" s="12">
+      <c r="BJ40" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="BK40" s="12">
         <v>0.01</v>
       </c>
-      <c r="BL36" s="12" t="s">
+      <c r="BL40" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="BM36" s="12">
-        <v>1</v>
-      </c>
-      <c r="BN36" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="BO36" s="12" t="b">
+      <c r="BM40" s="12">
+        <v>1</v>
+      </c>
+      <c r="BN40" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="BO40" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:67" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="B41" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="C41" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="D41" s="12">
+        <v>2</v>
+      </c>
+      <c r="E41" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="G41" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="R41" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="S41" s="12">
+        <v>0</v>
+      </c>
+      <c r="T41" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="U41" s="12">
+        <v>0</v>
+      </c>
+      <c r="V41" s="12">
+        <v>0.9</v>
+      </c>
+      <c r="W41" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="X41" s="12">
+        <v>0</v>
+      </c>
+      <c r="Y41" s="12">
+        <v>0.9</v>
+      </c>
+      <c r="Z41" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="AA41" s="12">
+        <v>1E-3</v>
+      </c>
+      <c r="AB41" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="AC41" s="12">
+        <v>0</v>
+      </c>
+      <c r="AD41" s="12">
+        <v>1</v>
+      </c>
+      <c r="AE41" s="12">
+        <f t="shared" si="1"/>
+        <v>7.4999999999999997E-3</v>
+      </c>
+      <c r="AF41" s="12">
+        <v>1E-3</v>
+      </c>
+      <c r="AG41" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="AH41" s="12">
+        <v>0</v>
+      </c>
+      <c r="AI41" s="12">
+        <v>1</v>
+      </c>
+      <c r="AJ41" s="12">
+        <v>1</v>
+      </c>
+      <c r="AN41" s="12">
+        <v>0.06</v>
+      </c>
+      <c r="AY41" s="12">
+        <v>15</v>
+      </c>
+      <c r="AZ41" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="BA41" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="BB41" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="BC41" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="BD41" s="12">
+        <v>5</v>
+      </c>
+      <c r="BE41" s="13">
+        <v>6.7199999999999996E-2</v>
+      </c>
+      <c r="BF41" s="12">
+        <v>0.12</v>
+      </c>
+      <c r="BG41" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="BH41" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="BI41" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="BJ41" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="BK41" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="BL41" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="BM41" s="12">
+        <v>1</v>
+      </c>
+      <c r="BN41" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="BO41" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:67" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="B42" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="C42" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="D42" s="12">
+        <v>2</v>
+      </c>
+      <c r="E42" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="G42" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="R42" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="S42" s="12">
+        <v>0</v>
+      </c>
+      <c r="T42" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="U42" s="12">
+        <v>0</v>
+      </c>
+      <c r="V42" s="12">
+        <v>0.9</v>
+      </c>
+      <c r="W42" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="X42" s="12">
+        <v>0</v>
+      </c>
+      <c r="Y42" s="12">
+        <v>0.9</v>
+      </c>
+      <c r="Z42" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="AA42" s="12">
+        <v>1E-3</v>
+      </c>
+      <c r="AB42" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="AC42" s="12">
+        <v>0</v>
+      </c>
+      <c r="AD42" s="12">
+        <v>1</v>
+      </c>
+      <c r="AE42" s="12">
+        <f t="shared" si="1"/>
+        <v>7.4999999999999997E-3</v>
+      </c>
+      <c r="AF42" s="12">
+        <v>1E-3</v>
+      </c>
+      <c r="AG42" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="AH42" s="12">
+        <v>0</v>
+      </c>
+      <c r="AI42" s="12">
+        <v>1</v>
+      </c>
+      <c r="AJ42" s="12">
+        <v>1</v>
+      </c>
+      <c r="AN42" s="12">
+        <v>0.06</v>
+      </c>
+      <c r="AY42" s="12">
+        <v>15</v>
+      </c>
+      <c r="AZ42" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="BA42" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="BB42" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="BC42" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="BD42" s="12">
+        <v>5</v>
+      </c>
+      <c r="BE42" s="13">
+        <v>6.7199999999999996E-2</v>
+      </c>
+      <c r="BF42" s="12">
+        <v>0.12</v>
+      </c>
+      <c r="BG42" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="BH42" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="BI42" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="BJ42" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="BK42" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="BL42" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="BM42" s="12">
+        <v>1</v>
+      </c>
+      <c r="BN42" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="BO42" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:67" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="B43" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="C43" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="D43" s="12">
+        <v>2</v>
+      </c>
+      <c r="E43" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="G43" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="R43" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="S43" s="12">
+        <v>0</v>
+      </c>
+      <c r="T43" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="U43" s="12">
+        <v>0</v>
+      </c>
+      <c r="V43" s="12">
+        <v>0.9</v>
+      </c>
+      <c r="W43" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="X43" s="12">
+        <v>0</v>
+      </c>
+      <c r="Y43" s="12">
+        <v>0.9</v>
+      </c>
+      <c r="Z43" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="AA43" s="12">
+        <v>1E-3</v>
+      </c>
+      <c r="AB43" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="AC43" s="12">
+        <v>0</v>
+      </c>
+      <c r="AD43" s="12">
+        <v>1</v>
+      </c>
+      <c r="AE43" s="12">
+        <f t="shared" si="1"/>
+        <v>7.4999999999999997E-3</v>
+      </c>
+      <c r="AF43" s="12">
+        <v>1E-3</v>
+      </c>
+      <c r="AG43" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="AH43" s="12">
+        <v>0</v>
+      </c>
+      <c r="AI43" s="12">
+        <v>1</v>
+      </c>
+      <c r="AJ43" s="12">
+        <v>2</v>
+      </c>
+      <c r="AN43" s="12">
+        <v>0.06</v>
+      </c>
+      <c r="AY43" s="12">
+        <v>15</v>
+      </c>
+      <c r="AZ43" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="BA43" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="BB43" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="BC43" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="BD43" s="12">
+        <v>5</v>
+      </c>
+      <c r="BE43" s="13">
+        <v>6.7199999999999996E-2</v>
+      </c>
+      <c r="BF43" s="12">
+        <v>0.12</v>
+      </c>
+      <c r="BG43" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="BH43" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="BI43" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="BJ43" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="BK43" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="BL43" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="BM43" s="12">
+        <v>1</v>
+      </c>
+      <c r="BN43" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="BO43" s="12" t="b">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B30:B36 B25:B28 B3:B23" xr:uid="{05E01AB2-72EC-4550-ACB8-4E83765DE296}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B37:B43 B32:B35 B3:B30" xr:uid="{05E01AB2-72EC-4550-ACB8-4E83765DE296}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3 H5:H8 H10:H12" xr:uid="{8DBFC5CB-438A-4309-B948-24597CAE3D7F}">

</xml_diff>

<commit_message>
add prelim component for SDRS cola policy
</commit_message>
<xml_diff>
--- a/RunControl.xlsx
+++ b/RunControl.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F45A375-C4DF-4B0A-AB6D-A6134485FDDE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72EC65A2-A7F5-4EA2-B3DF-AF70C3054133}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="paramlist" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="140">
   <si>
     <t>runname</t>
   </si>
@@ -447,6 +447,9 @@
   </si>
   <si>
     <t xml:space="preserve">EEC Policies </t>
+  </si>
+  <si>
+    <t>cola_SDRS</t>
   </si>
 </sst>
 </file>
@@ -846,11 +849,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BO43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="6" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C9" sqref="C9"/>
+      <selection pane="bottomRight" activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1178,7 +1181,7 @@
         <v>33</v>
       </c>
       <c r="B3" s="12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3" s="12">
         <v>1</v>
@@ -2615,7 +2618,186 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:67" s="12" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:67" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="B13" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="D13" s="12">
+        <v>1</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="G13" s="12">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="H13" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="I13" s="12">
+        <v>1</v>
+      </c>
+      <c r="J13" s="12">
+        <v>1</v>
+      </c>
+      <c r="K13" s="12">
+        <v>1</v>
+      </c>
+      <c r="L13" s="12">
+        <v>0.06</v>
+      </c>
+      <c r="M13" s="12">
+        <v>0.06</v>
+      </c>
+      <c r="R13" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="S13" s="12">
+        <v>0</v>
+      </c>
+      <c r="T13" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="U13" s="12">
+        <v>0</v>
+      </c>
+      <c r="V13" s="12">
+        <v>0.9</v>
+      </c>
+      <c r="W13" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="X13" s="12">
+        <v>0</v>
+      </c>
+      <c r="Y13" s="12">
+        <v>0.9</v>
+      </c>
+      <c r="Z13" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="AA13" s="12">
+        <v>1E-3</v>
+      </c>
+      <c r="AB13" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="AC13" s="12">
+        <v>0</v>
+      </c>
+      <c r="AD13" s="12">
+        <v>1</v>
+      </c>
+      <c r="AE13" s="12">
+        <f t="shared" si="0"/>
+        <v>7.4999999999999997E-3</v>
+      </c>
+      <c r="AF13" s="12">
+        <v>1E-3</v>
+      </c>
+      <c r="AG13" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="AH13" s="12">
+        <v>0</v>
+      </c>
+      <c r="AI13" s="12">
+        <v>1</v>
+      </c>
+      <c r="AJ13" s="12">
+        <v>1</v>
+      </c>
+      <c r="AN13" s="12">
+        <v>0.06</v>
+      </c>
+      <c r="AO13" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="AP13" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="AQ13" s="12">
+        <v>0.04</v>
+      </c>
+      <c r="AR13" s="12">
+        <v>0.08</v>
+      </c>
+      <c r="AS13" s="12">
+        <v>0.04</v>
+      </c>
+      <c r="AT13" s="12">
+        <v>0.11</v>
+      </c>
+      <c r="AU13" s="12">
+        <v>0.04</v>
+      </c>
+      <c r="AV13" s="12">
+        <v>0.08</v>
+      </c>
+      <c r="AW13" s="12">
+        <v>0.7</v>
+      </c>
+      <c r="AX13" s="12">
+        <v>1</v>
+      </c>
+      <c r="AY13" s="12">
+        <v>15</v>
+      </c>
+      <c r="AZ13" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="BA13" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="BB13" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="BC13" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="BD13" s="12">
+        <v>5</v>
+      </c>
+      <c r="BE13" s="12">
+        <v>8.2199999999999995E-2</v>
+      </c>
+      <c r="BF13" s="12">
+        <v>0.12</v>
+      </c>
+      <c r="BG13" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="BH13" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="BI13" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="BJ13" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="BK13" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="BL13" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="BM13" s="12">
+        <v>0.75</v>
+      </c>
+      <c r="BN13" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="BO13" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
     <row r="14" spans="1:67" s="12" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="1:67" s="12" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="1:67" s="12" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -5071,7 +5253,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B37:B43 B32:B35 B3:B30" xr:uid="{05E01AB2-72EC-4550-ACB8-4E83765DE296}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3 H5:H8 H10:H12" xr:uid="{8DBFC5CB-438A-4309-B948-24597CAE3D7F}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3 H5:H8 H10:H13" xr:uid="{8DBFC5CB-438A-4309-B948-24597CAE3D7F}">
       <formula1>"preSet, ALpct,MApct"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5084,7 +5266,7 @@
           <x14:formula1>
             <xm:f>Policies!$B$3:$B$8</xm:f>
           </x14:formula1>
-          <xm:sqref>F3 F5:F8 F10:F12</xm:sqref>
+          <xm:sqref>F3 F5:F8 F10:F13</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -5096,7 +5278,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC498317-3D78-4815-AFC0-F5D6A2FF4B8F}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
working version for SDRS policy
</commit_message>
<xml_diff>
--- a/RunControl.xlsx
+++ b/RunControl.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72EC65A2-A7F5-4EA2-B3DF-AF70C3054133}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{206C7AD4-0B6C-45FA-BE37-4453CCAFFA98}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="paramlist" sheetId="1" r:id="rId1"/>
@@ -850,10 +850,10 @@
   <dimension ref="A1:BO43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="2" topLeftCell="AZ3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B17" sqref="B17"/>
+      <selection pane="bottomRight" activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -863,7 +863,7 @@
     <col min="3" max="4" width="11.7109375" customWidth="1"/>
     <col min="5" max="5" width="11.140625" customWidth="1"/>
     <col min="6" max="6" width="14.28515625" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" customWidth="1"/>
     <col min="8" max="8" width="22.28515625" customWidth="1"/>
     <col min="9" max="13" width="12.85546875" customWidth="1"/>
     <col min="14" max="17" width="17.140625" customWidth="1"/>
@@ -875,8 +875,10 @@
     <col min="28" max="31" width="14.28515625" customWidth="1"/>
     <col min="32" max="32" width="23.42578125" customWidth="1"/>
     <col min="33" max="35" width="14.28515625" customWidth="1"/>
-    <col min="36" max="37" width="17.42578125" customWidth="1"/>
-    <col min="38" max="39" width="14.28515625" customWidth="1"/>
+    <col min="36" max="36" width="17.42578125" customWidth="1"/>
+    <col min="37" max="37" width="18" customWidth="1"/>
+    <col min="38" max="38" width="18.85546875" customWidth="1"/>
+    <col min="39" max="39" width="14.28515625" customWidth="1"/>
     <col min="40" max="40" width="18.5703125" style="12" customWidth="1"/>
     <col min="41" max="41" width="20.28515625" style="12" customWidth="1"/>
     <col min="42" max="42" width="21.42578125" style="12" customWidth="1"/>
@@ -2258,7 +2260,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:67" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:67" s="12" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>62</v>
       </c>
@@ -2711,7 +2713,13 @@
         <v>1</v>
       </c>
       <c r="AJ13" s="12">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="AK13" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="AL13" s="12">
+        <v>0.5</v>
       </c>
       <c r="AN13" s="12">
         <v>0.06</v>

</xml_diff>

<commit_message>
incorporate SDRS policy into DB
</commit_message>
<xml_diff>
--- a/RunControl.xlsx
+++ b/RunControl.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{206C7AD4-0B6C-45FA-BE37-4453CCAFFA98}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7C16E64-3A56-4338-9424-60DB41A1BA2F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="142">
   <si>
     <t>runname</t>
   </si>
@@ -450,6 +450,12 @@
   </si>
   <si>
     <t>cola_SDRS</t>
+  </si>
+  <si>
+    <t>DC_hybrid</t>
+  </si>
+  <si>
+    <t>DC_pure</t>
   </si>
 </sst>
 </file>
@@ -850,10 +856,10 @@
   <dimension ref="A1:BO43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6" ySplit="2" topLeftCell="AZ3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="2" topLeftCell="O3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C18" sqref="C18"/>
+      <selection pane="bottomRight" activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2085,7 +2091,7 @@
         <v>61</v>
       </c>
       <c r="B10" s="12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10" s="12">
         <v>1</v>
@@ -2265,7 +2271,7 @@
         <v>62</v>
       </c>
       <c r="B11" s="12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11" s="12">
         <v>1</v>
@@ -2445,7 +2451,7 @@
         <v>137</v>
       </c>
       <c r="B12" s="12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D12" s="12">
         <v>1</v>
@@ -2808,8 +2814,191 @@
     </row>
     <row r="14" spans="1:67" s="12" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="1:67" s="12" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:67" s="12" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="17" spans="1:67" s="12" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:67" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="B16" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="D16" s="12">
+        <v>1</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="G16" s="12">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="H16" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="I16" s="12">
+        <v>1</v>
+      </c>
+      <c r="J16" s="12">
+        <v>1</v>
+      </c>
+      <c r="K16" s="12">
+        <v>1</v>
+      </c>
+      <c r="L16" s="12">
+        <v>0.06</v>
+      </c>
+      <c r="M16" s="12">
+        <v>0.06</v>
+      </c>
+      <c r="R16" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="S16" s="12">
+        <v>0</v>
+      </c>
+      <c r="T16" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="U16" s="12">
+        <v>0</v>
+      </c>
+      <c r="V16" s="12">
+        <v>0.9</v>
+      </c>
+      <c r="W16" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="X16" s="12">
+        <v>0</v>
+      </c>
+      <c r="Y16" s="12">
+        <v>0.9</v>
+      </c>
+      <c r="Z16" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="AA16" s="12">
+        <v>1E-3</v>
+      </c>
+      <c r="AB16" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="AC16" s="12">
+        <v>0</v>
+      </c>
+      <c r="AD16" s="12">
+        <v>1</v>
+      </c>
+      <c r="AE16" s="12">
+        <f t="shared" si="0"/>
+        <v>7.4999999999999997E-3</v>
+      </c>
+      <c r="AF16" s="12">
+        <v>1E-3</v>
+      </c>
+      <c r="AG16" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="AH16" s="12">
+        <v>0</v>
+      </c>
+      <c r="AI16" s="12">
+        <v>1</v>
+      </c>
+      <c r="AJ16" s="12">
+        <v>1</v>
+      </c>
+      <c r="AN16" s="12">
+        <v>0.06</v>
+      </c>
+      <c r="AO16" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="AP16" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="AQ16" s="12">
+        <v>0.04</v>
+      </c>
+      <c r="AR16" s="12">
+        <v>0.08</v>
+      </c>
+      <c r="AS16" s="12">
+        <v>0.04</v>
+      </c>
+      <c r="AT16" s="12">
+        <v>0.11</v>
+      </c>
+      <c r="AU16" s="12">
+        <v>0.04</v>
+      </c>
+      <c r="AV16" s="12">
+        <v>0.08</v>
+      </c>
+      <c r="AW16" s="12">
+        <v>0.7</v>
+      </c>
+      <c r="AX16" s="12">
+        <v>1</v>
+      </c>
+      <c r="AY16" s="12">
+        <v>15</v>
+      </c>
+      <c r="AZ16" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="BA16" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="BB16" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="BC16" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="BD16" s="12">
+        <v>5</v>
+      </c>
+      <c r="BE16" s="12">
+        <v>8.2199999999999995E-2</v>
+      </c>
+      <c r="BF16" s="12">
+        <v>0.12</v>
+      </c>
+      <c r="BG16" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="BH16" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="BI16" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="BJ16" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="BK16" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="BL16" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="BM16" s="12">
+        <v>0.75</v>
+      </c>
+      <c r="BN16" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="BO16" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:67" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="12" t="s">
+        <v>141</v>
+      </c>
+    </row>
     <row r="18" spans="1:67" s="12" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="19" spans="1:67" s="12" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:67" s="12" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -5261,7 +5450,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B37:B43 B32:B35 B3:B30" xr:uid="{05E01AB2-72EC-4550-ACB8-4E83765DE296}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3 H5:H8 H10:H13" xr:uid="{8DBFC5CB-438A-4309-B948-24597CAE3D7F}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3 H5:H8 H10:H13 H16" xr:uid="{8DBFC5CB-438A-4309-B948-24597CAE3D7F}">
       <formula1>"preSet, ALpct,MApct"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5274,7 +5463,7 @@
           <x14:formula1>
             <xm:f>Policies!$B$3:$B$8</xm:f>
           </x14:formula1>
-          <xm:sqref>F3 F5:F8 F10:F13</xm:sqref>
+          <xm:sqref>F3 F5:F8 F10:F13 F16</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
remove more output files
</commit_message>
<xml_diff>
--- a/RunControl.xlsx
+++ b/RunControl.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{929859ED-0EEA-40C4-8A05-1192B72C4E69}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09FC7885-79D9-4CD4-8920-FDBCF095F042}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -845,7 +845,7 @@
       <pane xSplit="6" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D21" sqref="D21"/>
+      <selection pane="bottomRight" activeCell="M29" sqref="M29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
update analysis of DC plan
</commit_message>
<xml_diff>
--- a/RunControl.xlsx
+++ b/RunControl.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69B0DA5A-1BA2-4863-842A-9288CD6AD899}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2EAE392-AB77-4ABA-AF04-FDB9AC1D7922}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -848,7 +848,7 @@
       <pane xSplit="6" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D23" sqref="D23"/>
+      <selection pane="bottomRight" activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1307,7 +1307,7 @@
         <v>140</v>
       </c>
       <c r="B5" s="10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>140</v>
@@ -1460,7 +1460,7 @@
         <v>127</v>
       </c>
       <c r="B7" s="10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>137</v>
@@ -1612,7 +1612,7 @@
         <v>130</v>
       </c>
       <c r="B8" s="10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>137</v>
@@ -1764,7 +1764,7 @@
         <v>115</v>
       </c>
       <c r="B9" s="10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>137</v>
@@ -1916,7 +1916,7 @@
         <v>116</v>
       </c>
       <c r="B10" s="10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10" s="10" t="s">
         <v>137</v>
@@ -2069,7 +2069,7 @@
         <v>56</v>
       </c>
       <c r="B12" s="10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C12" s="10" t="s">
         <v>138</v>
@@ -2221,7 +2221,7 @@
         <v>57</v>
       </c>
       <c r="B13" s="10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13" s="10" t="s">
         <v>138</v>
@@ -2373,7 +2373,7 @@
         <v>131</v>
       </c>
       <c r="B14" s="10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C14" s="10" t="s">
         <v>138</v>
@@ -2525,7 +2525,7 @@
         <v>133</v>
       </c>
       <c r="B15" s="10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C15" s="10" t="s">
         <v>138</v>
@@ -5071,7 +5071,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5104,7 +5104,7 @@
         <v>91</v>
       </c>
       <c r="B2">
-        <v>2000</v>
+        <v>500</v>
       </c>
       <c r="C2">
         <v>6</v>

</xml_diff>

<commit_message>
make updating benefit faster
</commit_message>
<xml_diff>
--- a/RunControl.xlsx
+++ b/RunControl.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB9C0DBC-550A-4BE6-B6B2-4D2D5D8AD151}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{523A9C40-090D-40F0-9328-FBD8856FC90F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="paramlist" sheetId="1" r:id="rId1"/>
@@ -856,11 +856,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BK48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="6" ySplit="2" topLeftCell="AG3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C24" sqref="C24"/>
+      <selection pane="bottomRight" activeCell="AG25" sqref="AG25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1326,7 +1326,7 @@
         <v>140</v>
       </c>
       <c r="B5" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>140</v>
@@ -1482,7 +1482,7 @@
         <v>127</v>
       </c>
       <c r="B7" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>137</v>
@@ -1637,7 +1637,7 @@
         <v>143</v>
       </c>
       <c r="B8" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>137</v>
@@ -1792,7 +1792,7 @@
         <v>130</v>
       </c>
       <c r="B9" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>137</v>
@@ -1947,7 +1947,7 @@
         <v>115</v>
       </c>
       <c r="B10" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10" s="10" t="s">
         <v>137</v>
@@ -2102,7 +2102,7 @@
         <v>116</v>
       </c>
       <c r="B11" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11" s="10" t="s">
         <v>137</v>
@@ -2258,7 +2258,7 @@
         <v>56</v>
       </c>
       <c r="B13" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13" s="10" t="s">
         <v>138</v>
@@ -2413,7 +2413,7 @@
         <v>57</v>
       </c>
       <c r="B14" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14" s="10" t="s">
         <v>138</v>
@@ -2568,7 +2568,7 @@
         <v>131</v>
       </c>
       <c r="B15" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C15" s="10" t="s">
         <v>138</v>
@@ -2879,14 +2879,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:63" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="1:63" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
     <row r="18" spans="1:63" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="19" spans="1:63" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
         <v>135</v>
       </c>
       <c r="B19" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C19" s="10" t="s">
         <v>139</v>
@@ -5274,8 +5278,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC498317-3D78-4815-AFC0-F5D6A2FF4B8F}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P16" sqref="P16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5314,7 +5318,7 @@
         <v>500</v>
       </c>
       <c r="C2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2">
         <v>20</v>

</xml_diff>

<commit_message>
add figures for MFC2020
</commit_message>
<xml_diff>
--- a/RunControl.xlsx
+++ b/RunControl.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1E313AA-71E5-495D-9B65-29C718B36091}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0720751E-E388-45D4-8FC1-9071112643D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="18240" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="18240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="paramlist" sheetId="1" r:id="rId1"/>
@@ -891,7 +891,7 @@
       <pane xSplit="6" ySplit="2" topLeftCell="Q3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="S25" sqref="S25"/>
+      <selection pane="bottomRight" activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6854,8 +6854,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N23" sqref="N23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6891,7 +6891,7 @@
         <v>91</v>
       </c>
       <c r="B2">
-        <v>2000</v>
+        <v>500</v>
       </c>
       <c r="C2">
         <v>4</v>
@@ -6919,7 +6919,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A2:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
prepare tables for calibrated runs
</commit_message>
<xml_diff>
--- a/RunControl.xlsx
+++ b/RunControl.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E041E56A-4F36-43C0-B33A-F3D2DE6BA7CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03CD114D-463D-4E7B-BCE1-4F0AA962A651}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="142">
   <si>
     <t>runname</t>
   </si>
@@ -444,6 +444,18 @@
   </si>
   <si>
     <t>cola_returnSmooth_FR100</t>
+  </si>
+  <si>
+    <t>cola_returnSmooth_calib</t>
+  </si>
+  <si>
+    <t>cola_FR_calib</t>
+  </si>
+  <si>
+    <t>cola_returnSmooth_calib_FR100</t>
+  </si>
+  <si>
+    <t>cola_FR_calib_FR100</t>
   </si>
 </sst>
 </file>
@@ -814,22 +826,22 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:BK38"/>
+  <dimension ref="A1:BK42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6" ySplit="2" topLeftCell="AN3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="2" topLeftCell="O3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AN44" sqref="AN44"/>
+      <selection pane="bottomRight" activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" customWidth="1"/>
+    <col min="1" max="1" width="30.85546875" customWidth="1"/>
     <col min="2" max="2" width="10.140625" customWidth="1"/>
     <col min="3" max="4" width="11.7109375" customWidth="1"/>
     <col min="5" max="5" width="11.140625" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" customWidth="1"/>
     <col min="7" max="7" width="16.5703125" customWidth="1"/>
     <col min="8" max="8" width="11.7109375" customWidth="1"/>
     <col min="9" max="13" width="12.85546875" customWidth="1"/>
@@ -1161,6 +1173,9 @@
       <c r="Q3" s="10">
         <v>0</v>
       </c>
+      <c r="R3" s="10">
+        <v>1</v>
+      </c>
       <c r="S3" s="10">
         <v>0.02</v>
       </c>
@@ -1220,6 +1235,9 @@
       </c>
       <c r="AO3" s="10">
         <v>0.11</v>
+      </c>
+      <c r="AP3" s="10">
+        <v>1</v>
       </c>
       <c r="AQ3" s="10">
         <v>0.03</v>
@@ -1320,6 +1338,9 @@
       <c r="Q5" s="10">
         <v>0</v>
       </c>
+      <c r="R5" s="10">
+        <v>1</v>
+      </c>
       <c r="S5" s="10">
         <v>0.02</v>
       </c>
@@ -1379,6 +1400,9 @@
       </c>
       <c r="AO5" s="10">
         <v>0.11</v>
+      </c>
+      <c r="AP5" s="10">
+        <v>1</v>
       </c>
       <c r="AQ5" s="10">
         <v>0.03</v>
@@ -1478,6 +1502,9 @@
       <c r="Q6" s="10">
         <v>0</v>
       </c>
+      <c r="R6" s="10">
+        <v>1</v>
+      </c>
       <c r="S6" s="10">
         <v>0.02</v>
       </c>
@@ -1537,6 +1564,9 @@
       </c>
       <c r="AO6" s="10">
         <v>0.11</v>
+      </c>
+      <c r="AP6" s="10">
+        <v>1</v>
       </c>
       <c r="AQ6" s="10">
         <v>0.03</v>
@@ -2024,6 +2054,9 @@
       <c r="AO9" s="10">
         <v>0.11</v>
       </c>
+      <c r="AP9" s="10">
+        <v>1</v>
+      </c>
       <c r="AQ9" s="10">
         <v>0.03</v>
       </c>
@@ -2286,7 +2319,7 @@
       <c r="Q11" s="10">
         <v>0</v>
       </c>
-      <c r="R11" s="10">
+      <c r="R11" s="14">
         <v>5</v>
       </c>
       <c r="S11" s="10">
@@ -2416,9 +2449,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:63" s="10" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:63" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
-        <v>55</v>
+        <v>138</v>
       </c>
       <c r="B12" s="10" t="b">
         <v>0</v>
@@ -2430,7 +2463,7 @@
         <v>1</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F12" s="10" t="s">
         <v>63</v>
@@ -2445,10 +2478,13 @@
         <v>135</v>
       </c>
       <c r="P12" s="10">
-        <v>0.02</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="Q12" s="10">
-        <v>0</v>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="R12" s="14">
+        <v>5</v>
       </c>
       <c r="S12" s="10">
         <v>0.02</v>
@@ -2510,6 +2546,9 @@
       <c r="AO12" s="10">
         <v>0.11</v>
       </c>
+      <c r="AP12" s="10">
+        <v>5</v>
+      </c>
       <c r="AQ12" s="10">
         <v>0.03</v>
       </c>
@@ -2574,9 +2613,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:63" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:63" s="10" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
-        <v>104</v>
+        <v>55</v>
       </c>
       <c r="B13" s="10" t="b">
         <v>0</v>
@@ -2588,7 +2627,7 @@
         <v>1</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F13" s="10" t="s">
         <v>63</v>
@@ -2608,6 +2647,9 @@
       <c r="Q13" s="10">
         <v>0</v>
       </c>
+      <c r="R13" s="10">
+        <v>1</v>
+      </c>
       <c r="S13" s="10">
         <v>0.02</v>
       </c>
@@ -2668,6 +2710,9 @@
       <c r="AO13" s="10">
         <v>0.11</v>
       </c>
+      <c r="AP13" s="10">
+        <v>1</v>
+      </c>
       <c r="AQ13" s="10">
         <v>0.03</v>
       </c>
@@ -2732,9 +2777,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:63" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:63" s="10" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
-        <v>106</v>
+        <v>139</v>
       </c>
       <c r="B14" s="10" t="b">
         <v>0</v>
@@ -2746,7 +2791,7 @@
         <v>1</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="F14" s="10" t="s">
         <v>63</v>
@@ -2766,14 +2811,17 @@
       <c r="Q14" s="10">
         <v>0</v>
       </c>
+      <c r="R14" s="10">
+        <v>1</v>
+      </c>
       <c r="S14" s="10">
-        <v>0.02</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="T14" s="10">
-        <v>0</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="U14" s="10">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="V14" s="10">
         <v>0.02</v>
@@ -2800,13 +2848,7 @@
         <v>1</v>
       </c>
       <c r="AD14" s="10">
-        <v>2</v>
-      </c>
-      <c r="AE14" s="10">
-        <v>0.5</v>
-      </c>
-      <c r="AF14" s="10">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="AH14" s="10">
         <v>0.05</v>
@@ -2831,6 +2873,9 @@
       </c>
       <c r="AO14" s="10">
         <v>0.11</v>
+      </c>
+      <c r="AP14" s="10">
+        <v>1</v>
       </c>
       <c r="AQ14" s="10">
         <v>0.03</v>
@@ -2898,19 +2943,19 @@
     </row>
     <row r="15" spans="1:63" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B15" s="10" t="b">
         <v>0</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D15" s="10">
         <v>1</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="F15" s="10" t="s">
         <v>63</v>
@@ -2918,6 +2963,9 @@
       <c r="G15" s="10">
         <v>1.4999999999999999E-2</v>
       </c>
+      <c r="H15" s="10" t="s">
+        <v>77</v>
+      </c>
       <c r="N15" s="10" t="s">
         <v>135</v>
       </c>
@@ -2927,6 +2975,9 @@
       <c r="Q15" s="10">
         <v>0</v>
       </c>
+      <c r="R15" s="10">
+        <v>1</v>
+      </c>
       <c r="S15" s="10">
         <v>0.02</v>
       </c>
@@ -2987,6 +3038,9 @@
       <c r="AO15" s="10">
         <v>0.11</v>
       </c>
+      <c r="AP15" s="10">
+        <v>1</v>
+      </c>
       <c r="AQ15" s="10">
         <v>0.03</v>
       </c>
@@ -3051,16 +3105,185 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:63" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:63" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="B16" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="D16" s="10">
+        <v>1</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="G16" s="10">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="H16" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="N16" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="P16" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="Q16" s="10">
+        <v>0</v>
+      </c>
+      <c r="R16" s="10">
+        <v>1</v>
+      </c>
+      <c r="S16" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="T16" s="10">
+        <v>0</v>
+      </c>
+      <c r="U16" s="10">
+        <v>0.9</v>
+      </c>
+      <c r="V16" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="W16" s="10">
+        <v>0</v>
+      </c>
+      <c r="X16" s="10">
+        <v>0.9</v>
+      </c>
+      <c r="Y16" s="10">
+        <v>0.01</v>
+      </c>
+      <c r="Z16" s="10">
+        <v>1E-3</v>
+      </c>
+      <c r="AA16" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="AB16" s="10">
+        <v>0</v>
+      </c>
+      <c r="AC16" s="10">
+        <v>1</v>
+      </c>
+      <c r="AD16" s="10">
+        <v>2</v>
+      </c>
+      <c r="AE16" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="AF16" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="AH16" s="10">
+        <v>0.05</v>
+      </c>
+      <c r="AI16" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="AJ16" s="10">
+        <v>0</v>
+      </c>
+      <c r="AK16" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="AL16" s="10">
+        <v>0.03</v>
+      </c>
+      <c r="AM16" s="10">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AN16" s="10">
+        <v>0.04</v>
+      </c>
+      <c r="AO16" s="10">
+        <v>0.11</v>
+      </c>
+      <c r="AP16" s="10">
+        <v>1</v>
+      </c>
+      <c r="AQ16" s="10">
+        <v>0.03</v>
+      </c>
+      <c r="AR16" s="10">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AS16" s="10">
+        <v>0.7</v>
+      </c>
+      <c r="AT16" s="10">
+        <v>1</v>
+      </c>
+      <c r="AU16" s="10">
+        <v>15</v>
+      </c>
+      <c r="AV16" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="AW16" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="AX16" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="AY16" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="AZ16" s="10">
+        <v>5</v>
+      </c>
+      <c r="BA16" s="10">
+        <v>8.2199999999999995E-2</v>
+      </c>
+      <c r="BB16" s="10">
+        <v>0.12</v>
+      </c>
+      <c r="BC16" s="10">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="BD16" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="BE16" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="BF16" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="BG16" s="10">
+        <v>0.01</v>
+      </c>
+      <c r="BH16" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="BI16" s="10">
+        <v>0.75</v>
+      </c>
+      <c r="BJ16" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="BK16" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
     <row r="17" spans="1:63" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="B17" s="10" t="b">
         <v>0</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D17" s="10">
         <v>1</v>
@@ -3074,9 +3297,6 @@
       <c r="G17" s="10">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="H17" s="10" t="s">
-        <v>77</v>
-      </c>
       <c r="N17" s="10" t="s">
         <v>135</v>
       </c>
@@ -3086,6 +3306,9 @@
       <c r="Q17" s="10">
         <v>0</v>
       </c>
+      <c r="R17" s="10">
+        <v>1</v>
+      </c>
       <c r="S17" s="10">
         <v>0.02</v>
       </c>
@@ -3146,6 +3369,9 @@
       <c r="AO17" s="10">
         <v>0.11</v>
       </c>
+      <c r="AP17" s="10">
+        <v>1</v>
+      </c>
       <c r="AQ17" s="10">
         <v>0.03</v>
       </c>
@@ -3201,7 +3427,7 @@
         <v>23</v>
       </c>
       <c r="BI17" s="10">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="BJ17" s="10" t="b">
         <v>1</v>
@@ -3210,173 +3436,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:63" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="B18" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="D18" s="10">
-        <v>1</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="F18" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="G18" s="10">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="H18" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="N18" s="10" t="s">
-        <v>135</v>
-      </c>
-      <c r="P18" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="Q18" s="10">
-        <v>0</v>
-      </c>
-      <c r="S18" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="T18" s="10">
-        <v>0</v>
-      </c>
-      <c r="U18" s="10">
-        <v>0.9</v>
-      </c>
-      <c r="V18" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="W18" s="10">
-        <v>0</v>
-      </c>
-      <c r="X18" s="10">
-        <v>0.9</v>
-      </c>
-      <c r="Y18" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="Z18" s="10">
-        <v>1E-3</v>
-      </c>
-      <c r="AA18" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="AB18" s="10">
-        <v>0</v>
-      </c>
-      <c r="AC18" s="10">
-        <v>1</v>
-      </c>
-      <c r="AD18" s="10">
-        <v>1</v>
-      </c>
-      <c r="AH18" s="10">
-        <v>0.05</v>
-      </c>
-      <c r="AI18" s="10">
-        <v>0.5</v>
-      </c>
-      <c r="AJ18" s="10">
-        <v>0.05</v>
-      </c>
-      <c r="AK18" s="10">
-        <v>0.5</v>
-      </c>
-      <c r="AL18" s="10">
-        <v>0.03</v>
-      </c>
-      <c r="AM18" s="10">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="AN18" s="10">
-        <v>0.04</v>
-      </c>
-      <c r="AO18" s="10">
-        <v>0.11</v>
-      </c>
-      <c r="AQ18" s="10">
-        <v>0.03</v>
-      </c>
-      <c r="AR18" s="10">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="AS18" s="10">
-        <v>0.7</v>
-      </c>
-      <c r="AT18" s="10">
-        <v>1</v>
-      </c>
-      <c r="AU18" s="10">
-        <v>15</v>
-      </c>
-      <c r="AV18" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="AW18" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="AX18" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="AY18" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="AZ18" s="10">
-        <v>5</v>
-      </c>
-      <c r="BA18" s="10">
-        <v>8.2199999999999995E-2</v>
-      </c>
-      <c r="BB18" s="10">
-        <v>0.12</v>
-      </c>
-      <c r="BC18" s="10">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="BD18" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="BE18" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="BF18" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="BG18" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="BH18" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="BI18" s="10">
-        <v>1</v>
-      </c>
-      <c r="BJ18" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="BK18" s="10" t="b">
-        <v>1</v>
-      </c>
-    </row>
+    <row r="18" spans="1:63" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="19" spans="1:63" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B19" s="10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="D19" s="10">
         <v>1</v>
@@ -3385,7 +3454,7 @@
         <v>50</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>88</v>
+        <v>63</v>
       </c>
       <c r="G19" s="10">
         <v>1.4999999999999999E-2</v>
@@ -3534,10 +3603,10 @@
     </row>
     <row r="20" spans="1:63" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
       <c r="B20" s="10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C20" s="10" t="s">
         <v>110</v>
@@ -3549,7 +3618,7 @@
         <v>50</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G20" s="10">
         <v>1.4999999999999999E-2</v>
@@ -3567,7 +3636,7 @@
         <v>0</v>
       </c>
       <c r="R20" s="10">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="S20" s="10">
         <v>0.02</v>
@@ -3612,7 +3681,7 @@
         <v>0.5</v>
       </c>
       <c r="AJ20" s="10">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="AK20" s="10">
         <v>0.5</v>
@@ -3630,7 +3699,7 @@
         <v>0.11</v>
       </c>
       <c r="AP20" s="10">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="AQ20" s="10">
         <v>0.03</v>
@@ -3698,7 +3767,7 @@
     </row>
     <row r="21" spans="1:63" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B21" s="10" t="b">
         <v>0</v>
@@ -3713,7 +3782,7 @@
         <v>50</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G21" s="10">
         <v>1.4999999999999999E-2</v>
@@ -3730,6 +3799,9 @@
       <c r="Q21" s="10">
         <v>0</v>
       </c>
+      <c r="R21" s="10">
+        <v>1</v>
+      </c>
       <c r="S21" s="10">
         <v>0.02</v>
       </c>
@@ -3789,6 +3861,9 @@
       </c>
       <c r="AO21" s="10">
         <v>0.11</v>
+      </c>
+      <c r="AP21" s="10">
+        <v>1</v>
       </c>
       <c r="AQ21" s="10">
         <v>0.03</v>
@@ -3856,22 +3931,22 @@
     </row>
     <row r="22" spans="1:63" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
-        <v>124</v>
+        <v>136</v>
       </c>
       <c r="B22" s="10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D22" s="10">
         <v>1</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>63</v>
+        <v>88</v>
       </c>
       <c r="G22" s="10">
         <v>1.4999999999999999E-2</v>
@@ -3888,8 +3963,8 @@
       <c r="Q22" s="10">
         <v>0</v>
       </c>
-      <c r="R22" s="10">
-        <v>1</v>
+      <c r="R22" s="14">
+        <v>5</v>
       </c>
       <c r="S22" s="10">
         <v>0.02</v>
@@ -3952,7 +4027,7 @@
         <v>0.11</v>
       </c>
       <c r="AP22" s="10">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="AQ22" s="10">
         <v>0.03</v>
@@ -4020,22 +4095,22 @@
     </row>
     <row r="23" spans="1:63" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B23" s="10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D23" s="10">
         <v>1</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>63</v>
+        <v>89</v>
       </c>
       <c r="G23" s="10">
         <v>1.4999999999999999E-2</v>
@@ -4053,7 +4128,7 @@
         <v>0</v>
       </c>
       <c r="R23" s="10">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="S23" s="10">
         <v>0.02</v>
@@ -4116,7 +4191,7 @@
         <v>0.11</v>
       </c>
       <c r="AP23" s="10">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="AQ23" s="10">
         <v>0.03</v>
@@ -4182,9 +4257,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:63" s="10" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:63" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B24" s="10" t="b">
         <v>0</v>
@@ -4196,7 +4271,7 @@
         <v>1</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F24" s="10" t="s">
         <v>63</v>
@@ -4216,6 +4291,9 @@
       <c r="Q24" s="10">
         <v>0</v>
       </c>
+      <c r="R24" s="10">
+        <v>1</v>
+      </c>
       <c r="S24" s="10">
         <v>0.02</v>
       </c>
@@ -4275,6 +4353,9 @@
       </c>
       <c r="AO24" s="10">
         <v>0.11</v>
+      </c>
+      <c r="AP24" s="10">
+        <v>1</v>
       </c>
       <c r="AQ24" s="10">
         <v>0.03</v>
@@ -4342,7 +4423,7 @@
     </row>
     <row r="25" spans="1:63" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="B25" s="10" t="b">
         <v>0</v>
@@ -4354,7 +4435,7 @@
         <v>1</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F25" s="10" t="s">
         <v>63</v>
@@ -4374,6 +4455,9 @@
       <c r="Q25" s="10">
         <v>0</v>
       </c>
+      <c r="R25" s="14">
+        <v>5</v>
+      </c>
       <c r="S25" s="10">
         <v>0.02</v>
       </c>
@@ -4433,6 +4517,9 @@
       </c>
       <c r="AO25" s="10">
         <v>0.11</v>
+      </c>
+      <c r="AP25" s="10">
+        <v>5</v>
       </c>
       <c r="AQ25" s="10">
         <v>0.03</v>
@@ -4500,7 +4587,7 @@
     </row>
     <row r="26" spans="1:63" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
-        <v>127</v>
+        <v>140</v>
       </c>
       <c r="B26" s="10" t="b">
         <v>0</v>
@@ -4512,7 +4599,7 @@
         <v>1</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="F26" s="10" t="s">
         <v>63</v>
@@ -4527,10 +4614,13 @@
         <v>135</v>
       </c>
       <c r="P26" s="10">
-        <v>0.02</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="Q26" s="10">
-        <v>0</v>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="R26" s="14">
+        <v>5</v>
       </c>
       <c r="S26" s="10">
         <v>0.02</v>
@@ -4566,13 +4656,7 @@
         <v>1</v>
       </c>
       <c r="AD26" s="10">
-        <v>2</v>
-      </c>
-      <c r="AE26" s="10">
-        <v>0.5</v>
-      </c>
-      <c r="AF26" s="10">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="AH26" s="10">
         <v>0.05</v>
@@ -4598,6 +4682,9 @@
       <c r="AO26" s="10">
         <v>0.11</v>
       </c>
+      <c r="AP26" s="10">
+        <v>5</v>
+      </c>
       <c r="AQ26" s="10">
         <v>0.03</v>
       </c>
@@ -4662,21 +4749,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:63" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:63" s="10" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B27" s="10" t="b">
         <v>0</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D27" s="10">
         <v>1</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F27" s="10" t="s">
         <v>63</v>
@@ -4684,6 +4771,9 @@
       <c r="G27" s="10">
         <v>1.4999999999999999E-2</v>
       </c>
+      <c r="H27" s="10" t="s">
+        <v>77</v>
+      </c>
       <c r="N27" s="10" t="s">
         <v>135</v>
       </c>
@@ -4693,6 +4783,9 @@
       <c r="Q27" s="10">
         <v>0</v>
       </c>
+      <c r="R27" s="10">
+        <v>1</v>
+      </c>
       <c r="S27" s="10">
         <v>0.02</v>
       </c>
@@ -4753,6 +4846,9 @@
       <c r="AO27" s="10">
         <v>0.11</v>
       </c>
+      <c r="AP27" s="10">
+        <v>1</v>
+      </c>
       <c r="AQ27" s="10">
         <v>0.03</v>
       </c>
@@ -4817,540 +4913,1199 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:63" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:63" s="10" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="B28" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="D28" s="10">
+        <v>1</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="F28" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="G28" s="10">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="H28" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="N28" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="P28" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="Q28" s="10">
+        <v>0</v>
+      </c>
+      <c r="R28" s="10">
+        <v>1</v>
+      </c>
+      <c r="S28" s="10">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="T28" s="10">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="U28" s="10">
+        <v>1</v>
+      </c>
+      <c r="V28" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="W28" s="10">
+        <v>0</v>
+      </c>
+      <c r="X28" s="10">
+        <v>0.9</v>
+      </c>
+      <c r="Y28" s="10">
+        <v>0.01</v>
+      </c>
+      <c r="Z28" s="10">
+        <v>1E-3</v>
+      </c>
+      <c r="AA28" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="AB28" s="10">
+        <v>0</v>
+      </c>
+      <c r="AC28" s="10">
+        <v>1</v>
+      </c>
+      <c r="AD28" s="10">
+        <v>1</v>
+      </c>
+      <c r="AH28" s="10">
+        <v>0.05</v>
+      </c>
+      <c r="AI28" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="AJ28" s="10">
+        <v>0</v>
+      </c>
+      <c r="AK28" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="AL28" s="10">
+        <v>0.03</v>
+      </c>
+      <c r="AM28" s="10">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AN28" s="10">
+        <v>0.04</v>
+      </c>
+      <c r="AO28" s="10">
+        <v>0.11</v>
+      </c>
+      <c r="AP28" s="10">
+        <v>1</v>
+      </c>
+      <c r="AQ28" s="10">
+        <v>0.03</v>
+      </c>
+      <c r="AR28" s="10">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AS28" s="10">
+        <v>0.7</v>
+      </c>
+      <c r="AT28" s="10">
+        <v>1</v>
+      </c>
+      <c r="AU28" s="10">
+        <v>15</v>
+      </c>
+      <c r="AV28" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="AW28" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="AX28" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="AY28" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="AZ28" s="10">
+        <v>5</v>
+      </c>
+      <c r="BA28" s="10">
+        <v>8.2199999999999995E-2</v>
+      </c>
+      <c r="BB28" s="10">
+        <v>0.12</v>
+      </c>
+      <c r="BC28" s="10">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="BD28" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="BE28" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="BF28" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="BG28" s="10">
+        <v>0.01</v>
+      </c>
+      <c r="BH28" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="BI28" s="10">
+        <v>1</v>
+      </c>
+      <c r="BJ28" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="BK28" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:63" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="B29" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="D29" s="10">
+        <v>1</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="F29" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="G29" s="10">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="H29" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="N29" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="P29" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="Q29" s="10">
+        <v>0</v>
+      </c>
+      <c r="R29" s="10">
+        <v>1</v>
+      </c>
+      <c r="S29" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="T29" s="10">
+        <v>0</v>
+      </c>
+      <c r="U29" s="10">
+        <v>0.9</v>
+      </c>
+      <c r="V29" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="W29" s="10">
+        <v>0</v>
+      </c>
+      <c r="X29" s="10">
+        <v>0.9</v>
+      </c>
+      <c r="Y29" s="10">
+        <v>0.01</v>
+      </c>
+      <c r="Z29" s="10">
+        <v>1E-3</v>
+      </c>
+      <c r="AA29" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="AB29" s="10">
+        <v>0</v>
+      </c>
+      <c r="AC29" s="10">
+        <v>1</v>
+      </c>
+      <c r="AD29" s="10">
+        <v>1</v>
+      </c>
+      <c r="AH29" s="10">
+        <v>0.05</v>
+      </c>
+      <c r="AI29" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="AJ29" s="10">
+        <v>0</v>
+      </c>
+      <c r="AK29" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="AL29" s="10">
+        <v>0.03</v>
+      </c>
+      <c r="AM29" s="10">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AN29" s="10">
+        <v>0.04</v>
+      </c>
+      <c r="AO29" s="10">
+        <v>0.11</v>
+      </c>
+      <c r="AP29" s="10">
+        <v>1</v>
+      </c>
+      <c r="AQ29" s="10">
+        <v>0.03</v>
+      </c>
+      <c r="AR29" s="10">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AS29" s="10">
+        <v>0.7</v>
+      </c>
+      <c r="AT29" s="10">
+        <v>1</v>
+      </c>
+      <c r="AU29" s="10">
+        <v>15</v>
+      </c>
+      <c r="AV29" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="AW29" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="AX29" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="AY29" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="AZ29" s="10">
+        <v>5</v>
+      </c>
+      <c r="BA29" s="10">
+        <v>8.2199999999999995E-2</v>
+      </c>
+      <c r="BB29" s="10">
+        <v>0.12</v>
+      </c>
+      <c r="BC29" s="10">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="BD29" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="BE29" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="BF29" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="BG29" s="10">
+        <v>0.01</v>
+      </c>
+      <c r="BH29" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="BI29" s="10">
+        <v>1</v>
+      </c>
+      <c r="BJ29" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="BK29" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
     <row r="30" spans="1:63" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
-        <v>109</v>
+        <v>127</v>
       </c>
       <c r="B30" s="10" t="b">
         <v>0</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>112</v>
+        <v>111</v>
+      </c>
+      <c r="D30" s="10">
+        <v>1</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="F30" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="G30" s="10">
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="H30" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="I30" s="10">
-        <v>1</v>
-      </c>
-      <c r="J30" s="10">
-        <v>1</v>
-      </c>
-      <c r="K30" s="10">
-        <v>1</v>
-      </c>
-      <c r="L30" s="10">
+      <c r="N30" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="P30" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="Q30" s="10">
+        <v>0</v>
+      </c>
+      <c r="R30" s="10">
+        <v>1</v>
+      </c>
+      <c r="S30" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="T30" s="10">
+        <v>0</v>
+      </c>
+      <c r="U30" s="10">
+        <v>0.9</v>
+      </c>
+      <c r="V30" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="W30" s="10">
+        <v>0</v>
+      </c>
+      <c r="X30" s="10">
+        <v>0.9</v>
+      </c>
+      <c r="Y30" s="10">
+        <v>0.01</v>
+      </c>
+      <c r="Z30" s="10">
+        <v>1E-3</v>
+      </c>
+      <c r="AA30" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="AB30" s="10">
+        <v>0</v>
+      </c>
+      <c r="AC30" s="10">
+        <v>1</v>
+      </c>
+      <c r="AD30" s="10">
+        <v>2</v>
+      </c>
+      <c r="AE30" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="AF30" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="AH30" s="10">
+        <v>0.05</v>
+      </c>
+      <c r="AI30" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="AJ30" s="10">
+        <v>0</v>
+      </c>
+      <c r="AK30" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="AL30" s="10">
         <v>0.03</v>
       </c>
-      <c r="M30" s="10">
+      <c r="AM30" s="10">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AN30" s="10">
+        <v>0.04</v>
+      </c>
+      <c r="AO30" s="10">
+        <v>0.11</v>
+      </c>
+      <c r="AP30" s="10">
+        <v>1</v>
+      </c>
+      <c r="AQ30" s="10">
         <v>0.03</v>
+      </c>
+      <c r="AR30" s="10">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AS30" s="10">
+        <v>0.7</v>
+      </c>
+      <c r="AT30" s="10">
+        <v>1</v>
+      </c>
+      <c r="AU30" s="10">
+        <v>15</v>
+      </c>
+      <c r="AV30" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="AW30" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="AX30" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="AY30" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="AZ30" s="10">
+        <v>5</v>
+      </c>
+      <c r="BA30" s="10">
+        <v>8.2199999999999995E-2</v>
+      </c>
+      <c r="BB30" s="10">
+        <v>0.12</v>
+      </c>
+      <c r="BC30" s="10">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="BD30" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="BE30" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="BF30" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="BG30" s="10">
+        <v>0.01</v>
+      </c>
+      <c r="BH30" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="BI30" s="10">
+        <v>1</v>
+      </c>
+      <c r="BJ30" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="BK30" s="10" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:63" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="H31" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="I31" s="10">
-        <v>1</v>
-      </c>
-      <c r="J31" s="10">
-        <v>1</v>
-      </c>
-      <c r="K31" s="10">
-        <v>1</v>
-      </c>
-      <c r="L31" s="10">
-        <v>0.06</v>
-      </c>
-      <c r="M31" s="10">
-        <v>0.06</v>
+        <v>128</v>
+      </c>
+      <c r="B31" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="D31" s="10">
+        <v>1</v>
+      </c>
+      <c r="E31" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="F31" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="G31" s="10">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="N31" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="P31" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="Q31" s="10">
+        <v>0</v>
+      </c>
+      <c r="R31" s="10">
+        <v>1</v>
+      </c>
+      <c r="S31" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="T31" s="10">
+        <v>0</v>
+      </c>
+      <c r="U31" s="10">
+        <v>0.9</v>
+      </c>
+      <c r="V31" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="W31" s="10">
+        <v>0</v>
+      </c>
+      <c r="X31" s="10">
+        <v>0.9</v>
+      </c>
+      <c r="Y31" s="10">
+        <v>0.01</v>
+      </c>
+      <c r="Z31" s="10">
+        <v>1E-3</v>
+      </c>
+      <c r="AA31" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="AB31" s="10">
+        <v>0</v>
+      </c>
+      <c r="AC31" s="10">
+        <v>1</v>
+      </c>
+      <c r="AD31" s="10">
+        <v>1</v>
+      </c>
+      <c r="AH31" s="10">
+        <v>0.05</v>
+      </c>
+      <c r="AI31" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="AJ31" s="10">
+        <v>0</v>
+      </c>
+      <c r="AK31" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="AL31" s="10">
+        <v>0.03</v>
+      </c>
+      <c r="AM31" s="10">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AN31" s="10">
+        <v>0.04</v>
+      </c>
+      <c r="AO31" s="10">
+        <v>0.11</v>
+      </c>
+      <c r="AP31" s="10">
+        <v>1</v>
+      </c>
+      <c r="AQ31" s="10">
+        <v>0.03</v>
+      </c>
+      <c r="AR31" s="10">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AS31" s="10">
+        <v>0.7</v>
+      </c>
+      <c r="AT31" s="10">
+        <v>1</v>
+      </c>
+      <c r="AU31" s="10">
+        <v>15</v>
+      </c>
+      <c r="AV31" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="AW31" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="AX31" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="AY31" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="AZ31" s="10">
+        <v>5</v>
+      </c>
+      <c r="BA31" s="10">
+        <v>8.2199999999999995E-2</v>
+      </c>
+      <c r="BB31" s="10">
+        <v>0.12</v>
+      </c>
+      <c r="BC31" s="10">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="BD31" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="BE31" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="BF31" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="BG31" s="10">
+        <v>0.01</v>
+      </c>
+      <c r="BH31" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="BI31" s="10">
+        <v>1</v>
+      </c>
+      <c r="BJ31" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="BK31" s="10" t="b">
+        <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:63" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="B32" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="C32" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="D32" s="10">
-        <v>1</v>
-      </c>
-      <c r="E32" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="F32" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="G32" s="10">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="H32" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="P32" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="Q32" s="10">
-        <v>0</v>
-      </c>
-      <c r="S32" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="T32" s="10">
-        <v>0</v>
-      </c>
-      <c r="U32" s="10">
-        <v>0.9</v>
-      </c>
-      <c r="V32" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="W32" s="10">
-        <v>0</v>
-      </c>
-      <c r="X32" s="10">
-        <v>0.9</v>
-      </c>
-      <c r="Y32" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="Z32" s="10">
-        <v>1E-3</v>
-      </c>
-      <c r="AA32" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="AB32" s="10">
-        <v>0</v>
-      </c>
-      <c r="AC32" s="10">
-        <v>1</v>
-      </c>
-      <c r="AD32" s="10">
-        <v>1</v>
-      </c>
-      <c r="AH32" s="10">
-        <v>0.05</v>
-      </c>
-      <c r="AI32" s="10">
-        <v>0.5</v>
-      </c>
-      <c r="AJ32" s="10">
-        <v>0</v>
-      </c>
-      <c r="AK32" s="10">
-        <v>0.5</v>
-      </c>
-      <c r="AL32" s="10">
-        <v>0.03</v>
-      </c>
-      <c r="AM32" s="10">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="AN32" s="10">
-        <v>0.04</v>
-      </c>
-      <c r="AO32" s="10">
-        <v>0.11</v>
-      </c>
-      <c r="AQ32" s="10">
-        <v>0.03</v>
-      </c>
-      <c r="AR32" s="10">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="AS32" s="10">
-        <v>0.7</v>
-      </c>
-      <c r="AT32" s="10">
-        <v>1</v>
-      </c>
-      <c r="AU32" s="10">
-        <v>15</v>
-      </c>
-      <c r="AV32" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="AW32" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="AX32" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="AY32" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="AZ32" s="10">
-        <v>5</v>
-      </c>
-      <c r="BA32" s="10">
-        <v>8.2199999999999995E-2</v>
-      </c>
-      <c r="BB32" s="10">
-        <v>0.12</v>
-      </c>
-      <c r="BC32" s="10">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="BD32" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="BE32" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="BF32" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="BG32" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="BH32" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="BI32" s="10">
-        <v>0.75</v>
-      </c>
-      <c r="BJ32" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="BK32" s="10" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:63" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:63" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="34" spans="1:63" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="B34" s="10" t="b">
         <v>0</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="D34" s="10">
-        <v>1</v>
-      </c>
-      <c r="E34" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="F34" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="G34" s="10">
-        <v>1.4999999999999999E-2</v>
+        <v>112</v>
       </c>
       <c r="H34" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="P34" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="Q34" s="10">
-        <v>0</v>
-      </c>
-      <c r="S34" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="T34" s="10">
-        <v>0</v>
-      </c>
-      <c r="U34" s="10">
-        <v>0.9</v>
-      </c>
-      <c r="V34" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="W34" s="10">
-        <v>0</v>
-      </c>
-      <c r="X34" s="10">
-        <v>0.9</v>
-      </c>
-      <c r="Y34" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="Z34" s="10">
-        <v>1E-3</v>
-      </c>
-      <c r="AA34" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="AB34" s="10">
-        <v>0</v>
-      </c>
-      <c r="AC34" s="10">
-        <v>1</v>
-      </c>
-      <c r="AD34" s="10">
-        <v>1</v>
-      </c>
-      <c r="AH34" s="10">
-        <v>0.05</v>
-      </c>
-      <c r="AI34" s="10">
-        <v>0.5</v>
-      </c>
-      <c r="AJ34" s="10">
-        <v>0</v>
-      </c>
-      <c r="AK34" s="10">
-        <v>0.5</v>
-      </c>
-      <c r="AL34" s="10">
+      <c r="I34" s="10">
+        <v>1</v>
+      </c>
+      <c r="J34" s="10">
+        <v>1</v>
+      </c>
+      <c r="K34" s="10">
+        <v>1</v>
+      </c>
+      <c r="L34" s="10">
         <v>0.03</v>
       </c>
-      <c r="AM34" s="10">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="AN34" s="10">
-        <v>0.04</v>
-      </c>
-      <c r="AO34" s="10">
-        <v>0.11</v>
-      </c>
-      <c r="AP34" s="10">
-        <v>5</v>
-      </c>
-      <c r="AQ34" s="10">
+      <c r="M34" s="10">
         <v>0.03</v>
-      </c>
-      <c r="AR34" s="10">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="AS34" s="10">
-        <v>0.7</v>
-      </c>
-      <c r="AT34" s="10">
-        <v>1</v>
-      </c>
-      <c r="AU34" s="10">
-        <v>15</v>
-      </c>
-      <c r="AV34" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="AW34" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="AX34" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="AY34" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="AZ34" s="10">
-        <v>5</v>
-      </c>
-      <c r="BA34" s="10">
-        <v>8.2199999999999995E-2</v>
-      </c>
-      <c r="BB34" s="10">
-        <v>0.12</v>
-      </c>
-      <c r="BC34" s="10">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="BD34" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="BE34" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="BF34" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="BG34" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="BH34" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="BI34" s="10">
-        <v>0.75</v>
-      </c>
-      <c r="BJ34" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="BK34" s="10" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:63" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="B35" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="C35" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="D35" s="10">
-        <v>1</v>
-      </c>
-      <c r="E35" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="F35" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="G35" s="10">
-        <v>1.4999999999999999E-2</v>
+        <v>107</v>
       </c>
       <c r="H35" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="P35" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="Q35" s="10">
-        <v>0</v>
-      </c>
-      <c r="S35" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="T35" s="10">
-        <v>0</v>
-      </c>
-      <c r="U35" s="10">
+      <c r="I35" s="10">
+        <v>1</v>
+      </c>
+      <c r="J35" s="10">
+        <v>1</v>
+      </c>
+      <c r="K35" s="10">
+        <v>1</v>
+      </c>
+      <c r="L35" s="10">
+        <v>0.06</v>
+      </c>
+      <c r="M35" s="10">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="36" spans="1:63" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="B36" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="D36" s="10">
+        <v>1</v>
+      </c>
+      <c r="E36" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="F36" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G36" s="10">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="H36" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="P36" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="Q36" s="10">
+        <v>0</v>
+      </c>
+      <c r="S36" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="T36" s="10">
+        <v>0</v>
+      </c>
+      <c r="U36" s="10">
         <v>0.9</v>
       </c>
-      <c r="V35" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="W35" s="10">
-        <v>0</v>
-      </c>
-      <c r="X35" s="10">
+      <c r="V36" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="W36" s="10">
+        <v>0</v>
+      </c>
+      <c r="X36" s="10">
         <v>0.9</v>
       </c>
-      <c r="Y35" s="10">
+      <c r="Y36" s="10">
         <v>0.01</v>
       </c>
-      <c r="Z35" s="10">
+      <c r="Z36" s="10">
         <v>1E-3</v>
       </c>
-      <c r="AA35" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="AB35" s="10">
-        <v>0</v>
-      </c>
-      <c r="AC35" s="10">
-        <v>1</v>
-      </c>
-      <c r="AD35" s="10">
-        <v>1</v>
-      </c>
-      <c r="AH35" s="10">
+      <c r="AA36" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="AB36" s="10">
+        <v>0</v>
+      </c>
+      <c r="AC36" s="10">
+        <v>1</v>
+      </c>
+      <c r="AD36" s="10">
+        <v>1</v>
+      </c>
+      <c r="AH36" s="10">
         <v>0.05</v>
       </c>
-      <c r="AI35" s="10">
-        <v>0.5</v>
-      </c>
-      <c r="AJ35" s="10">
-        <v>0</v>
-      </c>
-      <c r="AK35" s="10">
-        <v>0.5</v>
-      </c>
-      <c r="AL35" s="10">
+      <c r="AI36" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="AJ36" s="10">
+        <v>0</v>
+      </c>
+      <c r="AK36" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="AL36" s="10">
         <v>0.03</v>
       </c>
-      <c r="AM35" s="10">
+      <c r="AM36" s="10">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AN35" s="10">
+      <c r="AN36" s="10">
         <v>0.04</v>
       </c>
-      <c r="AO35" s="10">
+      <c r="AO36" s="10">
         <v>0.11</v>
       </c>
-      <c r="AP35" s="10">
+      <c r="AQ36" s="10">
+        <v>0.03</v>
+      </c>
+      <c r="AR36" s="10">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AS36" s="10">
+        <v>0.7</v>
+      </c>
+      <c r="AT36" s="10">
+        <v>1</v>
+      </c>
+      <c r="AU36" s="10">
+        <v>15</v>
+      </c>
+      <c r="AV36" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="AW36" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="AX36" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="AY36" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="AZ36" s="10">
         <v>5</v>
       </c>
-      <c r="AQ35" s="10">
+      <c r="BA36" s="10">
+        <v>8.2199999999999995E-2</v>
+      </c>
+      <c r="BB36" s="10">
+        <v>0.12</v>
+      </c>
+      <c r="BC36" s="10">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="BD36" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="BE36" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="BF36" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="BG36" s="10">
+        <v>0.01</v>
+      </c>
+      <c r="BH36" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="BI36" s="10">
+        <v>0.75</v>
+      </c>
+      <c r="BJ36" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="BK36" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:63" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="1:63" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="B38" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="D38" s="10">
+        <v>1</v>
+      </c>
+      <c r="E38" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="F38" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="G38" s="10">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="H38" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="P38" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="Q38" s="10">
+        <v>0</v>
+      </c>
+      <c r="S38" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="T38" s="10">
+        <v>0</v>
+      </c>
+      <c r="U38" s="10">
+        <v>0.9</v>
+      </c>
+      <c r="V38" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="W38" s="10">
+        <v>0</v>
+      </c>
+      <c r="X38" s="10">
+        <v>0.9</v>
+      </c>
+      <c r="Y38" s="10">
+        <v>0.01</v>
+      </c>
+      <c r="Z38" s="10">
+        <v>1E-3</v>
+      </c>
+      <c r="AA38" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="AB38" s="10">
+        <v>0</v>
+      </c>
+      <c r="AC38" s="10">
+        <v>1</v>
+      </c>
+      <c r="AD38" s="10">
+        <v>1</v>
+      </c>
+      <c r="AH38" s="10">
+        <v>0.05</v>
+      </c>
+      <c r="AI38" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="AJ38" s="10">
+        <v>0</v>
+      </c>
+      <c r="AK38" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="AL38" s="10">
         <v>0.03</v>
       </c>
-      <c r="AR35" s="10">
+      <c r="AM38" s="10">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AS35" s="10">
+      <c r="AN38" s="10">
+        <v>0.04</v>
+      </c>
+      <c r="AO38" s="10">
+        <v>0.11</v>
+      </c>
+      <c r="AP38" s="10">
+        <v>5</v>
+      </c>
+      <c r="AQ38" s="10">
+        <v>0.03</v>
+      </c>
+      <c r="AR38" s="10">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AS38" s="10">
         <v>0.7</v>
       </c>
-      <c r="AT35" s="10">
-        <v>1</v>
-      </c>
-      <c r="AU35" s="10">
+      <c r="AT38" s="10">
+        <v>1</v>
+      </c>
+      <c r="AU38" s="10">
         <v>15</v>
       </c>
-      <c r="AV35" s="10" t="s">
+      <c r="AV38" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="AW35" s="10" t="s">
+      <c r="AW38" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="AX35" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="AY35" s="10" t="s">
+      <c r="AX38" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="AY38" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="AZ35" s="10">
+      <c r="AZ38" s="10">
         <v>5</v>
       </c>
-      <c r="BA35" s="10">
+      <c r="BA38" s="10">
         <v>8.2199999999999995E-2</v>
       </c>
-      <c r="BB35" s="10">
+      <c r="BB38" s="10">
         <v>0.12</v>
       </c>
-      <c r="BC35" s="10">
+      <c r="BC38" s="10">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="BD35" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="BE35" s="10" t="s">
+      <c r="BD38" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="BE38" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="BF35" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="BG35" s="10">
+      <c r="BF38" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="BG38" s="10">
         <v>0.01</v>
       </c>
-      <c r="BH35" s="10" t="s">
+      <c r="BH38" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="BI35" s="10">
-        <v>1</v>
-      </c>
-      <c r="BJ35" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="BK35" s="10" t="b">
+      <c r="BI38" s="10">
+        <v>0.75</v>
+      </c>
+      <c r="BJ38" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="BK38" s="10" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:63" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" spans="1:63" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" spans="1:63" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="1:63" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="B39" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="C39" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="D39" s="10">
+        <v>1</v>
+      </c>
+      <c r="E39" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="F39" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="G39" s="10">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="H39" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="P39" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="Q39" s="10">
+        <v>0</v>
+      </c>
+      <c r="S39" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="T39" s="10">
+        <v>0</v>
+      </c>
+      <c r="U39" s="10">
+        <v>0.9</v>
+      </c>
+      <c r="V39" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="W39" s="10">
+        <v>0</v>
+      </c>
+      <c r="X39" s="10">
+        <v>0.9</v>
+      </c>
+      <c r="Y39" s="10">
+        <v>0.01</v>
+      </c>
+      <c r="Z39" s="10">
+        <v>1E-3</v>
+      </c>
+      <c r="AA39" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="AB39" s="10">
+        <v>0</v>
+      </c>
+      <c r="AC39" s="10">
+        <v>1</v>
+      </c>
+      <c r="AD39" s="10">
+        <v>1</v>
+      </c>
+      <c r="AH39" s="10">
+        <v>0.05</v>
+      </c>
+      <c r="AI39" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="AJ39" s="10">
+        <v>0</v>
+      </c>
+      <c r="AK39" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="AL39" s="10">
+        <v>0.03</v>
+      </c>
+      <c r="AM39" s="10">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AN39" s="10">
+        <v>0.04</v>
+      </c>
+      <c r="AO39" s="10">
+        <v>0.11</v>
+      </c>
+      <c r="AP39" s="10">
+        <v>5</v>
+      </c>
+      <c r="AQ39" s="10">
+        <v>0.03</v>
+      </c>
+      <c r="AR39" s="10">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AS39" s="10">
+        <v>0.7</v>
+      </c>
+      <c r="AT39" s="10">
+        <v>1</v>
+      </c>
+      <c r="AU39" s="10">
+        <v>15</v>
+      </c>
+      <c r="AV39" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="AW39" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="AX39" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="AY39" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="AZ39" s="10">
+        <v>5</v>
+      </c>
+      <c r="BA39" s="10">
+        <v>8.2199999999999995E-2</v>
+      </c>
+      <c r="BB39" s="10">
+        <v>0.12</v>
+      </c>
+      <c r="BC39" s="10">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="BD39" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="BE39" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="BF39" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="BG39" s="10">
+        <v>0.01</v>
+      </c>
+      <c r="BH39" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="BI39" s="10">
+        <v>1</v>
+      </c>
+      <c r="BJ39" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="BK39" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:63" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="1:63" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="1:63" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B30:B38 B3:B28" xr:uid="{05E01AB2-72EC-4550-ACB8-4E83765DE296}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B34:B42 B3:B32" xr:uid="{05E01AB2-72EC-4550-ACB8-4E83765DE296}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H30:H32 H34:H35 H3:H14 H17:H26" xr:uid="{8DBFC5CB-438A-4309-B948-24597CAE3D7F}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H34:H36 H38:H39 H3:H16 H19:H30" xr:uid="{8DBFC5CB-438A-4309-B948-24597CAE3D7F}">
       <formula1>"preSet, ALpct,MApct"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5363,7 +6118,7 @@
           <x14:formula1>
             <xm:f>Policies!$B$3:$B$9</xm:f>
           </x14:formula1>
-          <xm:sqref>F32 F30 F34:F35 F3:F28</xm:sqref>
+          <xm:sqref>F36 F34 F38:F39 F3:F32</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -5377,7 +6132,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
start explore DA plans
</commit_message>
<xml_diff>
--- a/RunControl.xlsx
+++ b/RunControl.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B03F6BE-0B63-4DF3-834A-E6A76C0DB2F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98F958E7-B6CF-4B85-907C-46EBE87B7C01}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="-7590" windowWidth="16440" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="paramlist" sheetId="1" r:id="rId1"/>
@@ -845,10 +845,10 @@
   <dimension ref="A1:BL44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="2" topLeftCell="M3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B60" sqref="B60"/>
+      <selection pane="bottomRight" activeCell="B5" sqref="B5:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1328,7 +1328,7 @@
         <v>112</v>
       </c>
       <c r="B5" s="10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>112</v>
@@ -1492,7 +1492,7 @@
         <v>115</v>
       </c>
       <c r="B6" s="10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>109</v>
@@ -1656,7 +1656,7 @@
         <v>87</v>
       </c>
       <c r="B7" s="10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>109</v>
@@ -1820,7 +1820,7 @@
         <v>130</v>
       </c>
       <c r="B8" s="10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>109</v>
@@ -2012,6 +2012,9 @@
       </c>
       <c r="R9" s="10">
         <v>0</v>
+      </c>
+      <c r="S9" s="10">
+        <v>1</v>
       </c>
       <c r="T9" s="10">
         <v>0.02</v>

</xml_diff>

<commit_message>
first working DA plan
</commit_message>
<xml_diff>
--- a/RunControl.xlsx
+++ b/RunControl.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8839AF1B-FE6B-4E77-B98A-B6758BDB134F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E599221-A94E-483A-A19C-8B99DAE4A645}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-75" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="paramlist" sheetId="1" r:id="rId1"/>
@@ -870,7 +870,7 @@
       <pane xSplit="6" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J11" sqref="J11"/>
+      <selection pane="bottomRight" activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
DA plan with stochastic returns
</commit_message>
<xml_diff>
--- a/RunControl.xlsx
+++ b/RunControl.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E599221-A94E-483A-A19C-8B99DAE4A645}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24A7918D-A7A5-4C01-A88B-6CB87C0D30A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-75" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -482,10 +482,10 @@
     <t>dr_DA</t>
   </si>
   <si>
-    <t>idxFull_act_DA</t>
-  </si>
-  <si>
-    <t>idxFull_ret_DA</t>
+    <t>idxFull_DA</t>
+  </si>
+  <si>
+    <t>idxFloor_DA</t>
   </si>
 </sst>
 </file>
@@ -870,7 +870,7 @@
       <pane xSplit="6" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J27" sqref="J27"/>
+      <selection pane="bottomRight" activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3692,10 +3692,10 @@
         <v>2.1999999999999999E-2</v>
       </c>
       <c r="I19" s="10">
-        <v>0.02</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="J19" s="10">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="K19" s="10">
         <v>7.4999999999999997E-2</v>

</xml_diff>

<commit_message>
working version of DA plan
</commit_message>
<xml_diff>
--- a/RunControl.xlsx
+++ b/RunControl.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24A7918D-A7A5-4C01-A88B-6CB87C0D30A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DBFBAF1-701C-47B9-A6DE-F3C9EF77337F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-75" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="153">
   <si>
     <t>runname</t>
   </si>
@@ -486,6 +486,9 @@
   </si>
   <si>
     <t>idxFloor_DA</t>
+  </si>
+  <si>
+    <t>DA_FR100</t>
   </si>
 </sst>
 </file>
@@ -864,13 +867,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:BP44"/>
+  <dimension ref="A1:BP45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="6" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J24" sqref="J24"/>
+      <selection pane="bottomRight" activeCell="BN36" sqref="BN36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6145,38 +6148,192 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:68" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="B36" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="C36" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="O36" s="10" t="s">
+    <row r="35" spans="1:68" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="B35" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="D35" s="10">
+        <v>1</v>
+      </c>
+      <c r="E35" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="F35" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="G35" s="10">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="H35" s="10">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="I35" s="10">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="J35" s="10">
+        <v>0</v>
+      </c>
+      <c r="K35" s="10">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="L35" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="O35" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="P36" s="10">
-        <v>1</v>
-      </c>
-      <c r="Q36" s="10">
-        <v>1</v>
-      </c>
-      <c r="R36" s="10">
-        <v>1</v>
-      </c>
-      <c r="S36" s="10">
+      <c r="U35" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="V35" s="10">
+        <v>0</v>
+      </c>
+      <c r="W35" s="10">
+        <v>1</v>
+      </c>
+      <c r="X35" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="Y35" s="10">
+        <v>0</v>
+      </c>
+      <c r="Z35" s="10">
+        <v>0.9</v>
+      </c>
+      <c r="AA35" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="AB35" s="10">
+        <v>0</v>
+      </c>
+      <c r="AC35" s="10">
+        <v>0.9</v>
+      </c>
+      <c r="AD35" s="10">
+        <v>0.01</v>
+      </c>
+      <c r="AE35" s="10">
+        <v>1E-3</v>
+      </c>
+      <c r="AF35" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="AG35" s="10">
+        <v>0</v>
+      </c>
+      <c r="AH35" s="10">
+        <v>1</v>
+      </c>
+      <c r="AI35" s="10">
+        <v>1</v>
+      </c>
+      <c r="AM35" s="10">
+        <v>0.05</v>
+      </c>
+      <c r="AN35" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="AO35" s="10">
+        <v>0</v>
+      </c>
+      <c r="AP35" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="AQ35" s="10">
         <v>0.03</v>
       </c>
-      <c r="T36" s="10">
+      <c r="AR35" s="10">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AS35" s="10">
+        <v>0.04</v>
+      </c>
+      <c r="AT35" s="10">
+        <v>0.11</v>
+      </c>
+      <c r="AU35" s="10">
+        <v>1</v>
+      </c>
+      <c r="AV35" s="10">
         <v>0.03</v>
       </c>
+      <c r="AW35" s="10">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AX35" s="10">
+        <v>0.7</v>
+      </c>
+      <c r="AY35" s="10">
+        <v>1</v>
+      </c>
+      <c r="AZ35" s="10">
+        <v>15</v>
+      </c>
+      <c r="BA35" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="BB35" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="BC35" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="BD35" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="BE35" s="10">
+        <v>5</v>
+      </c>
+      <c r="BF35" s="10">
+        <v>8.2199999999999995E-2</v>
+      </c>
+      <c r="BG35" s="10">
+        <v>0.12</v>
+      </c>
+      <c r="BH35" s="10">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="BI35" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="BJ35" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="BK35" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="BL35" s="10">
+        <v>0.01</v>
+      </c>
+      <c r="BM35" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="BN35" s="10">
+        <v>1</v>
+      </c>
+      <c r="BO35" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="BP35" s="10" t="b">
+        <v>1</v>
+      </c>
     </row>
+    <row r="36" spans="1:68" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="37" spans="1:68" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
-        <v>106</v>
+        <v>108</v>
+      </c>
+      <c r="B37" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>111</v>
       </c>
       <c r="O37" s="10" t="s">
         <v>76</v>
@@ -6191,329 +6348,194 @@
         <v>1</v>
       </c>
       <c r="S37" s="10">
-        <v>0.06</v>
+        <v>0.03</v>
       </c>
       <c r="T37" s="10">
-        <v>0.06</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="38" spans="1:68" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="B38" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="C38" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="D38" s="10">
-        <v>1</v>
-      </c>
-      <c r="E38" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="F38" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="G38" s="10">
-        <v>1.4999999999999999E-2</v>
+        <v>106</v>
       </c>
       <c r="O38" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="U38" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="V38" s="10">
-        <v>0</v>
-      </c>
-      <c r="X38" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="Y38" s="10">
-        <v>0</v>
-      </c>
-      <c r="Z38" s="10">
+      <c r="P38" s="10">
+        <v>1</v>
+      </c>
+      <c r="Q38" s="10">
+        <v>1</v>
+      </c>
+      <c r="R38" s="10">
+        <v>1</v>
+      </c>
+      <c r="S38" s="10">
+        <v>0.06</v>
+      </c>
+      <c r="T38" s="10">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="39" spans="1:68" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="B39" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="C39" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="D39" s="10">
+        <v>1</v>
+      </c>
+      <c r="E39" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="F39" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="G39" s="10">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="O39" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="U39" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="V39" s="10">
+        <v>0</v>
+      </c>
+      <c r="X39" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="Y39" s="10">
+        <v>0</v>
+      </c>
+      <c r="Z39" s="10">
         <v>0.9</v>
       </c>
-      <c r="AA38" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="AB38" s="10">
-        <v>0</v>
-      </c>
-      <c r="AC38" s="10">
+      <c r="AA39" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="AB39" s="10">
+        <v>0</v>
+      </c>
+      <c r="AC39" s="10">
         <v>0.9</v>
       </c>
-      <c r="AD38" s="10">
+      <c r="AD39" s="10">
         <v>0.01</v>
       </c>
-      <c r="AE38" s="10">
+      <c r="AE39" s="10">
         <v>1E-3</v>
       </c>
-      <c r="AF38" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="AG38" s="10">
-        <v>0</v>
-      </c>
-      <c r="AH38" s="10">
-        <v>1</v>
-      </c>
-      <c r="AI38" s="10">
-        <v>1</v>
-      </c>
-      <c r="AM38" s="10">
+      <c r="AF39" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="AG39" s="10">
+        <v>0</v>
+      </c>
+      <c r="AH39" s="10">
+        <v>1</v>
+      </c>
+      <c r="AI39" s="10">
+        <v>1</v>
+      </c>
+      <c r="AM39" s="10">
         <v>0.05</v>
       </c>
-      <c r="AN38" s="10">
-        <v>0.5</v>
-      </c>
-      <c r="AO38" s="10">
-        <v>0</v>
-      </c>
-      <c r="AP38" s="10">
-        <v>0.5</v>
-      </c>
-      <c r="AQ38" s="10">
+      <c r="AN39" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="AO39" s="10">
+        <v>0</v>
+      </c>
+      <c r="AP39" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="AQ39" s="10">
         <v>0.03</v>
       </c>
-      <c r="AR38" s="10">
+      <c r="AR39" s="10">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AS38" s="10">
+      <c r="AS39" s="10">
         <v>0.04</v>
       </c>
-      <c r="AT38" s="10">
+      <c r="AT39" s="10">
         <v>0.11</v>
       </c>
-      <c r="AV38" s="10">
+      <c r="AV39" s="10">
         <v>0.03</v>
       </c>
-      <c r="AW38" s="10">
+      <c r="AW39" s="10">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AX38" s="10">
+      <c r="AX39" s="10">
         <v>0.7</v>
       </c>
-      <c r="AY38" s="10">
-        <v>1</v>
-      </c>
-      <c r="AZ38" s="10">
+      <c r="AY39" s="10">
+        <v>1</v>
+      </c>
+      <c r="AZ39" s="10">
         <v>15</v>
       </c>
-      <c r="BA38" s="10" t="s">
+      <c r="BA39" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="BB38" s="10" t="s">
+      <c r="BB39" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="BC38" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="BD38" s="10" t="s">
+      <c r="BC39" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="BD39" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="BE38" s="10">
+      <c r="BE39" s="10">
         <v>5</v>
       </c>
-      <c r="BF38" s="10">
+      <c r="BF39" s="10">
         <v>8.2199999999999995E-2</v>
       </c>
-      <c r="BG38" s="10">
+      <c r="BG39" s="10">
         <v>0.12</v>
       </c>
-      <c r="BH38" s="10">
+      <c r="BH39" s="10">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="BI38" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="BJ38" s="10" t="s">
+      <c r="BI39" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="BJ39" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="BK38" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="BL38" s="10">
+      <c r="BK39" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="BL39" s="10">
         <v>0.01</v>
       </c>
-      <c r="BM38" s="10" t="s">
+      <c r="BM39" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="BN38" s="10">
+      <c r="BN39" s="10">
         <v>0.75</v>
       </c>
-      <c r="BO38" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="BP38" s="10" t="b">
+      <c r="BO39" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="BP39" s="10" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:68" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" spans="1:68" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="B40" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="C40" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="D40" s="10">
-        <v>1</v>
-      </c>
-      <c r="E40" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="F40" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="G40" s="10">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="O40" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="U40" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="V40" s="10">
-        <v>0</v>
-      </c>
-      <c r="X40" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="Y40" s="10">
-        <v>0</v>
-      </c>
-      <c r="Z40" s="10">
-        <v>0.9</v>
-      </c>
-      <c r="AA40" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="AB40" s="10">
-        <v>0</v>
-      </c>
-      <c r="AC40" s="10">
-        <v>0.9</v>
-      </c>
-      <c r="AD40" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="AE40" s="10">
-        <v>1E-3</v>
-      </c>
-      <c r="AF40" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="AG40" s="10">
-        <v>0</v>
-      </c>
-      <c r="AH40" s="10">
-        <v>1</v>
-      </c>
-      <c r="AI40" s="10">
-        <v>1</v>
-      </c>
-      <c r="AM40" s="10">
-        <v>0.05</v>
-      </c>
-      <c r="AN40" s="10">
-        <v>0.5</v>
-      </c>
-      <c r="AO40" s="10">
-        <v>0</v>
-      </c>
-      <c r="AP40" s="10">
-        <v>0.5</v>
-      </c>
-      <c r="AQ40" s="10">
-        <v>0.03</v>
-      </c>
-      <c r="AR40" s="10">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="AS40" s="10">
-        <v>0.04</v>
-      </c>
-      <c r="AT40" s="10">
-        <v>0.11</v>
-      </c>
-      <c r="AU40" s="10">
-        <v>5</v>
-      </c>
-      <c r="AV40" s="10">
-        <v>0.03</v>
-      </c>
-      <c r="AW40" s="10">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="AX40" s="10">
-        <v>0.7</v>
-      </c>
-      <c r="AY40" s="10">
-        <v>1</v>
-      </c>
-      <c r="AZ40" s="10">
-        <v>15</v>
-      </c>
-      <c r="BA40" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="BB40" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="BC40" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="BD40" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="BE40" s="10">
-        <v>5</v>
-      </c>
-      <c r="BF40" s="10">
-        <v>8.2199999999999995E-2</v>
-      </c>
-      <c r="BG40" s="10">
-        <v>0.12</v>
-      </c>
-      <c r="BH40" s="10">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="BI40" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="BJ40" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="BK40" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="BL40" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="BM40" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="BN40" s="10">
-        <v>0.75</v>
-      </c>
-      <c r="BO40" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="BP40" s="10" t="b">
-        <v>1</v>
-      </c>
-    </row>
+    <row r="40" spans="1:68" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="41" spans="1:68" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="10" t="s">
-        <v>119</v>
+        <v>99</v>
       </c>
       <c r="B41" s="10" t="b">
         <v>0</v>
@@ -6660,7 +6682,7 @@
         <v>23</v>
       </c>
       <c r="BN41" s="10">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="BO41" s="10" t="b">
         <v>1</v>
@@ -6669,15 +6691,173 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:68" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="1:68" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="B42" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="C42" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="D42" s="10">
+        <v>1</v>
+      </c>
+      <c r="E42" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="F42" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="G42" s="10">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="O42" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="U42" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="V42" s="10">
+        <v>0</v>
+      </c>
+      <c r="X42" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="Y42" s="10">
+        <v>0</v>
+      </c>
+      <c r="Z42" s="10">
+        <v>0.9</v>
+      </c>
+      <c r="AA42" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="AB42" s="10">
+        <v>0</v>
+      </c>
+      <c r="AC42" s="10">
+        <v>0.9</v>
+      </c>
+      <c r="AD42" s="10">
+        <v>0.01</v>
+      </c>
+      <c r="AE42" s="10">
+        <v>1E-3</v>
+      </c>
+      <c r="AF42" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="AG42" s="10">
+        <v>0</v>
+      </c>
+      <c r="AH42" s="10">
+        <v>1</v>
+      </c>
+      <c r="AI42" s="10">
+        <v>1</v>
+      </c>
+      <c r="AM42" s="10">
+        <v>0.05</v>
+      </c>
+      <c r="AN42" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="AO42" s="10">
+        <v>0</v>
+      </c>
+      <c r="AP42" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="AQ42" s="10">
+        <v>0.03</v>
+      </c>
+      <c r="AR42" s="10">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AS42" s="10">
+        <v>0.04</v>
+      </c>
+      <c r="AT42" s="10">
+        <v>0.11</v>
+      </c>
+      <c r="AU42" s="10">
+        <v>5</v>
+      </c>
+      <c r="AV42" s="10">
+        <v>0.03</v>
+      </c>
+      <c r="AW42" s="10">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AX42" s="10">
+        <v>0.7</v>
+      </c>
+      <c r="AY42" s="10">
+        <v>1</v>
+      </c>
+      <c r="AZ42" s="10">
+        <v>15</v>
+      </c>
+      <c r="BA42" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="BB42" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="BC42" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="BD42" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="BE42" s="10">
+        <v>5</v>
+      </c>
+      <c r="BF42" s="10">
+        <v>8.2199999999999995E-2</v>
+      </c>
+      <c r="BG42" s="10">
+        <v>0.12</v>
+      </c>
+      <c r="BH42" s="10">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="BI42" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="BJ42" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="BK42" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="BL42" s="10">
+        <v>0.01</v>
+      </c>
+      <c r="BM42" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="BN42" s="10">
+        <v>1</v>
+      </c>
+      <c r="BO42" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="BP42" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
     <row r="43" spans="1:68" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="44" spans="1:68" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="1:68" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B36:B44 B3:B34" xr:uid="{05E01AB2-72EC-4550-ACB8-4E83765DE296}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B45" xr:uid="{05E01AB2-72EC-4550-ACB8-4E83765DE296}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O36:O38 O40:O41 O3:O16 O21:O32 O18:O19 O34" xr:uid="{8DBFC5CB-438A-4309-B948-24597CAE3D7F}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O41:O42 O3:O16 O21:O32 O18:O19 O34:O39" xr:uid="{8DBFC5CB-438A-4309-B948-24597CAE3D7F}">
       <formula1>"preSet, ALpct,MApct"</formula1>
     </dataValidation>
   </dataValidations>
@@ -6690,7 +6870,7 @@
           <x14:formula1>
             <xm:f>Policies!$B$3:$B$9</xm:f>
           </x14:formula1>
-          <xm:sqref>F38 F36 F40:F41 F3:F34</xm:sqref>
+          <xm:sqref>F39 F41:F42 F3:F37</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -6704,7 +6884,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6740,10 +6920,10 @@
         <v>91</v>
       </c>
       <c r="B2">
-        <v>2000</v>
+        <v>500</v>
       </c>
       <c r="C2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D2">
         <v>20</v>

</xml_diff>

<commit_message>
update with latest DA model
</commit_message>
<xml_diff>
--- a/RunControl.xlsx
+++ b/RunControl.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DBFBAF1-701C-47B9-A6DE-F3C9EF77337F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{836A63EE-63D6-4B89-9630-1EF42F3EB677}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-75" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="6855" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="paramlist" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="153">
   <si>
     <t>runname</t>
   </si>
@@ -870,10 +870,10 @@
   <dimension ref="A1:BP45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="2" topLeftCell="Q12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="BN36" sqref="BN36"/>
+      <selection pane="bottomRight" activeCell="A26" sqref="A26:XFD28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2192,7 +2192,7 @@
         <v>54</v>
       </c>
       <c r="B10" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10" s="10" t="s">
         <v>110</v>
@@ -2356,7 +2356,7 @@
         <v>131</v>
       </c>
       <c r="B11" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11" s="10" t="s">
         <v>110</v>
@@ -2520,7 +2520,7 @@
         <v>137</v>
       </c>
       <c r="B12" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C12" s="10" t="s">
         <v>110</v>
@@ -3510,7 +3510,7 @@
         <v>143</v>
       </c>
       <c r="B18" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C18" s="10" t="s">
         <v>144</v>
@@ -3674,7 +3674,7 @@
         <v>146</v>
       </c>
       <c r="B19" s="10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C19" s="10" t="s">
         <v>146</v>
@@ -3692,19 +3692,22 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="H19" s="10">
-        <v>2.1999999999999999E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="I19" s="10">
-        <v>2.5000000000000001E-2</v>
+        <v>0.02</v>
       </c>
       <c r="J19" s="10">
-        <v>0</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="K19" s="10">
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="L19" s="10" t="s">
-        <v>134</v>
+        <v>112</v>
+      </c>
+      <c r="M19" s="10" t="s">
+        <v>112</v>
       </c>
       <c r="O19" s="10" t="s">
         <v>76</v>
@@ -4671,7 +4674,7 @@
         <v>123</v>
       </c>
       <c r="B26" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C26" s="10" t="s">
         <v>110</v>
@@ -4835,7 +4838,7 @@
         <v>136</v>
       </c>
       <c r="B27" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C27" s="10" t="s">
         <v>110</v>
@@ -4999,7 +5002,7 @@
         <v>139</v>
       </c>
       <c r="B28" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C28" s="10" t="s">
         <v>110</v>
@@ -5989,7 +5992,7 @@
         <v>145</v>
       </c>
       <c r="B34" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C34" s="10" t="s">
         <v>144</v>
@@ -6153,7 +6156,7 @@
         <v>152</v>
       </c>
       <c r="B35" s="10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C35" s="10" t="s">
         <v>146</v>
@@ -6171,13 +6174,13 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="H35" s="10">
-        <v>2.1999999999999999E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="I35" s="10">
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="J35" s="10">
-        <v>0</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="K35" s="10">
         <v>7.4999999999999997E-2</v>
@@ -6884,7 +6887,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6920,10 +6923,10 @@
         <v>91</v>
       </c>
       <c r="B2">
-        <v>500</v>
+        <v>2000</v>
       </c>
       <c r="C2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D2">
         <v>20</v>

</xml_diff>

<commit_message>
update runs and analysis for guidebook
</commit_message>
<xml_diff>
--- a/RunControl.xlsx
+++ b/RunControl.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{836A63EE-63D6-4B89-9630-1EF42F3EB677}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01F3FCFD-3507-406F-B444-7D83235B96B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="6855" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="5460" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="paramlist" sheetId="1" r:id="rId1"/>
@@ -568,7 +568,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -586,6 +586,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -869,11 +870,11 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:BP45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6" ySplit="2" topLeftCell="Q12" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="6" ySplit="2" topLeftCell="AL3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A26" sqref="A26:XFD28"/>
+      <selection pane="bottomRight" activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2192,7 +2193,7 @@
         <v>54</v>
       </c>
       <c r="B10" s="10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10" s="10" t="s">
         <v>110</v>
@@ -2356,7 +2357,7 @@
         <v>131</v>
       </c>
       <c r="B11" s="10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C11" s="10" t="s">
         <v>110</v>
@@ -2520,7 +2521,7 @@
         <v>137</v>
       </c>
       <c r="B12" s="10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C12" s="10" t="s">
         <v>110</v>
@@ -3172,11 +3173,11 @@
       </c>
     </row>
     <row r="16" spans="1:68" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="14" t="s">
         <v>105</v>
       </c>
       <c r="B16" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C16" s="10" t="s">
         <v>110</v>
@@ -3233,7 +3234,7 @@
         <v>1E-3</v>
       </c>
       <c r="AF16" s="10">
-        <v>0.02</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="AG16" s="10">
         <v>0</v>
@@ -3415,7 +3416,7 @@
         <v>1</v>
       </c>
       <c r="AM17" s="10">
-        <v>0.05</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="AN17" s="10">
         <v>0.5</v>
@@ -3510,7 +3511,7 @@
         <v>143</v>
       </c>
       <c r="B18" s="10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C18" s="10" t="s">
         <v>144</v>
@@ -4014,7 +4015,7 @@
       </c>
     </row>
     <row r="22" spans="1:68" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="10" t="s">
+      <c r="A22" s="17" t="s">
         <v>120</v>
       </c>
       <c r="B22" s="10" t="b">
@@ -4674,7 +4675,7 @@
         <v>123</v>
       </c>
       <c r="B26" s="10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C26" s="10" t="s">
         <v>110</v>
@@ -4838,7 +4839,7 @@
         <v>136</v>
       </c>
       <c r="B27" s="10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C27" s="10" t="s">
         <v>110</v>
@@ -5002,7 +5003,7 @@
         <v>139</v>
       </c>
       <c r="B28" s="10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C28" s="10" t="s">
         <v>110</v>
@@ -5654,7 +5655,7 @@
       </c>
     </row>
     <row r="32" spans="1:68" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="10" t="s">
+      <c r="A32" s="14" t="s">
         <v>126</v>
       </c>
       <c r="B32" s="10" t="b">
@@ -5715,7 +5716,7 @@
         <v>1E-3</v>
       </c>
       <c r="AF32" s="10">
-        <v>0.02</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="AG32" s="10">
         <v>0</v>
@@ -5992,7 +5993,7 @@
         <v>145</v>
       </c>
       <c r="B34" s="10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C34" s="10" t="s">
         <v>144</v>
@@ -6537,7 +6538,7 @@
     </row>
     <row r="40" spans="1:68" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="41" spans="1:68" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="10" t="s">
+      <c r="A41" s="14" t="s">
         <v>99</v>
       </c>
       <c r="B41" s="10" t="b">
@@ -6695,7 +6696,7 @@
       </c>
     </row>
     <row r="42" spans="1:68" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="10" t="s">
+      <c r="A42" s="14" t="s">
         <v>119</v>
       </c>
       <c r="B42" s="10" t="b">
@@ -6886,8 +6887,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
update figures for policy guidebook
</commit_message>
<xml_diff>
--- a/RunControl.xlsx
+++ b/RunControl.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01F3FCFD-3507-406F-B444-7D83235B96B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27934D7B-AEBE-4B5F-81AF-493B4E236DA3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="5460" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="5460" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="paramlist" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="154">
   <si>
     <t>runname</t>
   </si>
@@ -489,6 +489,9 @@
   </si>
   <si>
     <t>DA_FR100</t>
+  </si>
+  <si>
+    <t>cola_SDRS_noCAeec</t>
   </si>
 </sst>
 </file>
@@ -868,13 +871,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:BP45"/>
+  <dimension ref="A1:BP46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="6" ySplit="2" topLeftCell="AL3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="6" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A34" sqref="A34"/>
+      <selection pane="bottomRight" activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1697,11 +1700,11 @@
       </c>
     </row>
     <row r="7" spans="1:68" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
-        <v>87</v>
+      <c r="A7" s="14" t="s">
+        <v>99</v>
       </c>
       <c r="B7" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>109</v>
@@ -1713,7 +1716,7 @@
         <v>50</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G7" s="10">
         <v>1.4999999999999999E-2</v>
@@ -1862,7 +1865,7 @@
     </row>
     <row r="8" spans="1:68" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>130</v>
+        <v>87</v>
       </c>
       <c r="B8" s="10" t="b">
         <v>0</v>
@@ -1895,7 +1898,7 @@
         <v>0</v>
       </c>
       <c r="W8" s="10">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="X8" s="10">
         <v>0.02</v>
@@ -1958,7 +1961,7 @@
         <v>0.11</v>
       </c>
       <c r="AU8" s="10">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="AV8" s="10">
         <v>0.03</v>
@@ -2026,7 +2029,7 @@
     </row>
     <row r="9" spans="1:68" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
-        <v>88</v>
+        <v>130</v>
       </c>
       <c r="B9" s="10" t="b">
         <v>0</v>
@@ -2041,7 +2044,7 @@
         <v>50</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G9" s="10">
         <v>1.4999999999999999E-2</v>
@@ -2059,7 +2062,7 @@
         <v>0</v>
       </c>
       <c r="W9" s="10">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="X9" s="10">
         <v>0.02</v>
@@ -2122,7 +2125,7 @@
         <v>0.11</v>
       </c>
       <c r="AU9" s="10">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="AV9" s="10">
         <v>0.03</v>
@@ -2190,22 +2193,22 @@
     </row>
     <row r="10" spans="1:68" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
-        <v>54</v>
+        <v>88</v>
       </c>
       <c r="B10" s="10" t="b">
         <v>0</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D10" s="10">
         <v>1</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>63</v>
+        <v>88</v>
       </c>
       <c r="G10" s="10">
         <v>1.4999999999999999E-2</v>
@@ -2354,7 +2357,7 @@
     </row>
     <row r="11" spans="1:68" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
-        <v>131</v>
+        <v>54</v>
       </c>
       <c r="B11" s="10" t="b">
         <v>0</v>
@@ -2386,8 +2389,8 @@
       <c r="V11" s="10">
         <v>0</v>
       </c>
-      <c r="W11" s="14">
-        <v>5</v>
+      <c r="W11" s="10">
+        <v>1</v>
       </c>
       <c r="X11" s="10">
         <v>0.02</v>
@@ -2450,7 +2453,7 @@
         <v>0.11</v>
       </c>
       <c r="AU11" s="10">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="AV11" s="10">
         <v>0.03</v>
@@ -2518,7 +2521,7 @@
     </row>
     <row r="12" spans="1:68" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B12" s="10" t="b">
         <v>0</v>
@@ -2545,10 +2548,10 @@
         <v>76</v>
       </c>
       <c r="U12" s="10">
-        <v>2.5000000000000001E-2</v>
+        <v>0.02</v>
       </c>
       <c r="V12" s="10">
-        <v>5.0000000000000001E-3</v>
+        <v>0</v>
       </c>
       <c r="W12" s="14">
         <v>5</v>
@@ -2680,9 +2683,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:68" s="10" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:68" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
-        <v>55</v>
+        <v>137</v>
       </c>
       <c r="B13" s="10" t="b">
         <v>0</v>
@@ -2694,7 +2697,7 @@
         <v>1</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F13" s="10" t="s">
         <v>63</v>
@@ -2709,13 +2712,13 @@
         <v>76</v>
       </c>
       <c r="U13" s="10">
-        <v>0.02</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="V13" s="10">
-        <v>0</v>
-      </c>
-      <c r="W13" s="10">
-        <v>1</v>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="W13" s="14">
+        <v>5</v>
       </c>
       <c r="X13" s="10">
         <v>0.02</v>
@@ -2778,7 +2781,7 @@
         <v>0.11</v>
       </c>
       <c r="AU13" s="10">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="AV13" s="10">
         <v>0.03</v>
@@ -2846,7 +2849,7 @@
     </row>
     <row r="14" spans="1:68" s="10" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
-        <v>138</v>
+        <v>55</v>
       </c>
       <c r="B14" s="10" t="b">
         <v>0</v>
@@ -2882,13 +2885,13 @@
         <v>1</v>
       </c>
       <c r="X14" s="10">
-        <v>2.5000000000000001E-2</v>
+        <v>0.02</v>
       </c>
       <c r="Y14" s="10">
-        <v>5.0000000000000001E-3</v>
+        <v>0</v>
       </c>
       <c r="Z14" s="10">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="AA14" s="10">
         <v>0.02</v>
@@ -3008,9 +3011,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:68" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:68" s="10" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
-        <v>103</v>
+        <v>138</v>
       </c>
       <c r="B15" s="10" t="b">
         <v>0</v>
@@ -3022,7 +3025,7 @@
         <v>1</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F15" s="10" t="s">
         <v>63</v>
@@ -3046,13 +3049,13 @@
         <v>1</v>
       </c>
       <c r="X15" s="10">
-        <v>0.02</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="Y15" s="10">
-        <v>0</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="Z15" s="10">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="AA15" s="10">
         <v>0.02</v>
@@ -3173,11 +3176,11 @@
       </c>
     </row>
     <row r="16" spans="1:68" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="14" t="s">
-        <v>105</v>
+      <c r="A16" s="10" t="s">
+        <v>103</v>
       </c>
       <c r="B16" s="10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C16" s="10" t="s">
         <v>110</v>
@@ -3186,7 +3189,7 @@
         <v>1</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F16" s="10" t="s">
         <v>63</v>
@@ -3234,7 +3237,7 @@
         <v>1E-3</v>
       </c>
       <c r="AF16" s="10">
-        <v>2.5000000000000001E-2</v>
+        <v>0.02</v>
       </c>
       <c r="AG16" s="10">
         <v>0</v>
@@ -3243,13 +3246,7 @@
         <v>1</v>
       </c>
       <c r="AI16" s="10">
-        <v>2</v>
-      </c>
-      <c r="AJ16" s="10">
-        <v>0.5</v>
-      </c>
-      <c r="AK16" s="10">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="AM16" s="10">
         <v>0.05</v>
@@ -3343,20 +3340,20 @@
       </c>
     </row>
     <row r="17" spans="1:68" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
-        <v>107</v>
+      <c r="A17" s="17" t="s">
+        <v>105</v>
       </c>
       <c r="B17" s="10" t="b">
         <v>0</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D17" s="10">
         <v>1</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="F17" s="10" t="s">
         <v>63</v>
@@ -3365,10 +3362,10 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="L17" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="M17" s="10" t="s">
-        <v>112</v>
+        <v>134</v>
+      </c>
+      <c r="O17" s="10" t="s">
+        <v>76</v>
       </c>
       <c r="U17" s="10">
         <v>0.02</v>
@@ -3404,7 +3401,7 @@
         <v>1E-3</v>
       </c>
       <c r="AF17" s="10">
-        <v>0.02</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="AG17" s="10">
         <v>0</v>
@@ -3413,10 +3410,16 @@
         <v>1</v>
       </c>
       <c r="AI17" s="10">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="AJ17" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="AK17" s="10">
+        <v>0.5</v>
       </c>
       <c r="AM17" s="10">
-        <v>2.5000000000000001E-2</v>
+        <v>0.05</v>
       </c>
       <c r="AN17" s="10">
         <v>0.5</v>
@@ -3507,23 +3510,23 @@
       </c>
     </row>
     <row r="18" spans="1:68" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="10" t="s">
-        <v>143</v>
+      <c r="A18" s="14" t="s">
+        <v>153</v>
       </c>
       <c r="B18" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>144</v>
+        <v>110</v>
       </c>
       <c r="D18" s="10">
         <v>1</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>85</v>
+        <v>63</v>
       </c>
       <c r="G18" s="10">
         <v>1.4999999999999999E-2</v>
@@ -3535,13 +3538,13 @@
         <v>76</v>
       </c>
       <c r="U18" s="10">
-        <v>2.5000000000000001E-2</v>
+        <v>0.02</v>
       </c>
       <c r="V18" s="10">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="W18" s="14">
-        <v>5</v>
+        <v>0</v>
+      </c>
+      <c r="W18" s="10">
+        <v>1</v>
       </c>
       <c r="X18" s="10">
         <v>0.02</v>
@@ -3568,7 +3571,7 @@
         <v>1E-3</v>
       </c>
       <c r="AF18" s="10">
-        <v>0.02</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="AG18" s="10">
         <v>0</v>
@@ -3577,7 +3580,13 @@
         <v>1</v>
       </c>
       <c r="AI18" s="10">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="AJ18" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="AK18" s="10">
+        <v>0</v>
       </c>
       <c r="AM18" s="10">
         <v>0.05</v>
@@ -3586,7 +3595,7 @@
         <v>0.5</v>
       </c>
       <c r="AO18" s="10">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="AP18" s="10">
         <v>0.5</v>
@@ -3604,7 +3613,7 @@
         <v>0.11</v>
       </c>
       <c r="AU18" s="10">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="AV18" s="10">
         <v>0.03</v>
@@ -3672,19 +3681,19 @@
     </row>
     <row r="19" spans="1:68" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
-        <v>146</v>
+        <v>107</v>
       </c>
       <c r="B19" s="10" t="b">
         <v>0</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>146</v>
+        <v>111</v>
       </c>
       <c r="D19" s="10">
         <v>1</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F19" s="10" t="s">
         <v>63</v>
@@ -3692,27 +3701,12 @@
       <c r="G19" s="10">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="H19" s="10">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="I19" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="J19" s="10">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="K19" s="10">
-        <v>7.4999999999999997E-2</v>
-      </c>
       <c r="L19" s="10" t="s">
         <v>112</v>
       </c>
       <c r="M19" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="O19" s="10" t="s">
-        <v>76</v>
-      </c>
       <c r="U19" s="10">
         <v>0.02</v>
       </c>
@@ -3759,7 +3753,7 @@
         <v>1</v>
       </c>
       <c r="AM19" s="10">
-        <v>0.05</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="AN19" s="10">
         <v>0.5</v>
@@ -3849,22 +3843,185 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:68" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:68" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="B20" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="D20" s="10">
+        <v>1</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="G20" s="10">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="L20" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="O20" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="U20" s="10">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="V20" s="10">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="W20" s="14">
+        <v>5</v>
+      </c>
+      <c r="X20" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="Y20" s="10">
+        <v>0</v>
+      </c>
+      <c r="Z20" s="10">
+        <v>0.9</v>
+      </c>
+      <c r="AA20" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="AB20" s="10">
+        <v>0</v>
+      </c>
+      <c r="AC20" s="10">
+        <v>0.9</v>
+      </c>
+      <c r="AD20" s="10">
+        <v>0.01</v>
+      </c>
+      <c r="AE20" s="10">
+        <v>1E-3</v>
+      </c>
+      <c r="AF20" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="AG20" s="10">
+        <v>0</v>
+      </c>
+      <c r="AH20" s="10">
+        <v>1</v>
+      </c>
+      <c r="AI20" s="10">
+        <v>1</v>
+      </c>
+      <c r="AM20" s="10">
+        <v>0.05</v>
+      </c>
+      <c r="AN20" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="AO20" s="10">
+        <v>0.05</v>
+      </c>
+      <c r="AP20" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="AQ20" s="10">
+        <v>0.03</v>
+      </c>
+      <c r="AR20" s="10">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AS20" s="10">
+        <v>0.04</v>
+      </c>
+      <c r="AT20" s="10">
+        <v>0.11</v>
+      </c>
+      <c r="AU20" s="10">
+        <v>5</v>
+      </c>
+      <c r="AV20" s="10">
+        <v>0.03</v>
+      </c>
+      <c r="AW20" s="10">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AX20" s="10">
+        <v>0.7</v>
+      </c>
+      <c r="AY20" s="10">
+        <v>1</v>
+      </c>
+      <c r="AZ20" s="10">
+        <v>15</v>
+      </c>
+      <c r="BA20" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="BB20" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="BC20" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="BD20" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="BE20" s="10">
+        <v>5</v>
+      </c>
+      <c r="BF20" s="10">
+        <v>8.2199999999999995E-2</v>
+      </c>
+      <c r="BG20" s="10">
+        <v>0.12</v>
+      </c>
+      <c r="BH20" s="10">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="BI20" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="BJ20" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="BK20" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="BL20" s="10">
+        <v>0.01</v>
+      </c>
+      <c r="BM20" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="BN20" s="10">
+        <v>0.75</v>
+      </c>
+      <c r="BO20" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="BP20" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
     <row r="21" spans="1:68" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
-        <v>118</v>
+        <v>146</v>
       </c>
       <c r="B21" s="10" t="b">
         <v>0</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>112</v>
+        <v>146</v>
       </c>
       <c r="D21" s="10">
         <v>1</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F21" s="10" t="s">
         <v>63</v>
@@ -3872,8 +4029,23 @@
       <c r="G21" s="10">
         <v>1.4999999999999999E-2</v>
       </c>
+      <c r="H21" s="10">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="I21" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="J21" s="10">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="K21" s="10">
+        <v>7.4999999999999997E-2</v>
+      </c>
       <c r="L21" s="10" t="s">
-        <v>134</v>
+        <v>112</v>
+      </c>
+      <c r="M21" s="10" t="s">
+        <v>112</v>
       </c>
       <c r="O21" s="10" t="s">
         <v>76</v>
@@ -4005,7 +4177,7 @@
         <v>23</v>
       </c>
       <c r="BN21" s="10">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="BO21" s="10" t="b">
         <v>1</v>
@@ -4014,179 +4186,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:68" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="17" t="s">
-        <v>120</v>
-      </c>
-      <c r="B22" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="D22" s="10">
-        <v>1</v>
-      </c>
-      <c r="E22" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="F22" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="G22" s="10">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="L22" s="10" t="s">
-        <v>134</v>
-      </c>
-      <c r="O22" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="U22" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="V22" s="10">
-        <v>0</v>
-      </c>
-      <c r="W22" s="10">
-        <v>1</v>
-      </c>
-      <c r="X22" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="Y22" s="10">
-        <v>0</v>
-      </c>
-      <c r="Z22" s="10">
-        <v>0.9</v>
-      </c>
-      <c r="AA22" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="AB22" s="10">
-        <v>0</v>
-      </c>
-      <c r="AC22" s="10">
-        <v>0.9</v>
-      </c>
-      <c r="AD22" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="AE22" s="10">
-        <v>1E-3</v>
-      </c>
-      <c r="AF22" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="AG22" s="10">
-        <v>0</v>
-      </c>
-      <c r="AH22" s="10">
-        <v>1</v>
-      </c>
-      <c r="AI22" s="10">
-        <v>1</v>
-      </c>
-      <c r="AM22" s="10">
-        <v>0.05</v>
-      </c>
-      <c r="AN22" s="10">
-        <v>0.5</v>
-      </c>
-      <c r="AO22" s="10">
-        <v>0.05</v>
-      </c>
-      <c r="AP22" s="10">
-        <v>0.5</v>
-      </c>
-      <c r="AQ22" s="10">
-        <v>0.03</v>
-      </c>
-      <c r="AR22" s="10">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="AS22" s="10">
-        <v>0.04</v>
-      </c>
-      <c r="AT22" s="10">
-        <v>0.11</v>
-      </c>
-      <c r="AU22" s="10">
-        <v>1</v>
-      </c>
-      <c r="AV22" s="10">
-        <v>0.03</v>
-      </c>
-      <c r="AW22" s="10">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="AX22" s="10">
-        <v>0.7</v>
-      </c>
-      <c r="AY22" s="10">
-        <v>1</v>
-      </c>
-      <c r="AZ22" s="10">
-        <v>15</v>
-      </c>
-      <c r="BA22" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="BB22" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="BC22" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="BD22" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="BE22" s="10">
-        <v>5</v>
-      </c>
-      <c r="BF22" s="10">
-        <v>8.2199999999999995E-2</v>
-      </c>
-      <c r="BG22" s="10">
-        <v>0.12</v>
-      </c>
-      <c r="BH22" s="10">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="BI22" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="BJ22" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="BK22" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="BL22" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="BM22" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="BN22" s="10">
-        <v>1</v>
-      </c>
-      <c r="BO22" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="BP22" s="10" t="b">
-        <v>1</v>
-      </c>
-    </row>
+    <row r="22" spans="1:68" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="23" spans="1:68" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B23" s="10" t="b">
         <v>0</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="D23" s="10">
         <v>1</v>
@@ -4195,7 +4204,7 @@
         <v>50</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>87</v>
+        <v>63</v>
       </c>
       <c r="G23" s="10">
         <v>1.4999999999999999E-2</v>
@@ -4343,8 +4352,8 @@
       </c>
     </row>
     <row r="24" spans="1:68" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="10" t="s">
-        <v>135</v>
+      <c r="A24" s="17" t="s">
+        <v>120</v>
       </c>
       <c r="B24" s="10" t="b">
         <v>0</v>
@@ -4359,7 +4368,7 @@
         <v>50</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G24" s="10">
         <v>1.4999999999999999E-2</v>
@@ -4376,8 +4385,8 @@
       <c r="V24" s="10">
         <v>0</v>
       </c>
-      <c r="W24" s="14">
-        <v>5</v>
+      <c r="W24" s="10">
+        <v>1</v>
       </c>
       <c r="X24" s="10">
         <v>0.02</v>
@@ -4422,7 +4431,7 @@
         <v>0.5</v>
       </c>
       <c r="AO24" s="10">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="AP24" s="10">
         <v>0.5</v>
@@ -4440,7 +4449,7 @@
         <v>0.11</v>
       </c>
       <c r="AU24" s="10">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="AV24" s="10">
         <v>0.03</v>
@@ -4508,7 +4517,7 @@
     </row>
     <row r="25" spans="1:68" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B25" s="10" t="b">
         <v>0</v>
@@ -4523,7 +4532,7 @@
         <v>50</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G25" s="10">
         <v>1.4999999999999999E-2</v>
@@ -4672,22 +4681,22 @@
     </row>
     <row r="26" spans="1:68" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
-        <v>123</v>
+        <v>135</v>
       </c>
       <c r="B26" s="10" t="b">
         <v>0</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D26" s="10">
         <v>1</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F26" s="10" t="s">
-        <v>63</v>
+        <v>87</v>
       </c>
       <c r="G26" s="10">
         <v>1.4999999999999999E-2</v>
@@ -4704,8 +4713,8 @@
       <c r="V26" s="10">
         <v>0</v>
       </c>
-      <c r="W26" s="10">
-        <v>1</v>
+      <c r="W26" s="14">
+        <v>5</v>
       </c>
       <c r="X26" s="10">
         <v>0.02</v>
@@ -4768,7 +4777,7 @@
         <v>0.11</v>
       </c>
       <c r="AU26" s="10">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="AV26" s="10">
         <v>0.03</v>
@@ -4836,22 +4845,22 @@
     </row>
     <row r="27" spans="1:68" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
-        <v>136</v>
+        <v>122</v>
       </c>
       <c r="B27" s="10" t="b">
         <v>0</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D27" s="10">
         <v>1</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>63</v>
+        <v>88</v>
       </c>
       <c r="G27" s="10">
         <v>1.4999999999999999E-2</v>
@@ -4868,8 +4877,8 @@
       <c r="V27" s="10">
         <v>0</v>
       </c>
-      <c r="W27" s="14">
-        <v>5</v>
+      <c r="W27" s="10">
+        <v>1</v>
       </c>
       <c r="X27" s="10">
         <v>0.02</v>
@@ -4932,7 +4941,7 @@
         <v>0.11</v>
       </c>
       <c r="AU27" s="10">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="AV27" s="10">
         <v>0.03</v>
@@ -5000,7 +5009,7 @@
     </row>
     <row r="28" spans="1:68" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
       <c r="B28" s="10" t="b">
         <v>0</v>
@@ -5027,13 +5036,13 @@
         <v>76</v>
       </c>
       <c r="U28" s="10">
-        <v>2.5000000000000001E-2</v>
+        <v>0.02</v>
       </c>
       <c r="V28" s="10">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="W28" s="14">
-        <v>5</v>
+        <v>0</v>
+      </c>
+      <c r="W28" s="10">
+        <v>1</v>
       </c>
       <c r="X28" s="10">
         <v>0.02</v>
@@ -5096,7 +5105,7 @@
         <v>0.11</v>
       </c>
       <c r="AU28" s="10">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="AV28" s="10">
         <v>0.03</v>
@@ -5162,9 +5171,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:68" s="10" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:68" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
-        <v>124</v>
+        <v>136</v>
       </c>
       <c r="B29" s="10" t="b">
         <v>0</v>
@@ -5176,7 +5185,7 @@
         <v>1</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F29" s="10" t="s">
         <v>63</v>
@@ -5196,8 +5205,8 @@
       <c r="V29" s="10">
         <v>0</v>
       </c>
-      <c r="W29" s="10">
-        <v>1</v>
+      <c r="W29" s="14">
+        <v>5</v>
       </c>
       <c r="X29" s="10">
         <v>0.02</v>
@@ -5260,7 +5269,7 @@
         <v>0.11</v>
       </c>
       <c r="AU29" s="10">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="AV29" s="10">
         <v>0.03</v>
@@ -5326,9 +5335,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:68" s="10" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:68" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B30" s="10" t="b">
         <v>0</v>
@@ -5340,7 +5349,7 @@
         <v>1</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F30" s="10" t="s">
         <v>63</v>
@@ -5355,22 +5364,22 @@
         <v>76</v>
       </c>
       <c r="U30" s="10">
-        <v>0.02</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="V30" s="10">
-        <v>0</v>
-      </c>
-      <c r="W30" s="10">
-        <v>1</v>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="W30" s="14">
+        <v>5</v>
       </c>
       <c r="X30" s="10">
-        <v>2.5000000000000001E-2</v>
+        <v>0.02</v>
       </c>
       <c r="Y30" s="10">
-        <v>5.0000000000000001E-3</v>
+        <v>0</v>
       </c>
       <c r="Z30" s="10">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="AA30" s="10">
         <v>0.02</v>
@@ -5424,7 +5433,7 @@
         <v>0.11</v>
       </c>
       <c r="AU30" s="10">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="AV30" s="10">
         <v>0.03</v>
@@ -5490,9 +5499,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:68" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:68" s="10" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B31" s="10" t="b">
         <v>0</v>
@@ -5504,7 +5513,7 @@
         <v>1</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F31" s="10" t="s">
         <v>63</v>
@@ -5654,9 +5663,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:68" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="14" t="s">
-        <v>126</v>
+    <row r="32" spans="1:68" s="10" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="10" t="s">
+        <v>140</v>
       </c>
       <c r="B32" s="10" t="b">
         <v>0</v>
@@ -5668,7 +5677,7 @@
         <v>1</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="F32" s="10" t="s">
         <v>63</v>
@@ -5692,13 +5701,13 @@
         <v>1</v>
       </c>
       <c r="X32" s="10">
-        <v>0.02</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="Y32" s="10">
-        <v>0</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="Z32" s="10">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="AA32" s="10">
         <v>0.02</v>
@@ -5716,7 +5725,7 @@
         <v>1E-3</v>
       </c>
       <c r="AF32" s="10">
-        <v>2.5000000000000001E-2</v>
+        <v>0.02</v>
       </c>
       <c r="AG32" s="10">
         <v>0</v>
@@ -5725,13 +5734,7 @@
         <v>1</v>
       </c>
       <c r="AI32" s="10">
-        <v>2</v>
-      </c>
-      <c r="AJ32" s="10">
-        <v>0.5</v>
-      </c>
-      <c r="AK32" s="10">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="AM32" s="10">
         <v>0.05</v>
@@ -5826,19 +5829,19 @@
     </row>
     <row r="33" spans="1:68" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B33" s="10" t="b">
         <v>0</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D33" s="10">
         <v>1</v>
       </c>
       <c r="E33" s="10" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="F33" s="10" t="s">
         <v>63</v>
@@ -5847,10 +5850,10 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="L33" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="M33" s="10" t="s">
-        <v>118</v>
+        <v>134</v>
+      </c>
+      <c r="O33" s="10" t="s">
+        <v>76</v>
       </c>
       <c r="U33" s="10">
         <v>0.02</v>
@@ -5898,7 +5901,7 @@
         <v>1</v>
       </c>
       <c r="AM33" s="10">
-        <v>2.5000000000000001E-2</v>
+        <v>0.05</v>
       </c>
       <c r="AN33" s="10">
         <v>0.5</v>
@@ -5989,23 +5992,23 @@
       </c>
     </row>
     <row r="34" spans="1:68" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="10" t="s">
-        <v>145</v>
+      <c r="A34" s="17" t="s">
+        <v>126</v>
       </c>
       <c r="B34" s="10" t="b">
         <v>0</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>144</v>
+        <v>110</v>
       </c>
       <c r="D34" s="10">
         <v>1</v>
       </c>
       <c r="E34" s="10" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="F34" s="10" t="s">
-        <v>85</v>
+        <v>63</v>
       </c>
       <c r="G34" s="10">
         <v>1.4999999999999999E-2</v>
@@ -6017,13 +6020,13 @@
         <v>76</v>
       </c>
       <c r="U34" s="10">
-        <v>2.5000000000000001E-2</v>
+        <v>0.02</v>
       </c>
       <c r="V34" s="10">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="W34" s="14">
-        <v>5</v>
+        <v>0</v>
+      </c>
+      <c r="W34" s="10">
+        <v>1</v>
       </c>
       <c r="X34" s="10">
         <v>0.02</v>
@@ -6050,7 +6053,7 @@
         <v>1E-3</v>
       </c>
       <c r="AF34" s="10">
-        <v>0.02</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="AG34" s="10">
         <v>0</v>
@@ -6059,7 +6062,13 @@
         <v>1</v>
       </c>
       <c r="AI34" s="10">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="AJ34" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="AK34" s="10">
+        <v>0.5</v>
       </c>
       <c r="AM34" s="10">
         <v>0.05</v>
@@ -6068,7 +6077,7 @@
         <v>0.5</v>
       </c>
       <c r="AO34" s="10">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="AP34" s="10">
         <v>0.5</v>
@@ -6086,7 +6095,7 @@
         <v>0.11</v>
       </c>
       <c r="AU34" s="10">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="AV34" s="10">
         <v>0.03</v>
@@ -6154,19 +6163,19 @@
     </row>
     <row r="35" spans="1:68" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
-        <v>152</v>
+        <v>127</v>
       </c>
       <c r="B35" s="10" t="b">
         <v>0</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>146</v>
+        <v>111</v>
       </c>
       <c r="D35" s="10">
         <v>1</v>
       </c>
       <c r="E35" s="10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F35" s="10" t="s">
         <v>63</v>
@@ -6174,23 +6183,11 @@
       <c r="G35" s="10">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="H35" s="10">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="I35" s="10">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="J35" s="10">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="K35" s="10">
-        <v>7.4999999999999997E-2</v>
-      </c>
       <c r="L35" s="10" t="s">
-        <v>134</v>
-      </c>
-      <c r="O35" s="10" t="s">
-        <v>76</v>
+        <v>112</v>
+      </c>
+      <c r="M35" s="10" t="s">
+        <v>118</v>
       </c>
       <c r="U35" s="10">
         <v>0.02</v>
@@ -6238,7 +6235,7 @@
         <v>1</v>
       </c>
       <c r="AM35" s="10">
-        <v>0.05</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="AN35" s="10">
         <v>0.5</v>
@@ -6328,218 +6325,402 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:68" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" spans="1:68" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="B36" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="D36" s="10">
+        <v>1</v>
+      </c>
+      <c r="E36" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="F36" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="G36" s="10">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="L36" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="O36" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="U36" s="10">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="V36" s="10">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="W36" s="14">
+        <v>5</v>
+      </c>
+      <c r="X36" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="Y36" s="10">
+        <v>0</v>
+      </c>
+      <c r="Z36" s="10">
+        <v>0.9</v>
+      </c>
+      <c r="AA36" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="AB36" s="10">
+        <v>0</v>
+      </c>
+      <c r="AC36" s="10">
+        <v>0.9</v>
+      </c>
+      <c r="AD36" s="10">
+        <v>0.01</v>
+      </c>
+      <c r="AE36" s="10">
+        <v>1E-3</v>
+      </c>
+      <c r="AF36" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="AG36" s="10">
+        <v>0</v>
+      </c>
+      <c r="AH36" s="10">
+        <v>1</v>
+      </c>
+      <c r="AI36" s="10">
+        <v>1</v>
+      </c>
+      <c r="AM36" s="10">
+        <v>0.05</v>
+      </c>
+      <c r="AN36" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="AO36" s="10">
+        <v>0.05</v>
+      </c>
+      <c r="AP36" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="AQ36" s="10">
+        <v>0.03</v>
+      </c>
+      <c r="AR36" s="10">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AS36" s="10">
+        <v>0.04</v>
+      </c>
+      <c r="AT36" s="10">
+        <v>0.11</v>
+      </c>
+      <c r="AU36" s="10">
+        <v>5</v>
+      </c>
+      <c r="AV36" s="10">
+        <v>0.03</v>
+      </c>
+      <c r="AW36" s="10">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AX36" s="10">
+        <v>0.7</v>
+      </c>
+      <c r="AY36" s="10">
+        <v>1</v>
+      </c>
+      <c r="AZ36" s="10">
+        <v>15</v>
+      </c>
+      <c r="BA36" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="BB36" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="BC36" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="BD36" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="BE36" s="10">
+        <v>5</v>
+      </c>
+      <c r="BF36" s="10">
+        <v>8.2199999999999995E-2</v>
+      </c>
+      <c r="BG36" s="10">
+        <v>0.12</v>
+      </c>
+      <c r="BH36" s="10">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="BI36" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="BJ36" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="BK36" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="BL36" s="10">
+        <v>0.01</v>
+      </c>
+      <c r="BM36" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="BN36" s="10">
+        <v>1</v>
+      </c>
+      <c r="BO36" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="BP36" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
     <row r="37" spans="1:68" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
-        <v>108</v>
+        <v>152</v>
       </c>
       <c r="B37" s="10" t="b">
         <v>0</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>111</v>
+        <v>146</v>
+      </c>
+      <c r="D37" s="10">
+        <v>1</v>
+      </c>
+      <c r="E37" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="F37" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="G37" s="10">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="H37" s="10">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="I37" s="10">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="J37" s="10">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="K37" s="10">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="L37" s="10" t="s">
+        <v>134</v>
       </c>
       <c r="O37" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="P37" s="10">
-        <v>1</v>
-      </c>
-      <c r="Q37" s="10">
-        <v>1</v>
-      </c>
-      <c r="R37" s="10">
-        <v>1</v>
-      </c>
-      <c r="S37" s="10">
+      <c r="U37" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="V37" s="10">
+        <v>0</v>
+      </c>
+      <c r="W37" s="10">
+        <v>1</v>
+      </c>
+      <c r="X37" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="Y37" s="10">
+        <v>0</v>
+      </c>
+      <c r="Z37" s="10">
+        <v>0.9</v>
+      </c>
+      <c r="AA37" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="AB37" s="10">
+        <v>0</v>
+      </c>
+      <c r="AC37" s="10">
+        <v>0.9</v>
+      </c>
+      <c r="AD37" s="10">
+        <v>0.01</v>
+      </c>
+      <c r="AE37" s="10">
+        <v>1E-3</v>
+      </c>
+      <c r="AF37" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="AG37" s="10">
+        <v>0</v>
+      </c>
+      <c r="AH37" s="10">
+        <v>1</v>
+      </c>
+      <c r="AI37" s="10">
+        <v>1</v>
+      </c>
+      <c r="AM37" s="10">
+        <v>0.05</v>
+      </c>
+      <c r="AN37" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="AO37" s="10">
+        <v>0</v>
+      </c>
+      <c r="AP37" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="AQ37" s="10">
         <v>0.03</v>
       </c>
-      <c r="T37" s="10">
+      <c r="AR37" s="10">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AS37" s="10">
+        <v>0.04</v>
+      </c>
+      <c r="AT37" s="10">
+        <v>0.11</v>
+      </c>
+      <c r="AU37" s="10">
+        <v>1</v>
+      </c>
+      <c r="AV37" s="10">
         <v>0.03</v>
       </c>
+      <c r="AW37" s="10">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AX37" s="10">
+        <v>0.7</v>
+      </c>
+      <c r="AY37" s="10">
+        <v>1</v>
+      </c>
+      <c r="AZ37" s="10">
+        <v>15</v>
+      </c>
+      <c r="BA37" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="BB37" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="BC37" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="BD37" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="BE37" s="10">
+        <v>5</v>
+      </c>
+      <c r="BF37" s="10">
+        <v>8.2199999999999995E-2</v>
+      </c>
+      <c r="BG37" s="10">
+        <v>0.12</v>
+      </c>
+      <c r="BH37" s="10">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="BI37" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="BJ37" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="BK37" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="BL37" s="10">
+        <v>0.01</v>
+      </c>
+      <c r="BM37" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="BN37" s="10">
+        <v>1</v>
+      </c>
+      <c r="BO37" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="BP37" s="10" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="38" spans="1:68" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="O38" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="P38" s="10">
-        <v>1</v>
-      </c>
-      <c r="Q38" s="10">
-        <v>1</v>
-      </c>
-      <c r="R38" s="10">
-        <v>1</v>
-      </c>
-      <c r="S38" s="10">
-        <v>0.06</v>
-      </c>
-      <c r="T38" s="10">
-        <v>0.06</v>
-      </c>
-    </row>
+    <row r="38" spans="1:68" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="39" spans="1:68" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="10" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="B39" s="10" t="b">
         <v>0</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="D39" s="10">
-        <v>1</v>
-      </c>
-      <c r="E39" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="F39" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="G39" s="10">
-        <v>1.4999999999999999E-2</v>
+        <v>111</v>
       </c>
       <c r="O39" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="U39" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="V39" s="10">
-        <v>0</v>
-      </c>
-      <c r="X39" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="Y39" s="10">
-        <v>0</v>
-      </c>
-      <c r="Z39" s="10">
-        <v>0.9</v>
-      </c>
-      <c r="AA39" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="AB39" s="10">
-        <v>0</v>
-      </c>
-      <c r="AC39" s="10">
-        <v>0.9</v>
-      </c>
-      <c r="AD39" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="AE39" s="10">
-        <v>1E-3</v>
-      </c>
-      <c r="AF39" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="AG39" s="10">
-        <v>0</v>
-      </c>
-      <c r="AH39" s="10">
-        <v>1</v>
-      </c>
-      <c r="AI39" s="10">
-        <v>1</v>
-      </c>
-      <c r="AM39" s="10">
-        <v>0.05</v>
-      </c>
-      <c r="AN39" s="10">
-        <v>0.5</v>
-      </c>
-      <c r="AO39" s="10">
-        <v>0</v>
-      </c>
-      <c r="AP39" s="10">
-        <v>0.5</v>
-      </c>
-      <c r="AQ39" s="10">
+      <c r="P39" s="10">
+        <v>1</v>
+      </c>
+      <c r="Q39" s="10">
+        <v>1</v>
+      </c>
+      <c r="R39" s="10">
+        <v>1</v>
+      </c>
+      <c r="S39" s="10">
         <v>0.03</v>
       </c>
-      <c r="AR39" s="10">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="AS39" s="10">
-        <v>0.04</v>
-      </c>
-      <c r="AT39" s="10">
-        <v>0.11</v>
-      </c>
-      <c r="AV39" s="10">
+      <c r="T39" s="10">
         <v>0.03</v>
       </c>
-      <c r="AW39" s="10">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="AX39" s="10">
-        <v>0.7</v>
-      </c>
-      <c r="AY39" s="10">
-        <v>1</v>
-      </c>
-      <c r="AZ39" s="10">
-        <v>15</v>
-      </c>
-      <c r="BA39" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="BB39" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="BC39" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="BD39" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="BE39" s="10">
-        <v>5</v>
-      </c>
-      <c r="BF39" s="10">
-        <v>8.2199999999999995E-2</v>
-      </c>
-      <c r="BG39" s="10">
-        <v>0.12</v>
-      </c>
-      <c r="BH39" s="10">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="BI39" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="BJ39" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="BK39" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="BL39" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="BM39" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="BN39" s="10">
-        <v>0.75</v>
-      </c>
-      <c r="BO39" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="BP39" s="10" t="b">
-        <v>1</v>
-      </c>
     </row>
-    <row r="40" spans="1:68" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="1:68" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="O40" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="P40" s="10">
+        <v>1</v>
+      </c>
+      <c r="Q40" s="10">
+        <v>1</v>
+      </c>
+      <c r="R40" s="10">
+        <v>1</v>
+      </c>
+      <c r="S40" s="10">
+        <v>0.06</v>
+      </c>
+      <c r="T40" s="10">
+        <v>0.06</v>
+      </c>
+    </row>
     <row r="41" spans="1:68" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="14" t="s">
-        <v>99</v>
+      <c r="A41" s="10" t="s">
+        <v>102</v>
       </c>
       <c r="B41" s="10" t="b">
         <v>0</v>
@@ -6554,7 +6735,7 @@
         <v>50</v>
       </c>
       <c r="F41" s="10" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="G41" s="10">
         <v>1.4999999999999999E-2</v>
@@ -6628,9 +6809,6 @@
       <c r="AT41" s="10">
         <v>0.11</v>
       </c>
-      <c r="AU41" s="10">
-        <v>5</v>
-      </c>
       <c r="AV41" s="10">
         <v>0.03</v>
       </c>
@@ -6695,174 +6873,175 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:68" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="14" t="s">
+    <row r="42" spans="1:68" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="1:68" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="B42" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="C42" s="10" t="s">
+      <c r="B43" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="C43" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="D42" s="10">
-        <v>1</v>
-      </c>
-      <c r="E42" s="10" t="s">
+      <c r="D43" s="10">
+        <v>1</v>
+      </c>
+      <c r="E43" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="F42" s="10" t="s">
+      <c r="F43" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="G42" s="10">
+      <c r="G43" s="10">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="O42" s="10" t="s">
+      <c r="O43" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="U42" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="V42" s="10">
-        <v>0</v>
-      </c>
-      <c r="X42" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="Y42" s="10">
-        <v>0</v>
-      </c>
-      <c r="Z42" s="10">
+      <c r="U43" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="V43" s="10">
+        <v>0</v>
+      </c>
+      <c r="X43" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="Y43" s="10">
+        <v>0</v>
+      </c>
+      <c r="Z43" s="10">
         <v>0.9</v>
       </c>
-      <c r="AA42" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="AB42" s="10">
-        <v>0</v>
-      </c>
-      <c r="AC42" s="10">
+      <c r="AA43" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="AB43" s="10">
+        <v>0</v>
+      </c>
+      <c r="AC43" s="10">
         <v>0.9</v>
       </c>
-      <c r="AD42" s="10">
+      <c r="AD43" s="10">
         <v>0.01</v>
       </c>
-      <c r="AE42" s="10">
+      <c r="AE43" s="10">
         <v>1E-3</v>
       </c>
-      <c r="AF42" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="AG42" s="10">
-        <v>0</v>
-      </c>
-      <c r="AH42" s="10">
-        <v>1</v>
-      </c>
-      <c r="AI42" s="10">
-        <v>1</v>
-      </c>
-      <c r="AM42" s="10">
+      <c r="AF43" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="AG43" s="10">
+        <v>0</v>
+      </c>
+      <c r="AH43" s="10">
+        <v>1</v>
+      </c>
+      <c r="AI43" s="10">
+        <v>1</v>
+      </c>
+      <c r="AM43" s="10">
         <v>0.05</v>
       </c>
-      <c r="AN42" s="10">
-        <v>0.5</v>
-      </c>
-      <c r="AO42" s="10">
-        <v>0</v>
-      </c>
-      <c r="AP42" s="10">
-        <v>0.5</v>
-      </c>
-      <c r="AQ42" s="10">
+      <c r="AN43" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="AO43" s="10">
+        <v>0</v>
+      </c>
+      <c r="AP43" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="AQ43" s="10">
         <v>0.03</v>
       </c>
-      <c r="AR42" s="10">
+      <c r="AR43" s="10">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AS42" s="10">
+      <c r="AS43" s="10">
         <v>0.04</v>
       </c>
-      <c r="AT42" s="10">
+      <c r="AT43" s="10">
         <v>0.11</v>
       </c>
-      <c r="AU42" s="10">
+      <c r="AU43" s="10">
         <v>5</v>
       </c>
-      <c r="AV42" s="10">
+      <c r="AV43" s="10">
         <v>0.03</v>
       </c>
-      <c r="AW42" s="10">
+      <c r="AW43" s="10">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AX42" s="10">
+      <c r="AX43" s="10">
         <v>0.7</v>
       </c>
-      <c r="AY42" s="10">
-        <v>1</v>
-      </c>
-      <c r="AZ42" s="10">
+      <c r="AY43" s="10">
+        <v>1</v>
+      </c>
+      <c r="AZ43" s="10">
         <v>15</v>
       </c>
-      <c r="BA42" s="10" t="s">
+      <c r="BA43" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="BB42" s="10" t="s">
+      <c r="BB43" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="BC42" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="BD42" s="10" t="s">
+      <c r="BC43" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="BD43" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="BE42" s="10">
+      <c r="BE43" s="10">
         <v>5</v>
       </c>
-      <c r="BF42" s="10">
+      <c r="BF43" s="10">
         <v>8.2199999999999995E-2</v>
       </c>
-      <c r="BG42" s="10">
+      <c r="BG43" s="10">
         <v>0.12</v>
       </c>
-      <c r="BH42" s="10">
+      <c r="BH43" s="10">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="BI42" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="BJ42" s="10" t="s">
+      <c r="BI43" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="BJ43" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="BK42" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="BL42" s="10">
+      <c r="BK43" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="BL43" s="10">
         <v>0.01</v>
       </c>
-      <c r="BM42" s="10" t="s">
+      <c r="BM43" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="BN42" s="10">
-        <v>1</v>
-      </c>
-      <c r="BO42" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="BP42" s="10" t="b">
+      <c r="BN43" s="10">
+        <v>1</v>
+      </c>
+      <c r="BO43" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="BP43" s="10" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:68" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="44" spans="1:68" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="45" spans="1:68" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="1:68" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B45" xr:uid="{05E01AB2-72EC-4550-ACB8-4E83765DE296}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O36:O41 O23:O34 O20:O21 O3:O18 O43" xr:uid="{8DBFC5CB-438A-4309-B948-24597CAE3D7F}">
+      <formula1>"preSet, ALpct,MApct"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B46" xr:uid="{05E01AB2-72EC-4550-ACB8-4E83765DE296}">
       <formula1>"TRUE,FALSE"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O41:O42 O3:O16 O21:O32 O18:O19 O34:O39" xr:uid="{8DBFC5CB-438A-4309-B948-24597CAE3D7F}">
-      <formula1>"preSet, ALpct,MApct"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6874,7 +7053,7 @@
           <x14:formula1>
             <xm:f>Policies!$B$3:$B$9</xm:f>
           </x14:formula1>
-          <xm:sqref>F39 F41:F42 F3:F37</xm:sqref>
+          <xm:sqref>F41 F3:F39 F43</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -6887,8 +7066,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6927,7 +7106,7 @@
         <v>2000</v>
       </c>
       <c r="C2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D2">
         <v>20</v>
@@ -6953,7 +7132,7 @@
   <dimension ref="A2:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
update figure for paper 1, before adding benefit of hybrid plan
</commit_message>
<xml_diff>
--- a/RunControl.xlsx
+++ b/RunControl.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A6C6A54-A786-4B5D-A3FD-51AF6475364C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABA979B4-8EBE-4A76-B983-0678B2DD401E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28050" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="paramlist" sheetId="1" r:id="rId1"/>
@@ -560,13 +560,13 @@
     <t>DA_as_ret_FR100</t>
   </si>
   <si>
-    <t>EEC_FR_t100</t>
-  </si>
-  <si>
-    <t>hybrid_DB_noLegacy</t>
-  </si>
-  <si>
     <t>Archived runs:</t>
+  </si>
+  <si>
+    <t>hybrid_DB_noLegacy_FR100</t>
+  </si>
+  <si>
+    <t>EEC_FR_t100_FR100</t>
   </si>
 </sst>
 </file>
@@ -989,10 +989,10 @@
   <dimension ref="A1:BT61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6" ySplit="2" topLeftCell="AO3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F37" sqref="F37"/>
+      <selection pane="bottomRight" activeCell="AL25" sqref="AL25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1673,7 +1673,7 @@
         <v>153</v>
       </c>
       <c r="B6" s="10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>106</v>
@@ -2332,22 +2332,22 @@
     </row>
     <row r="10" spans="1:72" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
-        <v>170</v>
+        <v>156</v>
       </c>
       <c r="B10" s="10" t="b">
         <v>0</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D10" s="10">
         <v>1</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>88</v>
+        <v>63</v>
       </c>
       <c r="G10" s="10">
         <v>1.4999999999999999E-2</v>
@@ -2359,12 +2359,15 @@
         <v>76</v>
       </c>
       <c r="W10" s="10">
-        <v>0.02</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="X10" s="10">
-        <v>0</v>
-      </c>
-      <c r="Y10" s="10">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="Y10" s="14">
+        <v>5</v>
+      </c>
+      <c r="Z10" s="14" t="b">
         <v>1</v>
       </c>
       <c r="AA10" s="10">
@@ -2428,7 +2431,7 @@
         <v>0.11</v>
       </c>
       <c r="AY10" s="10">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="AZ10" s="10">
         <v>0.03</v>
@@ -2437,10 +2440,10 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="BB10" s="10">
-        <v>0.85</v>
+        <v>0.7</v>
       </c>
       <c r="BC10" s="10">
-        <v>1.1499999999999999</v>
+        <v>1</v>
       </c>
       <c r="BD10" s="10">
         <v>15</v>
@@ -2496,7 +2499,7 @@
     </row>
     <row r="11" spans="1:72" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B11" s="10" t="b">
         <v>0</v>
@@ -2529,7 +2532,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="Y11" s="14">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="Z11" s="14" t="b">
         <v>1</v>
@@ -2661,9 +2664,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:72" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:72" s="10" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
-        <v>158</v>
+        <v>135</v>
       </c>
       <c r="B12" s="10" t="b">
         <v>0</v>
@@ -2675,7 +2678,7 @@
         <v>1</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F12" s="10" t="s">
         <v>63</v>
@@ -2690,25 +2693,25 @@
         <v>76</v>
       </c>
       <c r="W12" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="X12" s="10">
+        <v>0</v>
+      </c>
+      <c r="Y12" s="10">
+        <v>1</v>
+      </c>
+      <c r="Z12" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA12" s="10">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="X12" s="10">
+      <c r="AB12" s="10">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="Y12" s="14">
-        <v>10</v>
-      </c>
-      <c r="Z12" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="AA12" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="AB12" s="10">
-        <v>0</v>
-      </c>
       <c r="AC12" s="10">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="AD12" s="10">
         <v>0.02</v>
@@ -2762,7 +2765,7 @@
         <v>0.11</v>
       </c>
       <c r="AY12" s="10">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="AZ12" s="10">
         <v>0.03</v>
@@ -2828,9 +2831,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:72" s="10" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="20" t="s">
-        <v>135</v>
+    <row r="13" spans="1:72" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>102</v>
       </c>
       <c r="B13" s="10" t="b">
         <v>0</v>
@@ -2842,7 +2845,7 @@
         <v>1</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F13" s="10" t="s">
         <v>63</v>
@@ -2869,13 +2872,13 @@
         <v>0</v>
       </c>
       <c r="AA13" s="10">
-        <v>2.5000000000000001E-2</v>
+        <v>0.02</v>
       </c>
       <c r="AB13" s="10">
-        <v>5.0000000000000001E-3</v>
+        <v>0</v>
       </c>
       <c r="AC13" s="10">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="AD13" s="10">
         <v>0.02</v>
@@ -2996,8 +2999,8 @@
       </c>
     </row>
     <row r="14" spans="1:72" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
-        <v>102</v>
+      <c r="A14" s="20" t="s">
+        <v>104</v>
       </c>
       <c r="B14" s="10" t="b">
         <v>0</v>
@@ -3009,7 +3012,7 @@
         <v>1</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="F14" s="10" t="s">
         <v>63</v>
@@ -3060,7 +3063,7 @@
         <v>1E-3</v>
       </c>
       <c r="AI14" s="10">
-        <v>0.02</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="AJ14" s="10">
         <v>0</v>
@@ -3069,7 +3072,13 @@
         <v>1</v>
       </c>
       <c r="AL14" s="10">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="AM14" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="AN14" s="10">
+        <v>0.5</v>
       </c>
       <c r="AP14" s="10">
         <v>0.05</v>
@@ -3163,8 +3172,8 @@
       </c>
     </row>
     <row r="15" spans="1:72" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="20" t="s">
-        <v>104</v>
+      <c r="A15" s="17" t="s">
+        <v>148</v>
       </c>
       <c r="B15" s="10" t="b">
         <v>0</v>
@@ -3242,7 +3251,7 @@
         <v>0.5</v>
       </c>
       <c r="AN15" s="10">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="AP15" s="10">
         <v>0.05</v>
@@ -3336,20 +3345,20 @@
       </c>
     </row>
     <row r="16" spans="1:72" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
-        <v>148</v>
+      <c r="A16" s="20" t="s">
+        <v>105</v>
       </c>
       <c r="B16" s="10" t="b">
         <v>0</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D16" s="10">
         <v>1</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="F16" s="10" t="s">
         <v>63</v>
@@ -3358,10 +3367,10 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="N16" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="Q16" s="10" t="s">
-        <v>76</v>
+        <v>109</v>
+      </c>
+      <c r="O16" s="10" t="s">
+        <v>109</v>
       </c>
       <c r="W16" s="10">
         <v>0.02</v>
@@ -3371,9 +3380,6 @@
       </c>
       <c r="Y16" s="10">
         <v>1</v>
-      </c>
-      <c r="Z16" s="10" t="b">
-        <v>0</v>
       </c>
       <c r="AA16" s="10">
         <v>0.02</v>
@@ -3400,25 +3406,19 @@
         <v>1E-3</v>
       </c>
       <c r="AI16" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="AJ16" s="10">
+        <v>0</v>
+      </c>
+      <c r="AK16" s="10">
+        <v>1</v>
+      </c>
+      <c r="AL16" s="10">
+        <v>1</v>
+      </c>
+      <c r="AP16" s="10">
         <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="AJ16" s="10">
-        <v>0</v>
-      </c>
-      <c r="AK16" s="10">
-        <v>1</v>
-      </c>
-      <c r="AL16" s="10">
-        <v>2</v>
-      </c>
-      <c r="AM16" s="10">
-        <v>0.5</v>
-      </c>
-      <c r="AN16" s="10">
-        <v>0</v>
-      </c>
-      <c r="AP16" s="10">
-        <v>0.05</v>
       </c>
       <c r="AQ16" s="10">
         <v>0.5</v>
@@ -3510,19 +3510,19 @@
     </row>
     <row r="17" spans="1:72" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
-        <v>105</v>
+        <v>150</v>
       </c>
       <c r="B17" s="10" t="b">
         <v>0</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>108</v>
+        <v>143</v>
       </c>
       <c r="D17" s="10">
         <v>1</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F17" s="10" t="s">
         <v>63</v>
@@ -3530,12 +3530,33 @@
       <c r="G17" s="10">
         <v>1.4999999999999999E-2</v>
       </c>
+      <c r="H17" s="10">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="I17" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="J17" s="10">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="K17" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="L17" s="10">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="M17" s="10">
+        <v>7.4999999999999997E-2</v>
+      </c>
       <c r="N17" s="10" t="s">
-        <v>109</v>
+        <v>131</v>
       </c>
       <c r="O17" s="10" t="s">
         <v>109</v>
       </c>
+      <c r="Q17" s="10" t="s">
+        <v>76</v>
+      </c>
       <c r="W17" s="10">
         <v>0.02</v>
       </c>
@@ -3582,7 +3603,7 @@
         <v>1</v>
       </c>
       <c r="AP17" s="10">
-        <v>2.5000000000000001E-2</v>
+        <v>0.05</v>
       </c>
       <c r="AQ17" s="10">
         <v>0.5</v>
@@ -3673,20 +3694,20 @@
       </c>
     </row>
     <row r="18" spans="1:72" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="20" t="s">
-        <v>171</v>
+      <c r="A18" s="21" t="s">
+        <v>164</v>
       </c>
       <c r="B18" s="10" t="b">
         <v>0</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>108</v>
+        <v>143</v>
       </c>
       <c r="D18" s="10">
         <v>1</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F18" s="10" t="s">
         <v>63</v>
@@ -3694,9 +3715,33 @@
       <c r="G18" s="10">
         <v>1.4999999999999999E-2</v>
       </c>
+      <c r="H18" s="10">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="I18" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="J18" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="K18" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="L18" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="M18" s="10">
+        <v>7.4999999999999997E-2</v>
+      </c>
       <c r="N18" s="10" t="s">
         <v>131</v>
       </c>
+      <c r="O18" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q18" s="10" t="s">
+        <v>76</v>
+      </c>
       <c r="W18" s="10">
         <v>0.02</v>
       </c>
@@ -3743,7 +3788,7 @@
         <v>1</v>
       </c>
       <c r="AP18" s="10">
-        <v>2.5000000000000001E-2</v>
+        <v>0.05</v>
       </c>
       <c r="AQ18" s="10">
         <v>0.5</v>
@@ -3834,8 +3879,8 @@
       </c>
     </row>
     <row r="19" spans="1:72" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="20" t="s">
-        <v>150</v>
+      <c r="A19" s="21" t="s">
+        <v>165</v>
       </c>
       <c r="B19" s="10" t="b">
         <v>0</v>
@@ -3868,7 +3913,7 @@
         <v>0.02</v>
       </c>
       <c r="L19" s="10">
-        <v>5.0000000000000001E-3</v>
+        <v>0.02</v>
       </c>
       <c r="M19" s="10">
         <v>7.4999999999999997E-2</v>
@@ -4020,7 +4065,7 @@
     </row>
     <row r="20" spans="1:72" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="21" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B20" s="10" t="b">
         <v>0</v>
@@ -4053,7 +4098,7 @@
         <v>0.02</v>
       </c>
       <c r="L20" s="10">
-        <v>0.02</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="M20" s="10">
         <v>7.4999999999999997E-2</v>
@@ -4203,206 +4248,22 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:72" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="21" t="s">
-        <v>165</v>
-      </c>
-      <c r="B21" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>143</v>
-      </c>
-      <c r="D21" s="10">
-        <v>1</v>
-      </c>
-      <c r="E21" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="F21" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="G21" s="10">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="H21" s="10">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="I21" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="J21" s="10">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="K21" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="L21" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="M21" s="10">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="N21" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="O21" s="10" t="s">
+    <row r="21" spans="1:72" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:72" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="B22" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="C22" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="Q21" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="W21" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="X21" s="10">
-        <v>0</v>
-      </c>
-      <c r="Y21" s="10">
-        <v>1</v>
-      </c>
-      <c r="AA21" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="AB21" s="10">
-        <v>0</v>
-      </c>
-      <c r="AC21" s="10">
-        <v>0.9</v>
-      </c>
-      <c r="AD21" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="AE21" s="10">
-        <v>0</v>
-      </c>
-      <c r="AF21" s="10">
-        <v>0.9</v>
-      </c>
-      <c r="AG21" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="AH21" s="10">
-        <v>1E-3</v>
-      </c>
-      <c r="AI21" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="AJ21" s="10">
-        <v>0</v>
-      </c>
-      <c r="AK21" s="10">
-        <v>1</v>
-      </c>
-      <c r="AL21" s="10">
-        <v>1</v>
-      </c>
-      <c r="AP21" s="10">
-        <v>0.05</v>
-      </c>
-      <c r="AQ21" s="10">
-        <v>0.5</v>
-      </c>
-      <c r="AR21" s="10">
-        <v>0</v>
-      </c>
-      <c r="AT21" s="10">
-        <v>0.5</v>
-      </c>
-      <c r="AU21" s="10">
-        <v>0.03</v>
-      </c>
-      <c r="AV21" s="10">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="AW21" s="10">
-        <v>0.04</v>
-      </c>
-      <c r="AX21" s="10">
-        <v>0.11</v>
-      </c>
-      <c r="AY21" s="10">
-        <v>1</v>
-      </c>
-      <c r="AZ21" s="10">
-        <v>0.03</v>
-      </c>
-      <c r="BA21" s="10">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="BB21" s="10">
-        <v>0.7</v>
-      </c>
-      <c r="BC21" s="10">
-        <v>1</v>
-      </c>
-      <c r="BD21" s="10">
-        <v>15</v>
-      </c>
-      <c r="BE21" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="BF21" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="BG21" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="BH21" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="BI21" s="10">
-        <v>5</v>
-      </c>
-      <c r="BJ21" s="10">
-        <v>8.2199999999999995E-2</v>
-      </c>
-      <c r="BK21" s="10">
-        <v>0.12</v>
-      </c>
-      <c r="BL21" s="10">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="BM21" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="BN21" s="10" t="s">
+      <c r="D22" s="10">
+        <v>1</v>
+      </c>
+      <c r="E22" s="10" t="s">
         <v>50</v>
-      </c>
-      <c r="BO21" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="BP21" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="BQ21" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="BR21" s="10">
-        <v>0.75</v>
-      </c>
-      <c r="BS21" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="BT21" s="10" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:72" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="21" t="s">
-        <v>166</v>
-      </c>
-      <c r="B22" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>143</v>
-      </c>
-      <c r="D22" s="10">
-        <v>1</v>
-      </c>
-      <c r="E22" s="10" t="s">
-        <v>52</v>
       </c>
       <c r="F22" s="10" t="s">
         <v>63</v>
@@ -4410,30 +4271,9 @@
       <c r="G22" s="10">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="H22" s="10">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="I22" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="J22" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="K22" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="L22" s="10">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="M22" s="10">
-        <v>7.4999999999999997E-2</v>
-      </c>
       <c r="N22" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="O22" s="10" t="s">
-        <v>109</v>
-      </c>
       <c r="Q22" s="10" t="s">
         <v>76</v>
       </c>
@@ -4564,7 +4404,7 @@
         <v>23</v>
       </c>
       <c r="BR22" s="10">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="BS22" s="10" t="b">
         <v>1</v>
@@ -4573,16 +4413,182 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:72" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:72" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="B23" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="D23" s="10">
+        <v>1</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="G23" s="10">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="N23" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q23" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="W23" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="X23" s="10">
+        <v>0</v>
+      </c>
+      <c r="Y23" s="10">
+        <v>1</v>
+      </c>
+      <c r="AA23" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="AB23" s="10">
+        <v>0</v>
+      </c>
+      <c r="AC23" s="10">
+        <v>0.9</v>
+      </c>
+      <c r="AD23" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="AE23" s="10">
+        <v>0</v>
+      </c>
+      <c r="AF23" s="10">
+        <v>0.9</v>
+      </c>
+      <c r="AG23" s="10">
+        <v>0.01</v>
+      </c>
+      <c r="AH23" s="10">
+        <v>1E-3</v>
+      </c>
+      <c r="AI23" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="AJ23" s="10">
+        <v>0</v>
+      </c>
+      <c r="AK23" s="10">
+        <v>1</v>
+      </c>
+      <c r="AL23" s="10">
+        <v>1</v>
+      </c>
+      <c r="AP23" s="10">
+        <v>0.05</v>
+      </c>
+      <c r="AQ23" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="AR23" s="10">
+        <v>0</v>
+      </c>
+      <c r="AS23" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="AT23" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="AU23" s="10">
+        <v>0.03</v>
+      </c>
+      <c r="AV23" s="10">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AW23" s="10">
+        <v>0.04</v>
+      </c>
+      <c r="AX23" s="10">
+        <v>0.11</v>
+      </c>
+      <c r="AY23" s="10">
+        <v>1</v>
+      </c>
+      <c r="AZ23" s="10">
+        <v>0.03</v>
+      </c>
+      <c r="BA23" s="10">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="BB23" s="10">
+        <v>0.7</v>
+      </c>
+      <c r="BC23" s="10">
+        <v>1</v>
+      </c>
+      <c r="BD23" s="10">
+        <v>15</v>
+      </c>
+      <c r="BE23" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="BF23" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="BG23" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="BH23" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="BI23" s="10">
+        <v>5</v>
+      </c>
+      <c r="BJ23" s="10">
+        <v>8.2199999999999995E-2</v>
+      </c>
+      <c r="BK23" s="10">
+        <v>0.12</v>
+      </c>
+      <c r="BL23" s="10">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="BM23" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="BN23" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="BO23" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="BP23" s="10">
+        <v>0.01</v>
+      </c>
+      <c r="BQ23" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="BR23" s="10">
+        <v>1</v>
+      </c>
+      <c r="BS23" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="BT23" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
     <row r="24" spans="1:72" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="10" t="s">
-        <v>115</v>
+      <c r="A24" s="18" t="s">
+        <v>116</v>
       </c>
       <c r="B24" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D24" s="10">
         <v>1</v>
@@ -4591,7 +4597,7 @@
         <v>50</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>63</v>
+        <v>85</v>
       </c>
       <c r="G24" s="10">
         <v>1.4999999999999999E-2</v>
@@ -4656,6 +4662,9 @@
       <c r="AR24" s="10">
         <v>0</v>
       </c>
+      <c r="AS24" s="10">
+        <v>1</v>
+      </c>
       <c r="AT24" s="10">
         <v>0.5</v>
       </c>
@@ -4739,8 +4748,8 @@
       </c>
     </row>
     <row r="25" spans="1:72" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="14" t="s">
-        <v>154</v>
+      <c r="A25" s="18" t="s">
+        <v>172</v>
       </c>
       <c r="B25" s="10" t="b">
         <v>1</v>
@@ -4755,7 +4764,7 @@
         <v>50</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="G25" s="10">
         <v>1.4999999999999999E-2</v>
@@ -4820,9 +4829,6 @@
       <c r="AR25" s="10">
         <v>0</v>
       </c>
-      <c r="AS25" s="10">
-        <v>0.1</v>
-      </c>
       <c r="AT25" s="10">
         <v>0.5</v>
       </c>
@@ -4848,10 +4854,10 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="BB25" s="10">
-        <v>0.7</v>
+        <v>0.85</v>
       </c>
       <c r="BC25" s="10">
-        <v>1</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="BD25" s="10">
         <v>15</v>
@@ -4906,11 +4912,11 @@
       </c>
     </row>
     <row r="26" spans="1:72" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="14" t="s">
-        <v>116</v>
+      <c r="A26" s="18" t="s">
+        <v>132</v>
       </c>
       <c r="B26" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C26" s="10" t="s">
         <v>106</v>
@@ -4922,7 +4928,7 @@
         <v>50</v>
       </c>
       <c r="F26" s="10" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="G26" s="10">
         <v>1.4999999999999999E-2</v>
@@ -4939,9 +4945,10 @@
       <c r="X26" s="10">
         <v>0</v>
       </c>
-      <c r="Y26" s="10">
-        <v>1</v>
-      </c>
+      <c r="Y26" s="14">
+        <v>5</v>
+      </c>
+      <c r="Z26" s="14"/>
       <c r="AA26" s="10">
         <v>0.02</v>
       </c>
@@ -4987,9 +4994,6 @@
       <c r="AR26" s="10">
         <v>0</v>
       </c>
-      <c r="AS26" s="10">
-        <v>1</v>
-      </c>
       <c r="AT26" s="10">
         <v>0.5</v>
       </c>
@@ -5006,7 +5010,7 @@
         <v>0.11</v>
       </c>
       <c r="AY26" s="10">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="AZ26" s="10">
         <v>0.03</v>
@@ -5073,23 +5077,23 @@
       </c>
     </row>
     <row r="27" spans="1:72" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="10" t="s">
-        <v>132</v>
+      <c r="A27" s="18" t="s">
+        <v>157</v>
       </c>
       <c r="B27" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D27" s="10">
         <v>1</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>87</v>
+        <v>63</v>
       </c>
       <c r="G27" s="10">
         <v>1.4999999999999999E-2</v>
@@ -5101,15 +5105,17 @@
         <v>76</v>
       </c>
       <c r="W27" s="10">
-        <v>0.02</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="X27" s="10">
-        <v>0</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="Y27" s="14">
         <v>5</v>
       </c>
-      <c r="Z27" s="14"/>
+      <c r="Z27" s="14" t="b">
+        <v>1</v>
+      </c>
       <c r="AA27" s="10">
         <v>0.02</v>
       </c>
@@ -5238,11 +5244,11 @@
       </c>
     </row>
     <row r="28" spans="1:72" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="10" t="s">
-        <v>119</v>
+      <c r="A28" s="18" t="s">
+        <v>137</v>
       </c>
       <c r="B28" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C28" s="10" t="s">
         <v>106</v>
@@ -5402,20 +5408,20 @@
       </c>
     </row>
     <row r="29" spans="1:72" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="14" t="s">
-        <v>157</v>
+      <c r="A29" s="18" t="s">
+        <v>171</v>
       </c>
       <c r="B29" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D29" s="10">
         <v>1</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F29" s="10" t="s">
         <v>63</v>
@@ -5426,19 +5432,13 @@
       <c r="N29" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="Q29" s="10" t="s">
-        <v>76</v>
-      </c>
       <c r="W29" s="10">
-        <v>2.5000000000000001E-2</v>
+        <v>0.02</v>
       </c>
       <c r="X29" s="10">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="Y29" s="14">
-        <v>5</v>
-      </c>
-      <c r="Z29" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y29" s="10">
         <v>1</v>
       </c>
       <c r="AA29" s="10">
@@ -5478,7 +5478,7 @@
         <v>1</v>
       </c>
       <c r="AP29" s="10">
-        <v>0.05</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="AQ29" s="10">
         <v>0.5</v>
@@ -5502,7 +5502,7 @@
         <v>0.11</v>
       </c>
       <c r="AY29" s="10">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="AZ29" s="10">
         <v>0.03</v>
@@ -5569,8 +5569,8 @@
       </c>
     </row>
     <row r="30" spans="1:72" s="10" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="20" t="s">
-        <v>137</v>
+      <c r="A30" s="10" t="s">
+        <v>119</v>
       </c>
       <c r="B30" s="10" t="b">
         <v>0</v>
@@ -7157,7 +7157,7 @@
     <row r="41" spans="1:72" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="42" spans="1:72" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="14" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="43" spans="1:72" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -9863,10 +9863,10 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q46:Q47 Q3:Q16 Q49:Q54 Q43:Q44 Q56:Q61 Q19:Q33 Q35:Q41" xr:uid="{8DBFC5CB-438A-4309-B948-24597CAE3D7F}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q46:Q47 Q49:Q54 Q43:Q44 Q56:Q61 Q35:Q41 Q3:Q15 Q30:Q33 Q17:Q29" xr:uid="{8DBFC5CB-438A-4309-B948-24597CAE3D7F}">
       <formula1>"preSet, ALpct,MApct"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B61" xr:uid="{05E01AB2-72EC-4550-ACB8-4E83765DE296}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B30:B61 B3:B29" xr:uid="{05E01AB2-72EC-4550-ACB8-4E83765DE296}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
   </dataValidations>
@@ -9880,7 +9880,7 @@
           <x14:formula1>
             <xm:f>Policies!$B$3:$B$9</xm:f>
           </x14:formula1>
-          <xm:sqref>F46:F47 F49:F54 F43:F44 F56:F61 F3:F41</xm:sqref>
+          <xm:sqref>F46:F47 F49:F54 F43:F44 F56:F61 F30:F41 F3:F29</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>